<commit_message>
corrected parsing error in snails benchmark and reran affected experiments
</commit_message>
<xml_diff>
--- a/subsetting_results/subsetting-dtssql-snails-Native-lambda1.xlsx
+++ b/subsetting_results/subsetting-dtssql-snails-Native-lambda1.xlsx
@@ -835,7 +835,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>{'tblFieldDataTurtleMeasurements', 'tblFieldDataSnakeDataCollection'}</t>
+          <t>{'tblFieldDataSnakeDataCollection', 'tblFieldDataTurtleMeasurements'}</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
@@ -930,7 +930,7 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>{'tblFieldDataMinnowTrapSurveys.LocationID', 'tblFieldDataMinnowTrapSurveys.Trap_#'}</t>
+          <t>{'tblFieldDataMinnowTrapSurveys.Trap_#', 'tblFieldDataMinnowTrapSurveys.LocationID'}</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>{'tblFieldDataMinnowTrapSurveys.LocationID', 'tblFieldDataMinnowTrapSurveys.Count'}</t>
+          <t>{'tblFieldDataMinnowTrapSurveys.Count', 'tblFieldDataMinnowTrapSurveys.LocationID'}</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>{'tblFieldDataMinnowTrapSurveys.LocationID', 'tblFieldDataMinnowTrapSurveys.Trap_#', 'tblFieldDataMinnowTrapSurveys.Count'}</t>
+          <t>{'tblFieldDataMinnowTrapSurveys.Count', 'tblFieldDataMinnowTrapSurveys.Trap_#', 'tblFieldDataMinnowTrapSurveys.LocationID'}</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>{'tblFieldDataMinnowTrapSurveys.LocationID', 'tblFieldDataMinnowTrapSurveys.Stage', 'tblFieldDataMinnowTrapSurveys.Count'}</t>
+          <t>{'tblFieldDataMinnowTrapSurveys.Stage', 'tblFieldDataMinnowTrapSurveys.Count', 'tblFieldDataMinnowTrapSurveys.LocationID'}</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>{'tblFieldDataWaterProperties.TempC', 'tblFieldDataWaterProperties.LocationID', 'tblFieldDataAmphibianCallCounts.LocationID'}</t>
+          <t>{'tblFieldDataWaterProperties.TempC', 'tblFieldDataAmphibianCallCounts.LocationID', 'tblFieldDataWaterProperties.LocationID'}</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
@@ -1315,7 +1315,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>{'tblFieldDataWaterProperties', 'tblFieldDataTurtleTrapSurveys'}</t>
+          <t>{'tblFieldDataTurtleTrapSurveys', 'tblFieldDataWaterProperties'}</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>{'tblFieldDataWaterProperties.Conductivity', 'tblFieldDataWaterProperties.pH', 'tblFieldDataTurtleTrapSurveys.RecordID', 'tblFieldDataWaterProperties.TempC', 'tblFieldDataWaterProperties.Salinity', 'tblFieldDataWaterProperties.RecordID'}</t>
+          <t>{'tblFieldDataTurtleTrapSurveys.RecordID', 'tblFieldDataWaterProperties.pH', 'tblFieldDataWaterProperties.TempC', 'tblFieldDataWaterProperties.RecordID', 'tblFieldDataWaterProperties.Salinity', 'tblFieldDataWaterProperties.Conductivity'}</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
@@ -1395,7 +1395,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>{'tblFieldDataTurtleTrapSurveys', 'tblFieldDataTurtleMeasurements'}</t>
+          <t>{'tblFieldDataTurtleMeasurements', 'tblFieldDataTurtleTrapSurveys'}</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>{'tblFieldDataTurtleMeasurements.Comments', 'tblFieldDataTurtleMeasurements.Sex', 'tblFieldDataTurtleMeasurements.RecordID', 'tblFieldDataTurtleTrapSurveys.Comments', 'tblFieldDataTurtleTrapSurveys.Sex', 'tblFieldDataTurtleTrapSurveys.RecordID'}</t>
+          <t>{'tblFieldDataTurtleTrapSurveys.RecordID', 'tblFieldDataTurtleMeasurements.Comments', 'tblFieldDataTurtleMeasurements.Sex', 'tblFieldDataTurtleTrapSurveys.Comments', 'tblFieldDataTurtleTrapSurveys.Sex', 'tblFieldDataTurtleMeasurements.RecordID'}</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
@@ -1555,7 +1555,7 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tblFieldDataSnakeDataCollection'}</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tblFieldDataSnakeDataCollection.SVL'}</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="S15" t="inlineStr">
         <is>
-          <t>{'tblFieldDataSnakeDataCollection.Weight', 'tblFieldDataSnakeDataCollection.SVL', 'tblFieldDataSnakeDataCollection.Sex'}</t>
+          <t>{'tblFieldDataSnakeDataCollection.Sex', 'tblFieldDataSnakeDataCollection.SVL', 'tblFieldDataSnakeDataCollection.Weight'}</t>
         </is>
       </c>
       <c r="T15" t="inlineStr">
@@ -1730,7 +1730,7 @@
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>{'tblFieldDataSnakeDataCollection.Species_Code', 'tblFieldDataSnakeDataCollection.TLength', 'tblFieldDataSnakeDataCollection.Weight'}</t>
+          <t>{'tblFieldDataSnakeDataCollection.TLength', 'tblFieldDataSnakeDataCollection.Species_Code', 'tblFieldDataSnakeDataCollection.Weight'}</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
@@ -1795,7 +1795,7 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>{'Observer_LU', 'tlinkObservers', 'tblFieldDataTurtleMeasurements'}</t>
+          <t>{'tblFieldDataTurtleMeasurements', 'tlinkObservers', 'Observer_LU'}</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>{'Observer_LU.Agency/Title', 'Observer_LU.ObsInits', 'tblFieldDataTurtleMeasurements.EventID', 'tblFieldDataTurtleMeasurements.RecordID', 'tlinkObservers.EventID', 'tlinkObservers.ObsInits'}</t>
+          <t>{'tlinkObservers.EventID', 'tlinkObservers.ObsInits', 'Observer_LU.Agency/Title', 'Observer_LU.ObsInits', 'tblFieldDataTurtleMeasurements.RecordID', 'tblFieldDataTurtleMeasurements.EventID'}</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
@@ -1875,7 +1875,7 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>{'Observer_LU', 'tlinkObservers', 'tblEventDataHerps', 'tblEvents'}</t>
+          <t>{'tblEvents', 'Observer_LU', 'tlinkObservers', 'tblEventDataHerps'}</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
@@ -1890,7 +1890,7 @@
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>{'Observer_LU.LastName', 'Observer_LU.ObsInits', 'Observer_LU.FirstName', 'tlinkObservers.EventID', 'tblEvents.EventID', 'tblEvents.Year', 'tlinkObservers.ObsInits', 'tblEventDataHerps.EventID', 'tblEventDataHerps.ObsInits'}</t>
+          <t>{'tlinkObservers.EventID', 'tlinkObservers.ObsInits', 'Observer_LU.ObsInits', 'Observer_LU.FirstName', 'Observer_LU.LastName', 'tblEventDataHerps.EventID', 'tblEvents.Year', 'tblEvents.EventID', 'tblEventDataHerps.ObsInits'}</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
@@ -1955,7 +1955,7 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>{'Observer_LU', 'tlinkObservers', 'tblFieldDataTurtleMeasurements'}</t>
+          <t>{'tblFieldDataTurtleMeasurements', 'tlinkObservers', 'Observer_LU'}</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>{'Observer_LU.LastName', 'tlinkObservers.EventID', 'Observer_LU.ObsInits', 'tblFieldDataTurtleMeasurements.EventID', 'Observer_LU.FirstName', 'tlinkObservers.ObsInits'}</t>
+          <t>{'Observer_LU.FirstName', 'Observer_LU.LastName', 'tlinkObservers.EventID', 'tlinkObservers.ObsInits', 'Observer_LU.ObsInits', 'tblFieldDataTurtleMeasurements.EventID'}</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
@@ -2115,7 +2115,7 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>{'tblFieldDataTimeConstrainedSearches', 'tblLocationsPoints'}</t>
+          <t>{'tblLocationsPoints', 'tblFieldDataTimeConstrainedSearches'}</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
@@ -2130,7 +2130,7 @@
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>{'tblLocationsPoints.UTMX', 'tblLocationsPoints.UTMY', 'tblFieldDataTimeConstrainedSearches.LocationID', 'tblLocationsPoints.LocationID'}</t>
+          <t>{'tblLocationsPoints.UTMY', 'tblFieldDataTimeConstrainedSearches.LocationID', 'tblLocationsPoints.LocationID', 'tblLocationsPoints.UTMX'}</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>{'tluStage.Stage', 'tblFieldDataMinnowTrapSurveys.Stage', 'tluStage.Description'}</t>
+          <t>{'tblFieldDataMinnowTrapSurveys.Stage', 'tluStage.Stage', 'tluStage.Description'}</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
@@ -2290,7 +2290,7 @@
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>{'tblAbundance_LU.AbundanceText', 'tblAbundance_LU.AbundanceID', 'tblAbundance_LU.Abundance'}</t>
+          <t>{'tblAbundance_LU.AbundanceText', 'tblAbundance_LU.Abundance', 'tblAbundance_LU.AbundanceID'}</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
@@ -2450,7 +2450,7 @@
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>{'tblFieldDataCoverBoard.LocationID', 'tblLocations.SiteID', 'tblLocations.LocationID', 'tblFieldDataCoverBoard.Type', 'tblFieldDataCoverBoard.Board_#'}</t>
+          <t>{'tblLocations.LocationID', 'tblFieldDataCoverBoard.LocationID', 'tblFieldDataCoverBoard.Type', 'tblFieldDataCoverBoard.Board_#', 'tblLocations.SiteID'}</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
@@ -2515,7 +2515,7 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>{'tblFieldDataCoverBoard', 'tblLocations', 'tblEventDataHerps'}</t>
+          <t>{'tblEventDataHerps', 'tblFieldDataCoverBoard', 'tblLocations'}</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
@@ -2530,7 +2530,7 @@
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>{'tblEventDataHerps.AirTemp', 'tblFieldDataCoverBoard.LocationID', 'tblLocations.SiteID', 'tblLocations.LocationID', 'tblFieldDataCoverBoard.Type', 'tblEventDataHerps.Weather', 'tblFieldDataCoverBoard.EventID', 'tblEventDataHerps.EventID'}</t>
+          <t>{'tblLocations.LocationID', 'tblFieldDataCoverBoard.LocationID', 'tblEventDataHerps.Weather', 'tblLocations.SiteID', 'tblEventDataHerps.AirTemp', 'tblFieldDataCoverBoard.Type', 'tblEventDataHerps.EventID', 'tblFieldDataCoverBoard.EventID'}</t>
         </is>
       </c>
       <c r="T26" t="inlineStr">
@@ -2690,7 +2690,7 @@
       </c>
       <c r="S28" t="inlineStr">
         <is>
-          <t>{'tblFieldDataSnakeDataCollection.CaptureMethod', 'tblFieldDataSnakeDataCollection.Behavior', 'tblFieldDataSnakeDataCollection.Notes'}</t>
+          <t>{'tblFieldDataSnakeDataCollection.Notes', 'tblFieldDataSnakeDataCollection.CaptureMethod', 'tblFieldDataSnakeDataCollection.Behavior'}</t>
         </is>
       </c>
       <c r="T28" t="inlineStr">
@@ -2755,7 +2755,7 @@
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>{'tblFieldDataCoverBoard', 'tblLocations', 'tblLocationsPoints'}</t>
+          <t>{'tblLocationsPoints', 'tblFieldDataCoverBoard', 'tblLocations'}</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
@@ -2770,7 +2770,7 @@
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>{'tblFieldDataCoverBoard.SnakeID', 'tblFieldDataCoverBoard.LocationID', 'tblLocationsPoints.PointID', 'tblLocations.SiteID', 'tblLocations.LocationID', 'tblLocationsPoints.UTMX', 'tblLocationsPoints.UTMY', 'tblLocationsPoints.LocationID', 'tblFieldDataCoverBoard.Board_#', 'tblFieldDataCoverBoard.Recapture'}</t>
+          <t>{'tblFieldDataCoverBoard.LocationID', 'tblLocations.SiteID', 'tblLocationsPoints.UTMY', 'tblFieldDataCoverBoard.Board_#', 'tblLocationsPoints.UTMX', 'tblLocationsPoints.LocationID', 'tblLocationsPoints.PointID', 'tblFieldDataCoverBoard.SnakeID', 'tblFieldDataCoverBoard.Recapture', 'tblLocations.LocationID'}</t>
         </is>
       </c>
       <c r="T29" t="inlineStr">
@@ -2835,7 +2835,7 @@
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>{'tblFieldDataCoverBoard', 'Observer_LU', 'tlinkObservers', 'tblEvents'}</t>
+          <t>{'tblEvents', 'tlinkObservers', 'Observer_LU', 'tblFieldDataCoverBoard'}</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
@@ -2850,7 +2850,7 @@
       </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>{'tblEvents.EventID', 'Observer_LU.ObsInits', 'tlinkObservers.ObsInits', 'tblFieldDataCoverBoard.EventID', 'tlinkObservers.EventID'}</t>
+          <t>{'tblFieldDataCoverBoard.EventID', 'tlinkObservers.EventID', 'tlinkObservers.ObsInits', 'tblEvents.EventID', 'Observer_LU.ObsInits'}</t>
         </is>
       </c>
       <c r="T30" t="inlineStr">
@@ -3010,7 +3010,7 @@
       </c>
       <c r="S32" t="inlineStr">
         <is>
-          <t>{'tblEventDataHerps.AirTemp', 'Observer_LU.ObsInits', 'tlinkObservers.EventID', 'tblEventDataHerps.EventID', 'tblEventDataHerps.ObsInits', 'tlinkObservers.ObsInits'}</t>
+          <t>{'tlinkObservers.EventID', 'tlinkObservers.ObsInits', 'tblEventDataHerps.AirTemp', 'Observer_LU.ObsInits', 'tblEventDataHerps.ObsInits', 'tblEventDataHerps.EventID'}</t>
         </is>
       </c>
       <c r="T32" t="inlineStr">
@@ -3170,7 +3170,7 @@
       </c>
       <c r="S34" t="inlineStr">
         <is>
-          <t>{'tluProject.Description', 'tluProject.Project'}</t>
+          <t>{'tluProject.Project', 'tluProject.Description'}</t>
         </is>
       </c>
       <c r="T34" t="inlineStr">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="S37" t="inlineStr">
         <is>
-          <t>{'tluMicroHabitat.Habitat', 'tluMicroHabitat.Description'}</t>
+          <t>{'tluMicroHabitat.Description', 'tluMicroHabitat.Habitat'}</t>
         </is>
       </c>
       <c r="T37" t="inlineStr">
@@ -3570,7 +3570,7 @@
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>{'tblFieldDataTurtleTrapSurveys.LocationID', 'tblFieldDataTurtleTrapSurveys.Trap_Type', 'tblLocations.LocationID'}</t>
+          <t>{'tblLocations.LocationID', 'tblFieldDataTurtleTrapSurveys.Trap_Type', 'tblFieldDataTurtleTrapSurveys.LocationID'}</t>
         </is>
       </c>
       <c r="T39" t="inlineStr">
@@ -3650,7 +3650,7 @@
       </c>
       <c r="S40" t="inlineStr">
         <is>
-          <t>{'tblFieldDataTurtleMeasurements.Plastron_Length', 'tblFieldDataTurtleMeasurements.Carapace_Length', 'tblFieldDataTurtleMeasurements.Weight', 'tblFieldDataTurtleMeasurements.Plastron_Width', 'tblFieldDataTurtleMeasurements.Sex', 'tblFieldDataTurtleMeasurements.Carapace_Width'}</t>
+          <t>{'tblFieldDataTurtleMeasurements.Plastron_Length', 'tblFieldDataTurtleMeasurements.Sex', 'tblFieldDataTurtleMeasurements.Weight', 'tblFieldDataTurtleMeasurements.Plastron_Width', 'tblFieldDataTurtleMeasurements.Carapace_Length', 'tblFieldDataTurtleMeasurements.Carapace_Width'}</t>
         </is>
       </c>
       <c r="T40" t="inlineStr">
@@ -3795,7 +3795,7 @@
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies', 'tbl_Nests'}</t>
+          <t>{'tbl_Nests', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr">
@@ -3810,7 +3810,7 @@
       </c>
       <c r="S42" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies.SpeciesCode', 'tlu_PlantSpecies.subgenus', 'tlu_PlantSpecies.genus', 'tlu_PlantSpecies.CommonName', 'tbl_Nests.SpCode'}</t>
+          <t>{'tlu_PlantSpecies.genus', 'tlu_PlantSpecies.CommonName', 'tbl_Nests.SpCode', 'tlu_PlantSpecies.SpeciesCode', 'tlu_PlantSpecies.subgenus'}</t>
         </is>
       </c>
       <c r="T42" t="inlineStr">
@@ -3875,7 +3875,7 @@
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies', 'tbl_Nests'}</t>
+          <t>{'tbl_Nests', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="S43" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies.CommonName', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Nests.SpCode'}</t>
+          <t>{'tbl_Nests.SpCode', 'tlu_PlantSpecies.SpeciesCode', 'tlu_PlantSpecies.CommonName'}</t>
         </is>
       </c>
       <c r="T43" t="inlineStr">
@@ -3955,7 +3955,7 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Nests', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
@@ -3970,7 +3970,7 @@
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tlu_PlantSpecies.genus', 'tbl_Nests.SpCode', 'tlu_PlantSpecies.SpeciesCode'}</t>
         </is>
       </c>
       <c r="T44" t="inlineStr">
@@ -4290,7 +4290,7 @@
       </c>
       <c r="S48" t="inlineStr">
         <is>
-          <t>{'tbl_Deadwood.Event_ID', 'tlu_DecayStage.DecayStage_ID', 'tlu_DecayStage.DecayStage_Descr', 'tbl_Deadwood.Decay'}</t>
+          <t>{'tlu_DecayStage.DecayStage_ID', 'tlu_DecayStage.DecayStage_Descr', 'tbl_Deadwood.Event_ID', 'tbl_Deadwood.Decay'}</t>
         </is>
       </c>
       <c r="T48" t="inlineStr">
@@ -4435,7 +4435,7 @@
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>{'tbl_Events', 'tbl_Locations'}</t>
+          <t>{'tbl_Events', 'tbl_Nests', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q50" t="inlineStr">
@@ -4450,7 +4450,7 @@
       </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.Plot_ID', 'tbl_Events.Location_ID', 'tbl_Locations.Location_ID', 'tbl_Locations.Y_Coord', 'tbl_Locations.Directions', 'tbl_Locations.X_Coord', 'tbl_Events.Event_ID'}</t>
+          <t>{'tbl_Locations.X_Coord', 'tbl_Events.Event_ID', 'tbl_Locations.Y_Coord', 'tbl_Locations.Location_ID', 'tbl_Events.Location_ID', 'tbl_Locations.Directions', 'tbl_Locations.Plot_ID', 'tbl_Nests.Event_ID'}</t>
         </is>
       </c>
       <c r="T50" t="inlineStr">
@@ -4515,7 +4515,7 @@
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies', 'tbl_Overstory'}</t>
+          <t>{'tbl_Overstory', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q51" t="inlineStr">
@@ -4530,7 +4530,7 @@
       </c>
       <c r="S51" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies.genus', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Overstory.DBH', 'tbl_Overstory.SpCode'}</t>
+          <t>{'tlu_PlantSpecies.genus', 'tbl_Overstory.SpCode', 'tbl_Overstory.DBH', 'tlu_PlantSpecies.SpeciesCode'}</t>
         </is>
       </c>
       <c r="T51" t="inlineStr">
@@ -4595,7 +4595,7 @@
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>{'tlu_Can_Pos', 'tbl_Overstory'}</t>
+          <t>{'tbl_Overstory', 'tlu_Can_Pos'}</t>
         </is>
       </c>
       <c r="Q52" t="inlineStr">
@@ -4675,7 +4675,7 @@
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>{'tlu_Tree_Cond', 'tlu_PlantSpecies', 'tbl_Overstory'}</t>
+          <t>{'tlu_Tree_Cond', 'tbl_Overstory', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q53" t="inlineStr">
@@ -4690,7 +4690,7 @@
       </c>
       <c r="S53" t="inlineStr">
         <is>
-          <t>{'tlu_Tree_Cond.TreeCond_Text', 'tbl_Overstory.TreeTag', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Overstory.SpCode', 'tlu_Tree_Cond.TreeCond_Num', 'tbl_Overstory.TreeCond', 'tlu_PlantSpecies.CommonName'}</t>
+          <t>{'tlu_Tree_Cond.TreeCond_Num', 'tbl_Overstory.SpCode', 'tlu_PlantSpecies.CommonName', 'tbl_Overstory.TreeCond', 'tbl_Overstory.TreeTag', 'tlu_PlantSpecies.SpeciesCode', 'tlu_Tree_Cond.TreeCond_Text'}</t>
         </is>
       </c>
       <c r="T53" t="inlineStr">
@@ -5090,7 +5090,7 @@
       </c>
       <c r="S58" t="inlineStr">
         <is>
-          <t>{'tbl_Tree_Tags.Tree_Tag_ID', 'tbl_Locations.Directions', 'tbl_Tree_Tags.Location_ID', 'tbl_Locations.Location_ID'}</t>
+          <t>{'tbl_Tree_Tags.Location_ID', 'tbl_Locations.Directions', 'tbl_Tree_Tags.Tree_Tag_ID', 'tbl_Locations.Location_ID'}</t>
         </is>
       </c>
       <c r="T58" t="inlineStr">
@@ -5170,7 +5170,7 @@
       </c>
       <c r="S59" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.Elevation', 'tbl_Locations.Loc_Notes', 'tbl_Locations.SiteDescription'}</t>
+          <t>{'tbl_Locations.SiteDescription', 'tbl_Locations.Elevation', 'tbl_Locations.Loc_Notes'}</t>
         </is>
       </c>
       <c r="T59" t="inlineStr">
@@ -5235,7 +5235,7 @@
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>{'tlu_Cover_Cls', 'tbl_Nests'}</t>
+          <t>{'tbl_Nests', 'tlu_Cover_Cls'}</t>
         </is>
       </c>
       <c r="Q60" t="inlineStr">
@@ -5250,7 +5250,7 @@
       </c>
       <c r="S60" t="inlineStr">
         <is>
-          <t>{'tlu_Cover_Cls.CoverClass_Num', 'tbl_Nests.Cover', 'tlu_Cover_Cls.CoverClass_Text', 'tbl_Nests.Event_ID'}</t>
+          <t>{'tbl_Nests.Cover', 'tlu_Cover_Cls.CoverClass_Text', 'tlu_Cover_Cls.CoverClass_Num', 'tbl_Nests.Event_ID'}</t>
         </is>
       </c>
       <c r="T60" t="inlineStr">
@@ -5330,7 +5330,7 @@
       </c>
       <c r="S61" t="inlineStr">
         <is>
-          <t>{'tbl_WitnessTrees.Witness_Azimuth', 'tbl_WitnessTrees.Witness_stake', 'tbl_WitnessTrees.Witness_DBH'}</t>
+          <t>{'tbl_WitnessTrees.Witness_Azimuth', 'tbl_WitnessTrees.Witness_DBH', 'tbl_WitnessTrees.Witness_stake'}</t>
         </is>
       </c>
       <c r="T61" t="inlineStr">
@@ -5410,7 +5410,7 @@
       </c>
       <c r="S62" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies.genus', 'tlu_PlantSpecies.SpeciesCode', 'tbl_WitnessTrees.Witness_SpCode', 'tlu_PlantSpecies.species'}</t>
+          <t>{'tlu_PlantSpecies.genus', 'tbl_WitnessTrees.Witness_SpCode', 'tlu_PlantSpecies.species', 'tlu_PlantSpecies.SpeciesCode'}</t>
         </is>
       </c>
       <c r="T62" t="inlineStr">
@@ -5475,7 +5475,7 @@
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>{'tbl_Events', 'tbl_Locations', 'tlu_Roads_and_Trails'}</t>
+          <t>{'tbl_Events', 'tlu_Roads_and_Trails', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q63" t="inlineStr">
@@ -5490,7 +5490,7 @@
       </c>
       <c r="S63" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.Trail', 'tbl_Events.Location_ID', 'tbl_Locations.Location_ID', 'tlu_Roads_and_Trails.ListedName', 'tbl_Events.Event_ID', 'tlu_Roads_and_Trails.ValidName'}</t>
+          <t>{'tbl_Events.Location_ID', 'tbl_Events.Event_ID', 'tbl_Locations.Location_ID', 'tlu_Roads_and_Trails.ListedName', 'tlu_Roads_and_Trails.ValidName', 'tbl_Locations.Trail'}</t>
         </is>
       </c>
       <c r="T63" t="inlineStr">
@@ -5570,7 +5570,7 @@
       </c>
       <c r="S64" t="inlineStr">
         <is>
-          <t>{'tlu_PlaceNames.County', 'tbl_Locations.PlaceNameID', 'tbl_Tree_Tags.Location_ID', 'tbl_Locations.Location_ID', 'tlu_PlaceNames.State', 'tlu_PlaceNames.ID'}</t>
+          <t>{'tlu_PlaceNames.ID', 'tlu_PlaceNames.County', 'tbl_Locations.PlaceNameID', 'tbl_Locations.Location_ID', 'tbl_Tree_Tags.Location_ID', 'tlu_PlaceNames.State'}</t>
         </is>
       </c>
       <c r="T64" t="inlineStr">
@@ -5650,7 +5650,7 @@
       </c>
       <c r="S65" t="inlineStr">
         <is>
-          <t>{'tlu_PlaceNames.Name', 'tlu_PlaceNames.County', 'tlu_PlaceNames.utmN', 'tlu_PlaceNames.utmE'}</t>
+          <t>{'tlu_PlaceNames.utmE', 'tlu_PlaceNames.utmN', 'tlu_PlaceNames.County', 'tlu_PlaceNames.Name'}</t>
         </is>
       </c>
       <c r="T65" t="inlineStr">
@@ -5730,7 +5730,7 @@
       </c>
       <c r="S66" t="inlineStr">
         <is>
-          <t>{'tlu_topo_position.TopoPosition', 'tbl_Locations.Y_Coord', 'tbl_Locations.X_Coord', 'tlu_topo_position.ID', 'tbl_Locations.Topo_Position'}</t>
+          <t>{'tbl_Locations.Topo_Position', 'tbl_Locations.X_Coord', 'tbl_Locations.Y_Coord', 'tlu_topo_position.ID', 'tlu_topo_position.TopoPosition'}</t>
         </is>
       </c>
       <c r="T66" t="inlineStr">
@@ -5810,7 +5810,7 @@
       </c>
       <c r="S67" t="inlineStr">
         <is>
-          <t>{'tlu_Live_Dead.Cond_Text', 'tlu_Live_Dead.Cond_Num'}</t>
+          <t>{'tlu_Live_Dead.Cond_Num', 'tlu_Live_Dead.Cond_Text'}</t>
         </is>
       </c>
       <c r="T67" t="inlineStr">
@@ -6035,7 +6035,7 @@
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>{'tbl_Tree_Tags', 'tbl_Locations', 'tbl_Overstory', 'tlu_PlaceNames', 'tlu_PlantSpecies'}</t>
+          <t>{'tbl_Locations', 'tlu_PlaceNames', 'tlu_PlantSpecies', 'tbl_Overstory', 'tbl_Tree_Tags'}</t>
         </is>
       </c>
       <c r="Q70" t="inlineStr">
@@ -6050,7 +6050,7 @@
       </c>
       <c r="S70" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.PlaceNameID', 'tbl_Overstory.TreeTag', 'tbl_Locations.Location_ID', 'tlu_PlantSpecies.genus', 'tbl_Tree_Tags.Tree_Tag_ID', 'tlu_PlaceNames.County', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Overstory.SpCode', 'tbl_Tree_Tags.Location_ID', 'tbl_Tree_Tags.SpCode', 'tlu_PlaceNames.ID', 'tlu_PlantSpecies.CommonName', 'tlu_PlantSpecies.species'}</t>
+          <t>{'tlu_PlaceNames.ID', 'tlu_PlaceNames.County', 'tlu_PlantSpecies.CommonName', 'tbl_Tree_Tags.Tree_Tag_ID', 'tbl_Locations.Location_ID', 'tbl_Tree_Tags.Location_ID', 'tbl_Tree_Tags.SpCode', 'tbl_Overstory.SpCode', 'tbl_Locations.PlaceNameID', 'tlu_PlantSpecies.genus', 'tbl_Overstory.TreeTag', 'tlu_PlantSpecies.species', 'tlu_PlantSpecies.SpeciesCode'}</t>
         </is>
       </c>
       <c r="T70" t="inlineStr">
@@ -6115,7 +6115,7 @@
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>{'tbl_Seedlings', 'tlu_PlantSpecies', 'tbl_Overstory'}</t>
+          <t>{'tbl_Seedlings', 'tbl_Overstory', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q71" t="inlineStr">
@@ -6130,7 +6130,7 @@
       </c>
       <c r="S71" t="inlineStr">
         <is>
-          <t>{'tbl_Overstory.Overstory_ID', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Overstory.SpCode', 'tbl_Seedlings.SpCode', 'tbl_Seedlings.Seedlings_ID', 'tlu_PlantSpecies.CommonName', 'tlu_PlantSpecies.species'}</t>
+          <t>{'tbl_Overstory.SpCode', 'tbl_Seedlings.Seedlings_ID', 'tbl_Overstory.Overstory_ID', 'tlu_PlantSpecies.CommonName', 'tbl_Seedlings.SpCode', 'tlu_PlantSpecies.species', 'tlu_PlantSpecies.SpeciesCode'}</t>
         </is>
       </c>
       <c r="T71" t="inlineStr">
@@ -6210,7 +6210,7 @@
       </c>
       <c r="S72" t="inlineStr">
         <is>
-          <t>{'tbl_Tree_Tags.Tag', 'tbl_Tree_Tags.Ycoord', 'tbl_Tree_Tags.Xcoord'}</t>
+          <t>{'tbl_Tree_Tags.Tag', 'tbl_Tree_Tags.Xcoord', 'tbl_Tree_Tags.Ycoord'}</t>
         </is>
       </c>
       <c r="T72" t="inlineStr">
@@ -6275,7 +6275,7 @@
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>{'tlu_Cover_Cls', 'tbl_Nests'}</t>
+          <t>{'tbl_Nests', 'tlu_Cover_Cls'}</t>
         </is>
       </c>
       <c r="Q73" t="inlineStr">
@@ -6290,7 +6290,7 @@
       </c>
       <c r="S73" t="inlineStr">
         <is>
-          <t>{'tlu_Cover_Cls.CoverClass_Num', 'tbl_Nests.R2', 'tlu_Cover_Cls.CoverClass_Text'}</t>
+          <t>{'tbl_Nests.R2', 'tlu_Cover_Cls.CoverClass_Text', 'tlu_Cover_Cls.CoverClass_Num'}</t>
         </is>
       </c>
       <c r="T73" t="inlineStr">
@@ -6355,7 +6355,7 @@
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>{'tlu_Presence', 'tbl_Nests'}</t>
+          <t>{'tbl_Nests', 'tlu_Presence'}</t>
         </is>
       </c>
       <c r="Q74" t="inlineStr">
@@ -6370,7 +6370,7 @@
       </c>
       <c r="S74" t="inlineStr">
         <is>
-          <t>{'tlu_Presence.Pres_Num', 'tlu_Presence.Pres_Text', 'tbl_Nests.Presence_First'}</t>
+          <t>{'tlu_Presence.Pres_Num', 'tbl_Nests.Presence_First', 'tlu_Presence.Pres_Text'}</t>
         </is>
       </c>
       <c r="T74" t="inlineStr">
@@ -6530,7 +6530,7 @@
       </c>
       <c r="S76" t="inlineStr">
         <is>
-          <t>{'tbl_Deadwood.Length', 'tbl_Deadwood.Decay'}</t>
+          <t>{'tbl_Deadwood.Decay', 'tbl_Deadwood.Length'}</t>
         </is>
       </c>
       <c r="T76" t="inlineStr">
@@ -6595,7 +6595,7 @@
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>{'tlu_DecayStage'}</t>
+          <t>{'tlu_DecayStage', 'tbl_Deadwood'}</t>
         </is>
       </c>
       <c r="Q77" t="inlineStr">
@@ -6610,7 +6610,7 @@
       </c>
       <c r="S77" t="inlineStr">
         <is>
-          <t>{'tlu_DecayStage.DecayStage_ID', 'tlu_DecayStage.DecayStage_Descr'}</t>
+          <t>{'tbl_Deadwood.MPD', 'tlu_DecayStage.DecayStage_ID', 'tlu_DecayStage.DecayStage_Descr', 'tbl_Deadwood.Decay'}</t>
         </is>
       </c>
       <c r="T77" t="inlineStr">
@@ -6675,7 +6675,7 @@
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>{'tlu_DecayStage'}</t>
+          <t>{'tlu_DecayStage', 'tbl_Deadwood'}</t>
         </is>
       </c>
       <c r="Q78" t="inlineStr">
@@ -6690,7 +6690,7 @@
       </c>
       <c r="S78" t="inlineStr">
         <is>
-          <t>{'tlu_DecayStage.DecayStage_ID', 'tlu_DecayStage.DecayStage_Descr'}</t>
+          <t>{'tlu_DecayStage.DecayStage_ID', 'tbl_Deadwood.Length', 'tlu_DecayStage.DecayStage_Descr', 'tbl_Deadwood.Decay'}</t>
         </is>
       </c>
       <c r="T78" t="inlineStr">
@@ -6770,7 +6770,7 @@
       </c>
       <c r="S79" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.Aspect', 'tbl_Locations.Slope', 'tbl_Locations.Loc_Notes', 'tbl_Locations.SiteDescription', 'tbl_Locations.Slope_shape', 'tbl_Locations.Accuracy_Notes'}</t>
+          <t>{'tbl_Locations.SiteDescription', 'tbl_Locations.Slope', 'tbl_Locations.Accuracy_Notes', 'tbl_Locations.Aspect', 'tbl_Locations.Loc_Notes', 'tbl_Locations.Slope_shape'}</t>
         </is>
       </c>
       <c r="T79" t="inlineStr">
@@ -6850,7 +6850,7 @@
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.QuadName', 'tbl_Locations.Topo_Position'}</t>
+          <t>{'tbl_Locations.Topo_Position', 'tbl_Locations.QuadName'}</t>
         </is>
       </c>
       <c r="T80" t="inlineStr">
@@ -6930,7 +6930,7 @@
       </c>
       <c r="S81" t="inlineStr">
         <is>
-          <t>{'tbl_Saplings.Condition', 'tlu_Tree_Cond.TreeCond_Text', 'tlu_Tree_Cond.TreeCond_Num'}</t>
+          <t>{'tlu_Tree_Cond.TreeCond_Num', 'tbl_Saplings.Condition', 'tlu_Tree_Cond.TreeCond_Text'}</t>
         </is>
       </c>
       <c r="T81" t="inlineStr">
@@ -7010,7 +7010,7 @@
       </c>
       <c r="S82" t="inlineStr">
         <is>
-          <t>{'VERTEBRATES.Notes', 'VERTEBRATES.Common_Name', 'VERTEBRATES.Ownership'}</t>
+          <t>{'VERTEBRATES.Ownership', 'VERTEBRATES.Common_Name', 'VERTEBRATES.Notes'}</t>
         </is>
       </c>
       <c r="T82" t="inlineStr">
@@ -7170,7 +7170,7 @@
       </c>
       <c r="S84" t="inlineStr">
         <is>
-          <t>{'Breeding_Codes.Definition', 'VERTEBRATES.Common_Name', 'VERTEBRATES.BREED', 'Breeding_Codes.Breed'}</t>
+          <t>{'Breeding_Codes.Breed', 'VERTEBRATES.BREED', 'Breeding_Codes.Definition', 'VERTEBRATES.Common_Name'}</t>
         </is>
       </c>
       <c r="T84" t="inlineStr">
@@ -7250,7 +7250,7 @@
       </c>
       <c r="S85" t="inlineStr">
         <is>
-          <t>{'INVERTEBRATES.Genus_species', 'INVERTEBRATES.Class', 'INVERTEBRATES.Common_Name'}</t>
+          <t>{'INVERTEBRATES.Common_Name', 'INVERTEBRATES.Class', 'INVERTEBRATES.Genus_species'}</t>
         </is>
       </c>
       <c r="T85" t="inlineStr">
@@ -7330,7 +7330,7 @@
       </c>
       <c r="S86" t="inlineStr">
         <is>
-          <t>{'INVERTEBRATES.Family', 'Invert_Family.Invert_Family'}</t>
+          <t>{'Invert_Family.Invert_Family', 'INVERTEBRATES.Family'}</t>
         </is>
       </c>
       <c r="T86" t="inlineStr">
@@ -7410,7 +7410,7 @@
       </c>
       <c r="S87" t="inlineStr">
         <is>
-          <t>{'Roadkill.HWY_Mile_Marker', 'Roadkill.Species'}</t>
+          <t>{'Roadkill.Species', 'Roadkill.HWY_Mile_Marker'}</t>
         </is>
       </c>
       <c r="T87" t="inlineStr">
@@ -7490,7 +7490,7 @@
       </c>
       <c r="S88" t="inlineStr">
         <is>
-          <t>{'Roadkill.Year', 'Roadkill.Month'}</t>
+          <t>{'Roadkill.Month', 'Roadkill.Year'}</t>
         </is>
       </c>
       <c r="T88" t="inlineStr">
@@ -7570,7 +7570,7 @@
       </c>
       <c r="S89" t="inlineStr">
         <is>
-          <t>{'Roadkill.Comments', 'Roadkill.Year'}</t>
+          <t>{'Roadkill.Year', 'Roadkill.Comments'}</t>
         </is>
       </c>
       <c r="T89" t="inlineStr">
@@ -7650,7 +7650,7 @@
       </c>
       <c r="S90" t="inlineStr">
         <is>
-          <t>{'Roadkill.Year', 'Roadkill.Species'}</t>
+          <t>{'Roadkill.Species', 'Roadkill.Year'}</t>
         </is>
       </c>
       <c r="T90" t="inlineStr">
@@ -7715,7 +7715,7 @@
       </c>
       <c r="P91" t="inlineStr">
         <is>
-          <t>{'Roadkill', 'VERTEBRATES'}</t>
+          <t>{'VERTEBRATES', 'Roadkill'}</t>
         </is>
       </c>
       <c r="Q91" t="inlineStr">
@@ -7730,7 +7730,7 @@
       </c>
       <c r="S91" t="inlineStr">
         <is>
-          <t>{'Roadkill.Date', 'VERTEBRATES.Date'}</t>
+          <t>{'VERTEBRATES.Date', 'Roadkill.Date'}</t>
         </is>
       </c>
       <c r="T91" t="inlineStr">
@@ -7795,7 +7795,7 @@
       </c>
       <c r="P92" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Roadkill'}</t>
         </is>
       </c>
       <c r="Q92" t="inlineStr">
@@ -7810,7 +7810,7 @@
       </c>
       <c r="S92" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Roadkill.Species', 'Roadkill.number_killed', 'Roadkill.Month', 'Roadkill.Year'}</t>
         </is>
       </c>
       <c r="T92" t="inlineStr">
@@ -7875,7 +7875,7 @@
       </c>
       <c r="P93" t="inlineStr">
         <is>
-          <t>{'HABITAT_CODES', 'VERTEBRATES', 'INVERTEBRATES'}</t>
+          <t>{'VERTEBRATES', 'HABITAT_CODES', 'INVERTEBRATES'}</t>
         </is>
       </c>
       <c r="Q93" t="inlineStr">
@@ -7890,7 +7890,7 @@
       </c>
       <c r="S93" t="inlineStr">
         <is>
-          <t>{'HABITAT_CODES.Definition', 'INVERTEBRATES.Habitat', 'VERTEBRATES.Habitat', 'HABITAT_CODES.Code'}</t>
+          <t>{'VERTEBRATES.Habitat', 'HABITAT_CODES.Definition', 'INVERTEBRATES.Habitat', 'HABITAT_CODES.Code'}</t>
         </is>
       </c>
       <c r="T93" t="inlineStr">
@@ -8050,7 +8050,7 @@
       </c>
       <c r="S95" t="inlineStr">
         <is>
-          <t>{'VERTEBRATES.Habitat', 'VERTEBRATES.Observer', 'INVERTEBRATES.Date', 'INVERTEBRATES.Observer', 'INVERTEBRATES.Habitat', 'INVERTEBRATES.Common_Name', 'VERTEBRATES.Common_Name', 'VERTEBRATES.Date'}</t>
+          <t>{'INVERTEBRATES.Date', 'INVERTEBRATES.Habitat', 'VERTEBRATES.Habitat', 'VERTEBRATES.Common_Name', 'VERTEBRATES.Observer', 'VERTEBRATES.Date', 'INVERTEBRATES.Common_Name', 'INVERTEBRATES.Observer'}</t>
         </is>
       </c>
       <c r="T95" t="inlineStr">
@@ -8115,7 +8115,7 @@
       </c>
       <c r="P96" t="inlineStr">
         <is>
-          <t>{'HABITAT_CODES', 'VERTEBRATES', 'INVERTEBRATES'}</t>
+          <t>{'VERTEBRATES', 'HABITAT_CODES', 'INVERTEBRATES'}</t>
         </is>
       </c>
       <c r="Q96" t="inlineStr">
@@ -8130,7 +8130,7 @@
       </c>
       <c r="S96" t="inlineStr">
         <is>
-          <t>{'VERTEBRATES.Habitat', 'VERTEBRATES.Observer', 'INVERTEBRATES.Date', 'INVERTEBRATES.Observer', 'INVERTEBRATES.Habitat', 'HABITAT_CODES.Definition', 'VERTEBRATES.Date', 'HABITAT_CODES.Code'}</t>
+          <t>{'INVERTEBRATES.Date', 'INVERTEBRATES.Habitat', 'VERTEBRATES.Habitat', 'HABITAT_CODES.Code', 'VERTEBRATES.Observer', 'VERTEBRATES.Date', 'HABITAT_CODES.Definition', 'INVERTEBRATES.Observer'}</t>
         </is>
       </c>
       <c r="T96" t="inlineStr">
@@ -8370,7 +8370,7 @@
       </c>
       <c r="S99" t="inlineStr">
         <is>
-          <t>{'INVERTEBRATES.Observer', 'VERTEBRATES.Observer'}</t>
+          <t>{'VERTEBRATES.Observer', 'INVERTEBRATES.Observer'}</t>
         </is>
       </c>
       <c r="T99" t="inlineStr">
@@ -8450,7 +8450,7 @@
       </c>
       <c r="S100" t="inlineStr">
         <is>
-          <t>{'INVERTEBRATES.UTME', 'INVERTEBRATES.Common_Name', 'INVERTEBRATES.UTMN'}</t>
+          <t>{'INVERTEBRATES.Common_Name', 'INVERTEBRATES.UTMN', 'INVERTEBRATES.UTME'}</t>
         </is>
       </c>
       <c r="T100" t="inlineStr">
@@ -8530,7 +8530,7 @@
       </c>
       <c r="S101" t="inlineStr">
         <is>
-          <t>{'VERTEBRATES.UTME', 'VERTEBRATES.Common_Name', 'VERTEBRATES.Scientific_Name', 'VERTEBRATES.UTMN'}</t>
+          <t>{'VERTEBRATES.Scientific_Name', 'VERTEBRATES.UTMN', 'VERTEBRATES.Common_Name', 'VERTEBRATES.UTME'}</t>
         </is>
       </c>
       <c r="T101" t="inlineStr">
@@ -8595,7 +8595,7 @@
       </c>
       <c r="P102" t="inlineStr">
         <is>
-          <t>{'Roadkill', 'VERTEBRATES'}</t>
+          <t>{'VERTEBRATES', 'Roadkill'}</t>
         </is>
       </c>
       <c r="Q102" t="inlineStr">
@@ -8610,7 +8610,7 @@
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>{'VERTEBRATES.Common_Name', 'Roadkill.Species', 'VERTEBRATES.Species'}</t>
+          <t>{'Roadkill.Species', 'VERTEBRATES.Species', 'VERTEBRATES.Common_Name'}</t>
         </is>
       </c>
       <c r="T102" t="inlineStr">
@@ -8690,7 +8690,7 @@
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>{'INVERTEBRATES.Family', 'INVERTEBRATES.Number'}</t>
+          <t>{'INVERTEBRATES.Number', 'INVERTEBRATES.Family'}</t>
         </is>
       </c>
       <c r="T103" t="inlineStr">
@@ -8850,7 +8850,7 @@
       </c>
       <c r="S105" t="inlineStr">
         <is>
-          <t>{'INVERTEBRATES.Order', 'INVERTEBRATES.Class'}</t>
+          <t>{'INVERTEBRATES.Class', 'INVERTEBRATES.Order'}</t>
         </is>
       </c>
       <c r="T105" t="inlineStr">
@@ -8930,7 +8930,7 @@
       </c>
       <c r="S106" t="inlineStr">
         <is>
-          <t>{'INVERTEBRATES.Location', 'INVERTEBRATES.OBS_TYPE'}</t>
+          <t>{'INVERTEBRATES.OBS_TYPE', 'INVERTEBRATES.Location'}</t>
         </is>
       </c>
       <c r="T106" t="inlineStr">
@@ -9235,7 +9235,7 @@
       </c>
       <c r="P110" t="inlineStr">
         <is>
-          <t>{'Class', 'VERTEBRATES'}</t>
+          <t>{'VERTEBRATES', 'Class'}</t>
         </is>
       </c>
       <c r="Q110" t="inlineStr">
@@ -9250,7 +9250,7 @@
       </c>
       <c r="S110" t="inlineStr">
         <is>
-          <t>{'Class.Field2', 'Class.Class', 'VERTEBRATES.CLASS'}</t>
+          <t>{'VERTEBRATES.CLASS', 'Class.Field2', 'Class.Class'}</t>
         </is>
       </c>
       <c r="T110" t="inlineStr">
@@ -9315,7 +9315,7 @@
       </c>
       <c r="P111" t="inlineStr">
         <is>
-          <t>{'HABITAT_CODES', 'VERTEBRATES'}</t>
+          <t>{'VERTEBRATES', 'HABITAT_CODES'}</t>
         </is>
       </c>
       <c r="Q111" t="inlineStr">
@@ -9330,7 +9330,7 @@
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>{'VERTEBRATES.Number', 'VERTEBRATES.Habitat', 'VERTEBRATES.Common_Name', 'VERTEBRATES.Species', 'HABITAT_CODES.Definition', 'VERTEBRATES.Scientific_Name', 'HABITAT_CODES.Code'}</t>
+          <t>{'VERTEBRATES.Scientific_Name', 'HABITAT_CODES.Definition', 'VERTEBRATES.Species', 'VERTEBRATES.Habitat', 'VERTEBRATES.Number', 'VERTEBRATES.Common_Name', 'HABITAT_CODES.Code'}</t>
         </is>
       </c>
       <c r="T111" t="inlineStr">
@@ -9475,7 +9475,7 @@
       </c>
       <c r="P113" t="inlineStr">
         <is>
-          <t>{'INVERTEBRATES', 'WILDLIFE_MASTERLIST'}</t>
+          <t>{'WILDLIFE_MASTERLIST', 'INVERTEBRATES'}</t>
         </is>
       </c>
       <c r="Q113" t="inlineStr">
@@ -9570,7 +9570,7 @@
       </c>
       <c r="S114" t="inlineStr">
         <is>
-          <t>{'Roadkill.Year', 'Roadkill.Species'}</t>
+          <t>{'Roadkill.Species', 'Roadkill.Year'}</t>
         </is>
       </c>
       <c r="T114" t="inlineStr">
@@ -9635,7 +9635,7 @@
       </c>
       <c r="P115" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Roadkill'}</t>
         </is>
       </c>
       <c r="Q115" t="inlineStr">
@@ -9650,7 +9650,7 @@
       </c>
       <c r="S115" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Roadkill.HWY_Mile_Marker', 'Roadkill.Year', 'Roadkill.Location'}</t>
         </is>
       </c>
       <c r="T115" t="inlineStr">
@@ -9810,7 +9810,7 @@
       </c>
       <c r="S117" t="inlineStr">
         <is>
-          <t>{'VERTEBRATES.Notes', 'VERTEBRATES.Common_Name', 'VERTEBRATES.Observer'}</t>
+          <t>{'VERTEBRATES.Common_Name', 'VERTEBRATES.Observer', 'VERTEBRATES.Notes'}</t>
         </is>
       </c>
       <c r="T117" t="inlineStr">
@@ -9890,7 +9890,7 @@
       </c>
       <c r="S118" t="inlineStr">
         <is>
-          <t>{'INVERTEBRATES.Order', 'INVERTEBRATES.Class', 'INVERTEBRATES.Common_Name', 'INVERTEBRATES.Genus_species', 'INVERTEBRATES.Family', 'INVERTEBRATES.Location'}</t>
+          <t>{'INVERTEBRATES.Common_Name', 'INVERTEBRATES.Genus_species', 'INVERTEBRATES.Class', 'INVERTEBRATES.Order', 'INVERTEBRATES.Family', 'INVERTEBRATES.Location'}</t>
         </is>
       </c>
       <c r="T118" t="inlineStr">
@@ -9970,7 +9970,7 @@
       </c>
       <c r="S119" t="inlineStr">
         <is>
-          <t>{'INVERTEBRATES.Observer', 'INVERTEBRATES.Location'}</t>
+          <t>{'INVERTEBRATES.Location', 'INVERTEBRATES.Observer'}</t>
         </is>
       </c>
       <c r="T119" t="inlineStr">
@@ -10050,7 +10050,7 @@
       </c>
       <c r="S120" t="inlineStr">
         <is>
-          <t>{'INVERTEBRATES.Habitat', 'INVERTEBRATES.Common_Name', 'VERTEBRATES.Common_Name', 'VERTEBRATES.Habitat'}</t>
+          <t>{'INVERTEBRATES.Common_Name', 'VERTEBRATES.Habitat', 'INVERTEBRATES.Habitat', 'VERTEBRATES.Common_Name'}</t>
         </is>
       </c>
       <c r="T120" t="inlineStr">
@@ -10210,7 +10210,7 @@
       </c>
       <c r="S122" t="inlineStr">
         <is>
-          <t>{'tbl_Events.Start_Date', 'tbl_Event_Details.Event_Notes', 'tbl_Event_Details.Event_ID', 'tbl_Events.Location_ID', 'tbl_Events.Event_ID'}</t>
+          <t>{'tbl_Events.Location_ID', 'tbl_Event_Details.Event_Notes', 'tbl_Events.Event_ID', 'tbl_Events.Start_Date', 'tbl_Event_Details.Event_ID'}</t>
         </is>
       </c>
       <c r="T122" t="inlineStr">
@@ -10275,7 +10275,7 @@
       </c>
       <c r="P123" t="inlineStr">
         <is>
-          <t>{'tbl_Events', 'tbl_Locations', 'tbl_Event_Details'}</t>
+          <t>{'tbl_Events', 'tbl_Event_Details', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q123" t="inlineStr">
@@ -10290,7 +10290,7 @@
       </c>
       <c r="S123" t="inlineStr">
         <is>
-          <t>{'tbl_Events.Start_Date', 'tbl_Event_Details.Event_Notes', 'tbl_Events.Location_ID', 'tbl_Locations.Location_ID', 'tbl_Event_Details.Event_ID', 'tbl_Locations.Loc_Name', 'tbl_Events.Event_ID'}</t>
+          <t>{'tbl_Events.Location_ID', 'tbl_Event_Details.Event_Notes', 'tbl_Event_Details.Event_ID', 'tbl_Events.Event_ID', 'tbl_Events.Start_Date', 'tbl_Locations.Location_ID', 'tbl_Locations.Loc_Name'}</t>
         </is>
       </c>
       <c r="T123" t="inlineStr">
@@ -10435,7 +10435,7 @@
       </c>
       <c r="P125" t="inlineStr">
         <is>
-          <t>{'tbl_MacroHabitat', 'tbl_MicroHabitat'}</t>
+          <t>{'tbl_MicroHabitat', 'tbl_MacroHabitat'}</t>
         </is>
       </c>
       <c r="Q125" t="inlineStr">
@@ -10530,7 +10530,7 @@
       </c>
       <c r="S126" t="inlineStr">
         <is>
-          <t>{'tbl_MacroHabitat.Slope', 'tbl_MacroHabitat.Hydrology'}</t>
+          <t>{'tbl_MacroHabitat.Hydrology', 'tbl_MacroHabitat.Slope'}</t>
         </is>
       </c>
       <c r="T126" t="inlineStr">
@@ -10595,7 +10595,7 @@
       </c>
       <c r="P127" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Edit_Log'}</t>
         </is>
       </c>
       <c r="Q127" t="inlineStr">
@@ -10610,7 +10610,7 @@
       </c>
       <c r="S127" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Edit_Log.Table', 'tbl_Edit_Log.Date_Change', 'tbl_Edit_Log.Field', 'tbl_Edit_Log.Reason'}</t>
         </is>
       </c>
       <c r="T127" t="inlineStr">
@@ -10755,7 +10755,7 @@
       </c>
       <c r="P129" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Events', 'tbl_MicroHabitat', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q129" t="inlineStr">
@@ -10770,7 +10770,7 @@
       </c>
       <c r="S129" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Locations.Elevation', 'tbl_MicroHabitat.LightIndex', 'tbl_MicroHabitat.Litter', 'tbl_Events.Event_ID', 'tbl_Events.Start_Date', 'tbl_Locations.Location_ID', 'tbl_MicroHabitat.VegHeight', 'tbl_Events.Location_ID', 'tbl_MicroHabitat.Evergreen', 'tbl_MicroHabitat.Event_ID'}</t>
         </is>
       </c>
       <c r="T129" t="inlineStr">
@@ -11010,7 +11010,7 @@
       </c>
       <c r="S132" t="inlineStr">
         <is>
-          <t>{'tlu_Species_ORCA.Species', 'tlu_Species_ORCA.SampleYear'}</t>
+          <t>{'tlu_Species_ORCA.SampleYear', 'tlu_Species_ORCA.Species'}</t>
         </is>
       </c>
       <c r="T132" t="inlineStr">
@@ -11155,7 +11155,7 @@
       </c>
       <c r="P134" t="inlineStr">
         <is>
-          <t>{'tlu_Species_REDW', 'tlu_Species_WHIS'}</t>
+          <t>{'tlu_Species_WHIS', 'tlu_Species_REDW'}</t>
         </is>
       </c>
       <c r="Q134" t="inlineStr">
@@ -11250,7 +11250,7 @@
       </c>
       <c r="S135" t="inlineStr">
         <is>
-          <t>{'tlu_Species_ORCA.Species', 'tlu_Species_LAVO.Species'}</t>
+          <t>{'tlu_Species_LAVO.Species', 'tlu_Species_ORCA.Species'}</t>
         </is>
       </c>
       <c r="T135" t="inlineStr">
@@ -11330,7 +11330,7 @@
       </c>
       <c r="S136" t="inlineStr">
         <is>
-          <t>{'tlu_Contacts.State_Code', 'tlu_Contacts.First_Name', 'tlu_Contacts.Last_Name', 'tlu_Contacts.Position_Title', 'tlu_Contacts.City', 'tlu_Contacts.Zip_Code'}</t>
+          <t>{'tlu_Contacts.Zip_Code', 'tlu_Contacts.City', 'tlu_Contacts.Position_Title', 'tlu_Contacts.First_Name', 'tlu_Contacts.Last_Name', 'tlu_Contacts.State_Code'}</t>
         </is>
       </c>
       <c r="T136" t="inlineStr">
@@ -11570,7 +11570,7 @@
       </c>
       <c r="S139" t="inlineStr">
         <is>
-          <t>{'tlu_Enumerations.Enum_Group', 'tlu_Enumerations.Enum_Description', 'tlu_Enumerations.Enum_Code'}</t>
+          <t>{'tlu_Enumerations.Enum_Description', 'tlu_Enumerations.Enum_Group', 'tlu_Enumerations.Enum_Code'}</t>
         </is>
       </c>
       <c r="T139" t="inlineStr">
@@ -11715,7 +11715,7 @@
       </c>
       <c r="P141" t="inlineStr">
         <is>
-          <t>{'tlu_Contacts', 'tbl_Db_Revisions'}</t>
+          <t>{'tbl_Db_Revisions', 'tlu_Contacts'}</t>
         </is>
       </c>
       <c r="Q141" t="inlineStr">
@@ -11730,7 +11730,7 @@
       </c>
       <c r="S141" t="inlineStr">
         <is>
-          <t>{'tlu_Contacts.First_Name', 'tbl_Db_Revisions.Revision_Desc', 'tbl_Db_Revisions.Revision_Reason', 'tlu_Contacts.Last_Name', 'tbl_Db_Revisions.Revision_Contact_ID', 'tlu_Contacts.Contact_ID'}</t>
+          <t>{'tbl_Db_Revisions.Revision_Reason', 'tbl_Db_Revisions.Revision_Contact_ID', 'tlu_Contacts.Contact_ID', 'tlu_Contacts.Last_Name', 'tlu_Contacts.First_Name', 'tbl_Db_Revisions.Revision_Desc'}</t>
         </is>
       </c>
       <c r="T141" t="inlineStr">
@@ -11875,7 +11875,7 @@
       </c>
       <c r="P143" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Sites'}</t>
         </is>
       </c>
       <c r="Q143" t="inlineStr">
@@ -11890,7 +11890,7 @@
       </c>
       <c r="S143" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Sites.Site_Desc', 'tbl_Sites.Site_ID', 'tbl_Sites.Route', 'tbl_Sites.Site_Name', 'tbl_Sites.Site_Start_Y', 'tbl_Sites.Length'}</t>
         </is>
       </c>
       <c r="T143" t="inlineStr">
@@ -11970,7 +11970,7 @@
       </c>
       <c r="S144" t="inlineStr">
         <is>
-          <t>{'tbl_Sites.Site_End_Y', 'tbl_Sites.Site_End_X', 'tbl_Sites.Site_Start_Y', 'tbl_Sites.Site_Name', 'tbl_Sites.Site_Start_X'}</t>
+          <t>{'tbl_Sites.Site_End_X', 'tbl_Sites.Site_End_Y', 'tbl_Sites.Site_Start_X', 'tbl_Sites.Site_Name', 'tbl_Sites.Site_Start_Y'}</t>
         </is>
       </c>
       <c r="T144" t="inlineStr">
@@ -12035,7 +12035,7 @@
       </c>
       <c r="P145" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Sites', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q145" t="inlineStr">
@@ -12050,7 +12050,7 @@
       </c>
       <c r="S145" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Sites.Site_Name', 'tbl_Sites.Site_ID', 'tbl_Locations.Site_ID'}</t>
         </is>
       </c>
       <c r="T145" t="inlineStr">
@@ -12115,7 +12115,7 @@
       </c>
       <c r="P146" t="inlineStr">
         <is>
-          <t>{'tbl_Locations', 'tbl_Sites'}</t>
+          <t>{'tbl_Sites', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q146" t="inlineStr">
@@ -12130,7 +12130,7 @@
       </c>
       <c r="S146" t="inlineStr">
         <is>
-          <t>{'tbl_Sites.Site_Name', 'tbl_Locations.Y_Coord', 'tbl_Locations.Site_ID', 'tbl_Locations.X_Coord', 'tbl_Locations.Loc_Name', 'tbl_Sites.Site_ID'}</t>
+          <t>{'tbl_Locations.X_Coord', 'tbl_Locations.Loc_Name', 'tbl_Locations.Y_Coord', 'tbl_Sites.Site_Name', 'tbl_Sites.Site_ID', 'tbl_Locations.Site_ID'}</t>
         </is>
       </c>
       <c r="T146" t="inlineStr">
@@ -12195,7 +12195,7 @@
       </c>
       <c r="P147" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tlu_Contacts', 'xref_Event_Contacts'}</t>
         </is>
       </c>
       <c r="Q147" t="inlineStr">
@@ -12210,7 +12210,7 @@
       </c>
       <c r="S147" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'xref_Event_Contacts.Event_ID', 'tlu_Contacts.Contact_ID', 'xref_Event_Contacts.Contact_ID', 'tlu_Contacts.First_Name'}</t>
         </is>
       </c>
       <c r="T147" t="inlineStr">
@@ -12275,7 +12275,7 @@
       </c>
       <c r="P148" t="inlineStr">
         <is>
-          <t>{'tlu_Contacts', 'tbl_Events', 'xref_Event_Contacts'}</t>
+          <t>{'tbl_Events', 'tlu_Contacts', 'xref_Event_Contacts'}</t>
         </is>
       </c>
       <c r="Q148" t="inlineStr">
@@ -12290,7 +12290,7 @@
       </c>
       <c r="S148" t="inlineStr">
         <is>
-          <t>{'tbl_Events.Start_Date', 'tlu_Contacts.First_Name', 'xref_Event_Contacts.Event_ID', 'tbl_Events.Event_ID', 'xref_Event_Contacts.Contact_ID', 'tlu_Contacts.Last_Name', 'tlu_Contacts.Position_Title', 'tlu_Contacts.Contact_ID'}</t>
+          <t>{'tlu_Contacts.Contact_ID', 'tbl_Events.Event_ID', 'tbl_Events.Start_Date', 'tlu_Contacts.Last_Name', 'xref_Event_Contacts.Event_ID', 'tlu_Contacts.Position_Title', 'xref_Event_Contacts.Contact_ID', 'tlu_Contacts.First_Name'}</t>
         </is>
       </c>
       <c r="T148" t="inlineStr">
@@ -12355,7 +12355,7 @@
       </c>
       <c r="P149" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Events', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q149" t="inlineStr">
@@ -12370,7 +12370,7 @@
       </c>
       <c r="S149" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Events.Location_ID', 'tbl_Locations.Loc_Name', 'tbl_Locations.Location_ID'}</t>
         </is>
       </c>
       <c r="T149" t="inlineStr">
@@ -12435,7 +12435,7 @@
       </c>
       <c r="P150" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Events', 'tbl_Sites', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q150" t="inlineStr">
@@ -12450,7 +12450,7 @@
       </c>
       <c r="S150" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Sites.Site_Desc', 'tbl_Events.Location_ID', 'tbl_Locations.Location_ID', 'tbl_Sites.Site_Name', 'tbl_Sites.Site_ID', 'tbl_Locations.Site_ID'}</t>
         </is>
       </c>
       <c r="T150" t="inlineStr">
@@ -12515,7 +12515,7 @@
       </c>
       <c r="P151" t="inlineStr">
         <is>
-          <t>{'tbl_Locations', 'tbl_Sites'}</t>
+          <t>{'tbl_Sites', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q151" t="inlineStr">
@@ -12530,7 +12530,7 @@
       </c>
       <c r="S151" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.PDOP', 'tbl_Sites.Site_Name', 'tbl_Locations.Site_ID', 'tbl_Locations.HDOP', 'tbl_Locations.EPE', 'tbl_Sites.Site_ID'}</t>
+          <t>{'tbl_Locations.HDOP', 'tbl_Locations.PDOP', 'tbl_Sites.Site_Name', 'tbl_Locations.EPE', 'tbl_Sites.Site_ID', 'tbl_Locations.Site_ID'}</t>
         </is>
       </c>
       <c r="T151" t="inlineStr">
@@ -12755,7 +12755,7 @@
       </c>
       <c r="P154" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Sites', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q154" t="inlineStr">
@@ -12770,7 +12770,7 @@
       </c>
       <c r="S154" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Locations.Loc_Type', 'tbl_Sites.Site_Name', 'tbl_Sites.Site_ID', 'tbl_Locations.Site_ID'}</t>
         </is>
       </c>
       <c r="T154" t="inlineStr">
@@ -12850,7 +12850,7 @@
       </c>
       <c r="S155" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.Watershed', 'tbl_Events.Location_ID', 'tbl_Locations.Location_ID', 'tbl_Locations.Subwatershed', 'tbl_Events.Event_ID'}</t>
+          <t>{'tbl_Locations.Watershed', 'tbl_Events.Location_ID', 'tbl_Events.Event_ID', 'tbl_Locations.Location_ID', 'tbl_Locations.Subwatershed'}</t>
         </is>
       </c>
       <c r="T155" t="inlineStr">
@@ -13090,7 +13090,7 @@
       </c>
       <c r="S158" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.Loc_Type', 'tbl_Locations.Est_H_Error', 'tbl_Locations.Coord_System', 'tbl_Locations.Y_Coord', 'tbl_Locations.X_Coord', 'tbl_Locations.Datum', 'tbl_Locations.Coord_Units', 'tbl_Locations.Loc_Name', 'tbl_Locations.Accuracy_Notes'}</t>
+          <t>{'tbl_Locations.X_Coord', 'tbl_Locations.Coord_Units', 'tbl_Locations.Coord_System', 'tbl_Locations.Est_H_Error', 'tbl_Locations.Y_Coord', 'tbl_Locations.Datum', 'tbl_Locations.Accuracy_Notes', 'tbl_Locations.Loc_Type', 'tbl_Locations.Loc_Name'}</t>
         </is>
       </c>
       <c r="T158" t="inlineStr">
@@ -13250,7 +13250,7 @@
       </c>
       <c r="S160" t="inlineStr">
         <is>
-          <t>{'tbl_Events.Start_Date', 'tbl_MacroHabitat.MacroHab', 'tbl_MacroHabitat.Slope', 'tbl_MacroHabitat.MicroHab', 'tbl_MacroHabitat.Aspect', 'tbl_Events.Event_ID', 'tbl_MacroHabitat.LandUse', 'tbl_MacroHabitat.Event_ID', 'tbl_MacroHabitat.Hydrology'}</t>
+          <t>{'tbl_Events.Event_ID', 'tbl_Events.Start_Date', 'tbl_MacroHabitat.Event_ID', 'tbl_MacroHabitat.MicroHab', 'tbl_MacroHabitat.LandUse', 'tbl_MacroHabitat.Slope', 'tbl_MacroHabitat.Aspect', 'tbl_MacroHabitat.Hydrology', 'tbl_MacroHabitat.MacroHab'}</t>
         </is>
       </c>
       <c r="T160" t="inlineStr">
@@ -13330,7 +13330,7 @@
       </c>
       <c r="S161" t="inlineStr">
         <is>
-          <t>{'tbl_MicroHabitat.BareGround', 'tbl_MicroHabitat.Phenology', 'tbl_MicroHabitat.Deciduous', 'tbl_MicroHabitat.CoverPercent', 'tbl_MicroHabitat.WoodyDebris', 'tbl_MicroHabitat.Rock', 'tbl_MicroHabitat.Herb', 'tbl_MicroHabitat.Litter', 'tbl_MicroHabitat.Shrub'}</t>
+          <t>{'tbl_MicroHabitat.Rock', 'tbl_MicroHabitat.Litter', 'tbl_MicroHabitat.Deciduous', 'tbl_MicroHabitat.WoodyDebris', 'tbl_MicroHabitat.Phenology', 'tbl_MicroHabitat.BareGround', 'tbl_MicroHabitat.Shrub', 'tbl_MicroHabitat.CoverPercent', 'tbl_MicroHabitat.Herb'}</t>
         </is>
       </c>
       <c r="T161" t="inlineStr">
@@ -13570,7 +13570,7 @@
       </c>
       <c r="S164" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.Trail', 'tbl_Locations.Directions'}</t>
+          <t>{'tbl_Locations.Directions', 'tbl_Locations.Trail'}</t>
         </is>
       </c>
       <c r="T164" t="inlineStr">
@@ -13650,7 +13650,7 @@
       </c>
       <c r="S165" t="inlineStr">
         <is>
-          <t>{'tbl_Events.Event_Date', 'tbl_Events.Location_ID', 'tbl_Locations.Location_ID', 'tbl_Locations.SiteDescription'}</t>
+          <t>{'tbl_Locations.SiteDescription', 'tbl_Events.Location_ID', 'tbl_Events.Event_Date', 'tbl_Locations.Location_ID'}</t>
         </is>
       </c>
       <c r="T165" t="inlineStr">
@@ -13715,7 +13715,7 @@
       </c>
       <c r="P166" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies', 'tbl_Nests'}</t>
+          <t>{'tbl_Nests', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q166" t="inlineStr">
@@ -13730,7 +13730,7 @@
       </c>
       <c r="S166" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies.SpeciesCode', 'tlu_PlantSpecies.species', 'tlu_PlantSpecies.genus', 'tlu_PlantSpecies.CommonName', 'tbl_Nests.SpCode', 'tbl_Nests.Event_ID'}</t>
+          <t>{'tlu_PlantSpecies.genus', 'tlu_PlantSpecies.CommonName', 'tbl_Nests.SpCode', 'tlu_PlantSpecies.species', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Nests.Event_ID'}</t>
         </is>
       </c>
       <c r="T166" t="inlineStr">
@@ -13795,7 +13795,7 @@
       </c>
       <c r="P167" t="inlineStr">
         <is>
-          <t>{'tbl_Events', 'tlu_PlantSpecies', 'tbl_Overstory'}</t>
+          <t>{'tbl_Events', 'tbl_Overstory', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q167" t="inlineStr">
@@ -13810,7 +13810,7 @@
       </c>
       <c r="S167" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies.SpeciesCode', 'tbl_Overstory.SpCode', 'tbl_Overstory.Event_ID', 'tbl_Overstory.DBH', 'tbl_Events.Event_ID', 'tlu_PlantSpecies.species'}</t>
+          <t>{'tbl_Overstory.DBH', 'tbl_Overstory.SpCode', 'tbl_Events.Event_ID', 'tbl_Overstory.Event_ID', 'tlu_PlantSpecies.species', 'tlu_PlantSpecies.SpeciesCode'}</t>
         </is>
       </c>
       <c r="T167" t="inlineStr">
@@ -13890,7 +13890,7 @@
       </c>
       <c r="S168" t="inlineStr">
         <is>
-          <t>{'tbl_Saplings.DClass1', 'tbl_Saplings.DClass3', 'tbl_Saplings.DClass4', 'tbl_Saplings.DClass2', 'tbl_Saplings.spcode'}</t>
+          <t>{'tbl_Saplings.spcode', 'tbl_Saplings.DClass3', 'tbl_Saplings.DClass4', 'tbl_Saplings.DClass2', 'tbl_Saplings.DClass1'}</t>
         </is>
       </c>
       <c r="T168" t="inlineStr">
@@ -13970,7 +13970,7 @@
       </c>
       <c r="S169" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies.genus', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Seedlings.SpCode', 'tbl_Seedlings.Density'}</t>
+          <t>{'tlu_PlantSpecies.genus', 'tbl_Seedlings.SpCode', 'tbl_Seedlings.Density', 'tlu_PlantSpecies.SpeciesCode'}</t>
         </is>
       </c>
       <c r="T169" t="inlineStr">
@@ -14035,7 +14035,7 @@
       </c>
       <c r="P170" t="inlineStr">
         <is>
-          <t>{'tbl_Events', 'tbl_Seedlings', 'tlu_PlantSpecies'}</t>
+          <t>{'tbl_Seedlings', 'tbl_Events', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q170" t="inlineStr">
@@ -14050,7 +14050,7 @@
       </c>
       <c r="S170" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies.SpeciesCode', 'tbl_Events.Location_ID', 'tbl_Seedlings.Event_ID', 'tlu_PlantSpecies.genus', 'tbl_Seedlings.SpCode', 'tbl_Seedlings.Density', 'tbl_Events.Event_ID'}</t>
+          <t>{'tbl_Events.Location_ID', 'tbl_Seedlings.SpCode', 'tbl_Seedlings.Density', 'tbl_Events.Event_ID', 'tlu_PlantSpecies.genus', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Seedlings.Event_ID'}</t>
         </is>
       </c>
       <c r="T170" t="inlineStr">
@@ -14130,7 +14130,7 @@
       </c>
       <c r="S171" t="inlineStr">
         <is>
-          <t>{'tlu_PlaceNames.County', 'tlu_PlaceNames.utmN', 'tlu_PlaceNames.utmE', 'tlu_PlaceNames.State'}</t>
+          <t>{'tlu_PlaceNames.utmE', 'tlu_PlaceNames.utmN', 'tlu_PlaceNames.County', 'tlu_PlaceNames.State'}</t>
         </is>
       </c>
       <c r="T171" t="inlineStr">
@@ -14210,7 +14210,7 @@
       </c>
       <c r="S172" t="inlineStr">
         <is>
-          <t>{'tbl_Tree_Tags.Tree_Tag_ID', 'tbl_Tree_Tags.Ycoord', 'tbl_Tree_Tags.Xcoord', 'tbl_Tree_Tags.SpCode'}</t>
+          <t>{'tbl_Tree_Tags.SpCode', 'tbl_Tree_Tags.Tree_Tag_ID', 'tbl_Tree_Tags.Xcoord', 'tbl_Tree_Tags.Ycoord'}</t>
         </is>
       </c>
       <c r="T172" t="inlineStr">
@@ -14275,7 +14275,7 @@
       </c>
       <c r="P173" t="inlineStr">
         <is>
-          <t>{'tbl_Tree_Tags', 'tbl_Overstory'}</t>
+          <t>{'tbl_Overstory', 'tbl_Tree_Tags'}</t>
         </is>
       </c>
       <c r="Q173" t="inlineStr">
@@ -14290,7 +14290,7 @@
       </c>
       <c r="S173" t="inlineStr">
         <is>
-          <t>{'tbl_Tree_Tags.Tree_Tag_ID', 'tbl_Tree_Tags.Tag', 'tbl_Overstory.TreeTag', 'tbl_Overstory.TreeCond'}</t>
+          <t>{'tbl_Overstory.TreeCond', 'tbl_Overstory.TreeTag', 'tbl_Tree_Tags.Tag', 'tbl_Tree_Tags.Tree_Tag_ID'}</t>
         </is>
       </c>
       <c r="T173" t="inlineStr">
@@ -14370,7 +14370,7 @@
       </c>
       <c r="S174" t="inlineStr">
         <is>
-          <t>{'tlu_Tree_Cond.TreeCond_Text', 'tlu_Tree_Cond.TreeCond_Num', 'tbl_Overstory.TreeCond'}</t>
+          <t>{'tlu_Tree_Cond.TreeCond_Num', 'tbl_Overstory.TreeCond', 'tlu_Tree_Cond.TreeCond_Text'}</t>
         </is>
       </c>
       <c r="T174" t="inlineStr">
@@ -14435,7 +14435,7 @@
       </c>
       <c r="P175" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_WitnessTrees'}</t>
         </is>
       </c>
       <c r="Q175" t="inlineStr">
@@ -14450,7 +14450,7 @@
       </c>
       <c r="S175" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_WitnessTrees.Witness_SpCode', 'tbl_WitnessTrees.Witness_DBH', 'tbl_WitnessTrees.Witness_stake', 'tbl_WitnessTrees.Location_ID'}</t>
         </is>
       </c>
       <c r="T175" t="inlineStr">
@@ -14515,7 +14515,7 @@
       </c>
       <c r="P176" t="inlineStr">
         <is>
-          <t>{'tlu_Can_Pos', 'tbl_Overstory'}</t>
+          <t>{'tbl_Overstory', 'tlu_Can_Pos'}</t>
         </is>
       </c>
       <c r="Q176" t="inlineStr">
@@ -14595,7 +14595,7 @@
       </c>
       <c r="P177" t="inlineStr">
         <is>
-          <t>{'tlu_Can_Pos', 'tlu_PlantSpecies', 'tbl_Overstory'}</t>
+          <t>{'tbl_Overstory', 'tlu_Can_Pos', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q177" t="inlineStr">
@@ -14610,7 +14610,7 @@
       </c>
       <c r="S177" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies.SpeciesCode', 'tbl_Overstory.SpCode', 'tbl_Overstory.CanPos', 'tlu_Can_Pos.CanPos_Name', 'tlu_Can_Pos.CanPos_Num', 'tlu_PlantSpecies.CommonName'}</t>
+          <t>{'tlu_Can_Pos.CanPos_Name', 'tbl_Overstory.SpCode', 'tlu_PlantSpecies.CommonName', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Overstory.CanPos', 'tlu_Can_Pos.CanPos_Num'}</t>
         </is>
       </c>
       <c r="T177" t="inlineStr">
@@ -14690,7 +14690,7 @@
       </c>
       <c r="S178" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.Aspect', 'tbl_Locations.Elevation', 'tlu_topo_position.ID', 'tbl_Locations.Slope_shape', 'tbl_Locations.Topo_Position', 'tbl_Locations.Slope', 'tlu_topo_position.TopoPosition', 'tbl_Locations.SiteDescription'}</t>
+          <t>{'tbl_Locations.Topo_Position', 'tbl_Locations.Elevation', 'tbl_Locations.Slope', 'tlu_topo_position.ID', 'tlu_topo_position.TopoPosition', 'tbl_Locations.Slope_shape', 'tbl_Locations.SiteDescription', 'tbl_Locations.Aspect'}</t>
         </is>
       </c>
       <c r="T178" t="inlineStr">
@@ -14755,7 +14755,7 @@
       </c>
       <c r="P179" t="inlineStr">
         <is>
-          <t>{'tlu_Cover_Cls', 'tbl_Nests'}</t>
+          <t>{'tbl_Nests', 'tlu_Cover_Cls'}</t>
         </is>
       </c>
       <c r="Q179" t="inlineStr">
@@ -14770,7 +14770,7 @@
       </c>
       <c r="S179" t="inlineStr">
         <is>
-          <t>{'tlu_Cover_Cls.CoverClass_Num', 'tbl_Nests.SpCode', 'tbl_Nests.Cover', 'tbl_Nests.Nest_ID', 'tlu_Cover_Cls.CoverClass_Text'}</t>
+          <t>{'tbl_Nests.Nest_ID', 'tbl_Nests.SpCode', 'tbl_Nests.Cover', 'tlu_Cover_Cls.CoverClass_Text', 'tlu_Cover_Cls.CoverClass_Num'}</t>
         </is>
       </c>
       <c r="T179" t="inlineStr">
@@ -15010,7 +15010,7 @@
       </c>
       <c r="S182" t="inlineStr">
         <is>
-          <t>{'tlu_DecayStage.DecayStage_ID', 'tbl_Deadwood.Decay', 'tbl_Deadwood.Length', 'tbl_Deadwood.MPD', 'tlu_DecayStage.DecayStage_Descr'}</t>
+          <t>{'tbl_Deadwood.MPD', 'tlu_DecayStage.DecayStage_ID', 'tbl_Deadwood.Decay', 'tlu_DecayStage.DecayStage_Descr', 'tbl_Deadwood.Length'}</t>
         </is>
       </c>
       <c r="T182" t="inlineStr">
@@ -15075,7 +15075,7 @@
       </c>
       <c r="P183" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies', 'tlu_R1_RestOfPlot', 'tbl_Nests'}</t>
+          <t>{'tbl_Nests', 'tlu_R1_RestOfPlot', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q183" t="inlineStr">
@@ -15090,7 +15090,7 @@
       </c>
       <c r="S183" t="inlineStr">
         <is>
-          <t>{'tbl_Nests.R1', 'tlu_PlantSpecies.SpeciesCode', 'tlu_R1_RestOfPlot.Pres_Text', 'tlu_PlantSpecies.genus', 'tlu_R1_RestOfPlot.Pres_Num', 'tbl_Nests.SpCode'}</t>
+          <t>{'tbl_Nests.R1', 'tlu_PlantSpecies.genus', 'tlu_R1_RestOfPlot.Pres_Text', 'tlu_R1_RestOfPlot.Pres_Num', 'tbl_Nests.SpCode', 'tlu_PlantSpecies.SpeciesCode'}</t>
         </is>
       </c>
       <c r="T183" t="inlineStr">
@@ -15155,7 +15155,7 @@
       </c>
       <c r="P184" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q184" t="inlineStr">
@@ -15170,7 +15170,7 @@
       </c>
       <c r="S184" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tlu_PlantSpecies.genus', 'tlu_PlantSpecies.SpeciesNotes'}</t>
         </is>
       </c>
       <c r="T184" t="inlineStr">
@@ -15250,7 +15250,7 @@
       </c>
       <c r="S185" t="inlineStr">
         <is>
-          <t>{'tsys_App_Releases.Author_email', 'tsys_App_Releases.Author_org_name', 'tsys_App_Releases.Database_title', 'tsys_App_Releases.Release_notes', 'tsys_App_Releases.File_name', 'tsys_App_Releases.Release_date'}</t>
+          <t>{'tsys_App_Releases.Author_org_name', 'tsys_App_Releases.Release_notes', 'tsys_App_Releases.Release_date', 'tsys_App_Releases.Author_email', 'tsys_App_Releases.File_name', 'tsys_App_Releases.Database_title'}</t>
         </is>
       </c>
       <c r="T185" t="inlineStr">
@@ -15395,7 +15395,7 @@
       </c>
       <c r="P187" t="inlineStr">
         <is>
-          <t>{'tbl_Events', 'tbl_Seedlings'}</t>
+          <t>{'tbl_Seedlings', 'tbl_Events'}</t>
         </is>
       </c>
       <c r="Q187" t="inlineStr">
@@ -15410,7 +15410,7 @@
       </c>
       <c r="S187" t="inlineStr">
         <is>
-          <t>{'tbl_Events.Location_ID', 'tbl_Seedlings.Event_ID', 'tbl_Events.Event_Date', 'tbl_Seedlings.Density', 'tbl_Events.Event_ID'}</t>
+          <t>{'tbl_Events.Location_ID', 'tbl_Seedlings.Density', 'tbl_Events.Event_ID', 'tbl_Events.Event_Date', 'tbl_Seedlings.Event_ID'}</t>
         </is>
       </c>
       <c r="T187" t="inlineStr">
@@ -15475,7 +15475,7 @@
       </c>
       <c r="P188" t="inlineStr">
         <is>
-          <t>{'tbl_Events', 'tlu_PlantSpecies', 'tbl_Overstory'}</t>
+          <t>{'tbl_Events', 'tbl_Overstory', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q188" t="inlineStr">
@@ -15490,7 +15490,7 @@
       </c>
       <c r="S188" t="inlineStr">
         <is>
-          <t>{'tlu_PlantSpecies.SpeciesCode', 'tbl_Overstory.SpCode', 'tbl_Overstory.Event_ID', 'tbl_Events.Event_Date', 'tbl_Overstory.DBH', 'tbl_Events.Event_ID', 'tlu_PlantSpecies.species'}</t>
+          <t>{'tbl_Overstory.DBH', 'tbl_Overstory.SpCode', 'tbl_Events.Event_ID', 'tbl_Overstory.Event_ID', 'tlu_PlantSpecies.SpeciesCode', 'tlu_PlantSpecies.species', 'tbl_Events.Event_Date'}</t>
         </is>
       </c>
       <c r="T188" t="inlineStr">
@@ -15650,7 +15650,7 @@
       </c>
       <c r="S190" t="inlineStr">
         <is>
-          <t>{'tlu_Roads_and_Trails.Layer', 'tlu_Roads_and_Trails.ValidName'}</t>
+          <t>{'tlu_Roads_and_Trails.ValidName', 'tlu_Roads_and_Trails.Layer'}</t>
         </is>
       </c>
       <c r="T190" t="inlineStr">
@@ -15795,7 +15795,7 @@
       </c>
       <c r="P192" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tlu_PlaceNames'}</t>
         </is>
       </c>
       <c r="Q192" t="inlineStr">
@@ -15810,7 +15810,7 @@
       </c>
       <c r="S192" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tlu_PlaceNames.County', 'tlu_PlaceNames.Name', 'tlu_PlaceNames.utmE', 'tlu_PlaceNames.utmN', 'tlu_PlaceNames.State'}</t>
         </is>
       </c>
       <c r="T192" t="inlineStr">
@@ -15875,7 +15875,7 @@
       </c>
       <c r="P193" t="inlineStr">
         <is>
-          <t>{'tlu_Presence', 'tbl_Nests'}</t>
+          <t>{'tbl_Nests', 'tlu_Presence'}</t>
         </is>
       </c>
       <c r="Q193" t="inlineStr">
@@ -15890,7 +15890,7 @@
       </c>
       <c r="S193" t="inlineStr">
         <is>
-          <t>{'tlu_Presence.Pres_Num', 'tlu_Presence.Pres_Text', 'tbl_Nests.Presence_First', 'tbl_Nests.Event_ID'}</t>
+          <t>{'tbl_Nests.Event_ID', 'tlu_Presence.Pres_Num', 'tbl_Nests.Presence_First', 'tlu_Presence.Pres_Text'}</t>
         </is>
       </c>
       <c r="T193" t="inlineStr">
@@ -16035,7 +16035,7 @@
       </c>
       <c r="P195" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Seedlings', 'tlu_PlantSpecies'}</t>
         </is>
       </c>
       <c r="Q195" t="inlineStr">
@@ -16050,7 +16050,7 @@
       </c>
       <c r="S195" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Seedlings.SpCode', 'tbl_Seedlings.Density', 'tlu_PlantSpecies.CommonName', 'tlu_PlantSpecies.genus', 'tlu_PlantSpecies.species', 'tlu_PlantSpecies.SpeciesCode'}</t>
         </is>
       </c>
       <c r="T195" t="inlineStr">
@@ -16115,7 +16115,7 @@
       </c>
       <c r="P196" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Seedlings', 'tbl_Events'}</t>
         </is>
       </c>
       <c r="Q196" t="inlineStr">
@@ -16130,7 +16130,7 @@
       </c>
       <c r="S196" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Events.Event_Date', 'tbl_Seedlings.Density', 'tbl_Events.Event_ID', 'tbl_Seedlings.Event_ID'}</t>
         </is>
       </c>
       <c r="T196" t="inlineStr">
@@ -16210,7 +16210,7 @@
       </c>
       <c r="S197" t="inlineStr">
         <is>
-          <t>{'tbl_Tree_Tags.Location_ID', 'tlu_PlantSpecies.CommonName', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Tree_Tags.SpCode'}</t>
+          <t>{'tlu_PlantSpecies.CommonName', 'tbl_Tree_Tags.SpCode', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Tree_Tags.Location_ID'}</t>
         </is>
       </c>
       <c r="T197" t="inlineStr">
@@ -16275,7 +16275,7 @@
       </c>
       <c r="P198" t="inlineStr">
         <is>
-          <t>{'tbl_Locations', 'tlu_PlantSpecies', 'tbl_Tree_Tags'}</t>
+          <t>{'tlu_PlantSpecies', 'tbl_Locations', 'tbl_Tree_Tags'}</t>
         </is>
       </c>
       <c r="Q198" t="inlineStr">
@@ -16290,7 +16290,7 @@
       </c>
       <c r="S198" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.Elevation', 'tbl_Tree_Tags.Location_ID', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Locations.Location_ID', 'tlu_PlantSpecies.genus', 'tlu_PlantSpecies.CommonName', 'tbl_Tree_Tags.SpCode'}</t>
+          <t>{'tbl_Locations.Elevation', 'tlu_PlantSpecies.genus', 'tlu_PlantSpecies.CommonName', 'tbl_Locations.Location_ID', 'tbl_Tree_Tags.Location_ID', 'tlu_PlantSpecies.SpeciesCode', 'tbl_Tree_Tags.SpCode'}</t>
         </is>
       </c>
       <c r="T198" t="inlineStr">
@@ -16370,7 +16370,7 @@
       </c>
       <c r="S199" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.Plot_ID', 'tbl_Locations.Datum', 'tbl_Locations.Coord_System', 'tbl_Locations.Coord_Units', 'tbl_Locations.Eco_Notes'}</t>
+          <t>{'tbl_Locations.Datum', 'tbl_Locations.Coord_Units', 'tbl_Locations.Coord_System', 'tbl_Locations.Eco_Notes', 'tbl_Locations.Plot_ID'}</t>
         </is>
       </c>
       <c r="T199" t="inlineStr">
@@ -16450,7 +16450,7 @@
       </c>
       <c r="S200" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.Loc_Notes', 'tbl_Locations.Other_Disturbance'}</t>
+          <t>{'tbl_Locations.Other_Disturbance', 'tbl_Locations.Loc_Notes'}</t>
         </is>
       </c>
       <c r="T200" t="inlineStr">
@@ -16515,7 +16515,7 @@
       </c>
       <c r="P201" t="inlineStr">
         <is>
-          <t>{'tbl_Deadwood', 'tbl_Overstory'}</t>
+          <t>{'tbl_Overstory', 'tbl_Deadwood'}</t>
         </is>
       </c>
       <c r="Q201" t="inlineStr">
@@ -17170,7 +17170,7 @@
       </c>
       <c r="S209" t="inlineStr">
         <is>
-          <t>{'JKWGT.CATEGORY', 'JKWGT.JKWGT5'}</t>
+          <t>{'JKWGT.JKWGT5', 'JKWGT.CATEGORY'}</t>
         </is>
       </c>
       <c r="T209" t="inlineStr">
@@ -17250,7 +17250,7 @@
       </c>
       <c r="S210" t="inlineStr">
         <is>
-          <t>{'GV.ALCTESTRESULT', 'GV.CASEID'}</t>
+          <t>{'GV.CASEID', 'GV.ALCTESTRESULT'}</t>
         </is>
       </c>
       <c r="T210" t="inlineStr">
@@ -17315,7 +17315,7 @@
       </c>
       <c r="P211" t="inlineStr">
         <is>
-          <t>{'VPICDECODE', 'GV'}</t>
+          <t>{'GV', 'VPICDECODE'}</t>
         </is>
       </c>
       <c r="Q211" t="inlineStr">
@@ -17330,7 +17330,7 @@
       </c>
       <c r="S211" t="inlineStr">
         <is>
-          <t>{'GV.CURBWT', 'VPICDECODE.Make', 'GV.VEHNO', 'GV.MODEL', 'GV.MAKE', 'VPICDECODE.Model', 'VPICDECODE.CASEID', 'VPICDECODE.VEHNO', 'GV.CASEID'}</t>
+          <t>{'GV.CURBWT', 'GV.CASEID', 'GV.MAKE', 'VPICDECODE.VEHNO', 'GV.VEHNO', 'VPICDECODE.CASEID', 'VPICDECODE.Model', 'GV.MODEL', 'VPICDECODE.Make'}</t>
         </is>
       </c>
       <c r="T211" t="inlineStr">
@@ -17715,7 +17715,7 @@
       </c>
       <c r="P216" t="inlineStr">
         <is>
-          <t>{'EDRPRECRASH', 'GV'}</t>
+          <t>{'GV', 'EDRPRECRASH'}</t>
         </is>
       </c>
       <c r="Q216" t="inlineStr">
@@ -17730,7 +17730,7 @@
       </c>
       <c r="S216" t="inlineStr">
         <is>
-          <t>{'GV.SPEEDLIMIT', 'EDRPRECRASH.CASEID', 'EDRPRECRASH.PCODE', 'GV.VEHNO', 'EDRPRECRASH.PVALUE', 'GV.CASEID', 'EDRPRECRASH.VEHNO'}</t>
+          <t>{'EDRPRECRASH.VEHNO', 'EDRPRECRASH.CASEID', 'GV.CASEID', 'GV.SPEEDLIMIT', 'EDRPRECRASH.PCODE', 'EDRPRECRASH.PVALUE', 'GV.VEHNO'}</t>
         </is>
       </c>
       <c r="T216" t="inlineStr">
@@ -17970,7 +17970,7 @@
       </c>
       <c r="S219" t="inlineStr">
         <is>
-          <t>{'INTRUSION.CASEID', 'INTRUSION.VEHNO', 'INTRUSION.INTMAG'}</t>
+          <t>{'INTRUSION.INTMAG', 'INTRUSION.CASEID', 'INTRUSION.VEHNO'}</t>
         </is>
       </c>
       <c r="T219" t="inlineStr">
@@ -18050,7 +18050,7 @@
       </c>
       <c r="S220" t="inlineStr">
         <is>
-          <t>{'INTRUSION.CASEID', 'INTRUSION.INTMAG'}</t>
+          <t>{'INTRUSION.INTMAG', 'INTRUSION.CASEID'}</t>
         </is>
       </c>
       <c r="T220" t="inlineStr">
@@ -18130,7 +18130,7 @@
       </c>
       <c r="S221" t="inlineStr">
         <is>
-          <t>{'INTRUSION.CASEID', 'INTRUSION.INTMAG', 'INTRUSION.INTDIRECT', 'INTRUSION.VEHNO', 'INTRUSION.INTCOMP'}</t>
+          <t>{'INTRUSION.INTCOMP', 'INTRUSION.INTDIRECT', 'INTRUSION.CASEID', 'INTRUSION.INTMAG', 'INTRUSION.VEHNO'}</t>
         </is>
       </c>
       <c r="T221" t="inlineStr">
@@ -18210,7 +18210,7 @@
       </c>
       <c r="S222" t="inlineStr">
         <is>
-          <t>{'INTRUSION.CASEID', 'INTRUSION.VEHNO', 'INTRUSION.INTDIRECT'}</t>
+          <t>{'INTRUSION.INTDIRECT', 'INTRUSION.CASEID', 'INTRUSION.VEHNO'}</t>
         </is>
       </c>
       <c r="T222" t="inlineStr">
@@ -18675,7 +18675,7 @@
       </c>
       <c r="P228" t="inlineStr">
         <is>
-          <t>{'INJURY', 'VPICDECODE'}</t>
+          <t>{'VPICDECODE', 'INJURY'}</t>
         </is>
       </c>
       <c r="Q228" t="inlineStr">
@@ -18690,7 +18690,7 @@
       </c>
       <c r="S228" t="inlineStr">
         <is>
-          <t>{'VPICDECODE.Make', 'INJURY.VEHNO', 'INJURY.CASEID', 'VPICDECODE.CASEID', 'INJURY.AIS', 'VPICDECODE.VEHNO'}</t>
+          <t>{'VPICDECODE.CASEID', 'VPICDECODE.Make', 'INJURY.VEHNO', 'VPICDECODE.VEHNO', 'INJURY.CASEID', 'INJURY.AIS'}</t>
         </is>
       </c>
       <c r="T228" t="inlineStr">
@@ -18755,7 +18755,7 @@
       </c>
       <c r="P229" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'VPICDECODE', 'INJURY'}</t>
         </is>
       </c>
       <c r="Q229" t="inlineStr">
@@ -18770,7 +18770,7 @@
       </c>
       <c r="S229" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'VPICDECODE.CASEID', 'INJURY.VEHNO', 'VPICDECODE.VEHNO', 'INJURY.CASEID', 'VPICDECODE.Make', 'INJURY.REGION'}</t>
         </is>
       </c>
       <c r="T229" t="inlineStr">
@@ -19170,7 +19170,7 @@
       </c>
       <c r="S234" t="inlineStr">
         <is>
-          <t>{'EMSCARE.SCENEARR', 'EMSCARE.ARRMEDICAL', 'EMSCARE.EMSTYPE', 'EMSCARE.CASEID', 'EMSCARE.SCENEDEP', 'EMSCARE.NOTIFIED'}</t>
+          <t>{'EMSCARE.ARRMEDICAL', 'EMSCARE.NOTIFIED', 'EMSCARE.CASEID', 'EMSCARE.SCENEARR', 'EMSCARE.EMSTYPE', 'EMSCARE.SCENEDEP'}</t>
         </is>
       </c>
       <c r="T234" t="inlineStr">
@@ -19250,7 +19250,7 @@
       </c>
       <c r="S235" t="inlineStr">
         <is>
-          <t>{'VPICDECODE.Make', 'VPICDECODE.Model'}</t>
+          <t>{'VPICDECODE.Model', 'VPICDECODE.Make'}</t>
         </is>
       </c>
       <c r="T235" t="inlineStr">
@@ -19395,7 +19395,7 @@
       </c>
       <c r="P237" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'VPICDECODE'}</t>
         </is>
       </c>
       <c r="Q237" t="inlineStr">
@@ -19410,7 +19410,7 @@
       </c>
       <c r="S237" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'VPICDECODE.Make', 'VPICDECODE.ModelYear'}</t>
         </is>
       </c>
       <c r="T237" t="inlineStr">
@@ -19810,7 +19810,7 @@
       </c>
       <c r="S242" t="inlineStr">
         <is>
-          <t>{'CDC.CDCPLANE', 'CDC.CASEID', 'CDC.VEHNO'}</t>
+          <t>{'CDC.CASEID', 'CDC.VEHNO', 'CDC.CDCPLANE'}</t>
         </is>
       </c>
       <c r="T242" t="inlineStr">
@@ -19890,7 +19890,7 @@
       </c>
       <c r="S243" t="inlineStr">
         <is>
-          <t>{'INTERIOR.GLAZINGCONT', 'INTERIOR.CASEID'}</t>
+          <t>{'INTERIOR.CASEID', 'INTERIOR.GLAZINGCONT'}</t>
         </is>
       </c>
       <c r="T243" t="inlineStr">
@@ -19955,7 +19955,7 @@
       </c>
       <c r="P244" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'TIREPLAC'}</t>
         </is>
       </c>
       <c r="Q244" t="inlineStr">
@@ -19970,7 +19970,7 @@
       </c>
       <c r="S244" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'TIREPLAC.RECFRONT1'}</t>
         </is>
       </c>
       <c r="T244" t="inlineStr">
@@ -20115,7 +20115,7 @@
       </c>
       <c r="P246" t="inlineStr">
         <is>
-          <t>{'GLAZING', 'GV'}</t>
+          <t>{'GV', 'GLAZING'}</t>
         </is>
       </c>
       <c r="Q246" t="inlineStr">
@@ -20130,7 +20130,7 @@
       </c>
       <c r="S246" t="inlineStr">
         <is>
-          <t>{'GV.VEHNO', 'GLAZING.CASEID', 'GLAZING.GLAZIMP', 'GLAZING.VEHNO', 'GV.CASEID', 'GV.VIN'}</t>
+          <t>{'GV.VIN', 'GV.CASEID', 'GLAZING.VEHNO', 'GLAZING.CASEID', 'GLAZING.GLAZIMP', 'GV.VEHNO'}</t>
         </is>
       </c>
       <c r="T246" t="inlineStr">
@@ -20275,7 +20275,7 @@
       </c>
       <c r="P248" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'EDRPOSTCRASH'}</t>
         </is>
       </c>
       <c r="Q248" t="inlineStr">
@@ -20290,7 +20290,7 @@
       </c>
       <c r="S248" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'EDRPOSTCRASH.PCODE', 'EDRPOSTCRASH.PVALUE'}</t>
         </is>
       </c>
       <c r="T248" t="inlineStr">
@@ -20450,7 +20450,7 @@
       </c>
       <c r="S250" t="inlineStr">
         <is>
-          <t>{'EDRPRECRASH.CASEID', 'EDRPRECRASH.PVALUE', 'EDRPRECRASH.PCODE'}</t>
+          <t>{'EDRPRECRASH.PCODE', 'EDRPRECRASH.PVALUE', 'EDRPRECRASH.CASEID'}</t>
         </is>
       </c>
       <c r="T250" t="inlineStr">
@@ -20530,7 +20530,7 @@
       </c>
       <c r="S251" t="inlineStr">
         <is>
-          <t>{'EDRPRECRASH.CASEID', 'VPICDECODE.Make', 'EDRPRECRASH.PVALUE', 'EDRPRECRASH.PCODE', 'VPICDECODE.Model', 'VPICDECODE.CASEID', 'VPICDECODE.VEHNO', 'EDRPRECRASH.VEHNO'}</t>
+          <t>{'VPICDECODE.VEHNO', 'EDRPRECRASH.PCODE', 'VPICDECODE.CASEID', 'VPICDECODE.Model', 'EDRPRECRASH.CASEID', 'EDRPRECRASH.VEHNO', 'EDRPRECRASH.PVALUE', 'VPICDECODE.Make'}</t>
         </is>
       </c>
       <c r="T251" t="inlineStr">
@@ -20930,7 +20930,7 @@
       </c>
       <c r="S256" t="inlineStr">
         <is>
-          <t>{'OCC.HEIGHT', 'OCC.AGE'}</t>
+          <t>{'OCC.AGE', 'OCC.HEIGHT'}</t>
         </is>
       </c>
       <c r="T256" t="inlineStr">
@@ -21010,7 +21010,7 @@
       </c>
       <c r="S257" t="inlineStr">
         <is>
-          <t>{'OCC.CASEID', 'OCC.FETALMORT'}</t>
+          <t>{'OCC.FETALMORT', 'OCC.CASEID'}</t>
         </is>
       </c>
       <c r="T257" t="inlineStr">
@@ -21090,7 +21090,7 @@
       </c>
       <c r="S258" t="inlineStr">
         <is>
-          <t>{'OCC.CASEID', 'OCC.BELTAVAIL'}</t>
+          <t>{'OCC.BELTAVAIL', 'OCC.CASEID'}</t>
         </is>
       </c>
       <c r="T258" t="inlineStr">
@@ -21250,7 +21250,7 @@
       </c>
       <c r="S260" t="inlineStr">
         <is>
-          <t>{'OCC.BELTUSE', 'OCC.BELTAVAIL'}</t>
+          <t>{'OCC.BELTAVAIL', 'OCC.BELTUSE'}</t>
         </is>
       </c>
       <c r="T260" t="inlineStr">
@@ -21490,7 +21490,7 @@
       </c>
       <c r="S263" t="inlineStr">
         <is>
-          <t>{'CDC.CASEID', 'CDC.PDOF', 'CDC.VEHNO'}</t>
+          <t>{'CDC.CASEID', 'CDC.VEHNO', 'CDC.PDOF'}</t>
         </is>
       </c>
       <c r="T263" t="inlineStr">
@@ -21635,7 +21635,7 @@
       </c>
       <c r="P265" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'CDC'}</t>
         </is>
       </c>
       <c r="Q265" t="inlineStr">
@@ -21650,7 +21650,7 @@
       </c>
       <c r="S265" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'CDC.CMAX'}</t>
         </is>
       </c>
       <c r="T265" t="inlineStr">
@@ -21730,7 +21730,7 @@
       </c>
       <c r="S266" t="inlineStr">
         <is>
-          <t>{'CDC.DAMAPILLAR', 'CDC.CASEID', 'CDC.VEHNO'}</t>
+          <t>{'CDC.CASEID', 'CDC.VEHNO', 'CDC.DAMAPILLAR'}</t>
         </is>
       </c>
       <c r="T266" t="inlineStr">
@@ -21955,7 +21955,7 @@
       </c>
       <c r="P269" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'CDC'}</t>
         </is>
       </c>
       <c r="Q269" t="inlineStr">
@@ -21970,7 +21970,7 @@
       </c>
       <c r="S269" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'CDC.DVBARRIER'}</t>
         </is>
       </c>
       <c r="T269" t="inlineStr">
@@ -22050,7 +22050,7 @@
       </c>
       <c r="S270" t="inlineStr">
         <is>
-          <t>{'CDC.CASEID', 'CDC.C5', 'CDC.VEHNO', 'CDC.CMAX', 'CDC.C1', 'CDC.C4', 'CDC.C6', 'CDC.C3', 'CDC.C2'}</t>
+          <t>{'CDC.C1', 'CDC.C2', 'CDC.CASEID', 'CDC.C3', 'CDC.CMAX', 'CDC.VEHNO', 'CDC.C5', 'CDC.C6', 'CDC.C4'}</t>
         </is>
       </c>
       <c r="T270" t="inlineStr">
@@ -22130,7 +22130,7 @@
       </c>
       <c r="S271" t="inlineStr">
         <is>
-          <t>{'EDREVENT.EDRSUMMNO', 'EDREVENT.VEHNO', 'EDREVENT.CASEID'}</t>
+          <t>{'EDREVENT.CASEID', 'EDREVENT.VEHNO', 'EDREVENT.EDRSUMMNO'}</t>
         </is>
       </c>
       <c r="T271" t="inlineStr">
@@ -22210,7 +22210,7 @@
       </c>
       <c r="S272" t="inlineStr">
         <is>
-          <t>{'EDRPRECRASH.CASEID', 'EDRPRECRASH.EDREVENTNO', 'EDREVENT.CASEID', 'EDREVENT.EDREVENTNO'}</t>
+          <t>{'EDRPRECRASH.CASEID', 'EDREVENT.EDREVENTNO', 'EDREVENT.CASEID', 'EDRPRECRASH.EDREVENTNO'}</t>
         </is>
       </c>
       <c r="T272" t="inlineStr">
@@ -22290,7 +22290,7 @@
       </c>
       <c r="S273" t="inlineStr">
         <is>
-          <t>{'VPICDECODE.Make', 'EDREVENT.CASEID', 'VPICDECODE.ModelYear', 'EDREVENT.VEHNO', 'VPICDECODE.Model', 'EDREVENT.IGCYCRASH', 'VPICDECODE.CASEID', 'VPICDECODE.VEHNO'}</t>
+          <t>{'EDREVENT.IGCYCRASH', 'VPICDECODE.VEHNO', 'EDREVENT.VEHNO', 'VPICDECODE.ModelYear', 'VPICDECODE.CASEID', 'VPICDECODE.Model', 'VPICDECODE.Make', 'EDREVENT.CASEID'}</t>
         </is>
       </c>
       <c r="T273" t="inlineStr">
@@ -22370,7 +22370,7 @@
       </c>
       <c r="S274" t="inlineStr">
         <is>
-          <t>{'EDREVENT.VEHNO', 'EDREVENT.CASEID', 'EDREVENT.IGCYCRASH'}</t>
+          <t>{'EDREVENT.CASEID', 'EDREVENT.IGCYCRASH', 'EDREVENT.VEHNO'}</t>
         </is>
       </c>
       <c r="T274" t="inlineStr">
@@ -22450,7 +22450,7 @@
       </c>
       <c r="S275" t="inlineStr">
         <is>
-          <t>{'INJURY.INJNO', 'INJURY.VEHNO', 'INJURY.CASEID', 'INJURY.OCCNO'}</t>
+          <t>{'INJURY.CASEID', 'INJURY.OCCNO', 'INJURY.INJNO', 'INJURY.VEHNO'}</t>
         </is>
       </c>
       <c r="T275" t="inlineStr">
@@ -22530,7 +22530,7 @@
       </c>
       <c r="S276" t="inlineStr">
         <is>
-          <t>{'FUEL.FUELTYPE', 'FIRE.VEHNO', 'FUEL.CASEID', 'FUEL.VEHNO', 'FIRE.CASEID'}</t>
+          <t>{'FUEL.FUELTYPE', 'FIRE.CASEID', 'FIRE.VEHNO', 'FUEL.CASEID', 'FUEL.VEHNO'}</t>
         </is>
       </c>
       <c r="T276" t="inlineStr">
@@ -22595,7 +22595,7 @@
       </c>
       <c r="P277" t="inlineStr">
         <is>
-          <t>{'EJECT', 'OCC'}</t>
+          <t>{'OCC', 'EJECT'}</t>
         </is>
       </c>
       <c r="Q277" t="inlineStr">
@@ -22610,7 +22610,7 @@
       </c>
       <c r="S277" t="inlineStr">
         <is>
-          <t>{'OCC.VEHNO', 'EJECT.CASEID', 'EJECT.OCCNO', 'OCC.OCCNO', 'OCC.CASEID', 'OCC.SEX', 'EJECT.VEHNO'}</t>
+          <t>{'EJECT.OCCNO', 'EJECT.CASEID', 'OCC.CASEID', 'OCC.SEX', 'OCC.VEHNO', 'EJECT.VEHNO', 'OCC.OCCNO'}</t>
         </is>
       </c>
       <c r="T277" t="inlineStr">
@@ -22835,7 +22835,7 @@
       </c>
       <c r="P280" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'AVOID'}</t>
         </is>
       </c>
       <c r="Q280" t="inlineStr">
@@ -22850,7 +22850,7 @@
       </c>
       <c r="S280" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'AVOID.AVAIL', 'AVOID.EQUIP'}</t>
         </is>
       </c>
       <c r="T280" t="inlineStr">
@@ -22930,7 +22930,7 @@
       </c>
       <c r="S281" t="inlineStr">
         <is>
-          <t>{'AVOID.EQUIP', 'AVOID.CASEID', 'AVOID.VEHNO', 'AVOID.AVAIL'}</t>
+          <t>{'AVOID.AVAIL', 'AVOID.CASEID', 'AVOID.EQUIP', 'AVOID.VEHNO'}</t>
         </is>
       </c>
       <c r="T281" t="inlineStr">
@@ -23170,7 +23170,7 @@
       </c>
       <c r="S284" t="inlineStr">
         <is>
-          <t>{'TIREPLAC.GVWR', 'TIREPLAC.GAWRFRONT', 'TIREPLAC.GAWRREAR'}</t>
+          <t>{'TIREPLAC.GAWRFRONT', 'TIREPLAC.GAWRREAR', 'TIREPLAC.GVWR'}</t>
         </is>
       </c>
       <c r="T284" t="inlineStr">
@@ -23250,7 +23250,7 @@
       </c>
       <c r="S285" t="inlineStr">
         <is>
-          <t>{'TIREPLAC.GVWR', 'TIREPLAC.RECFRPRESS1', 'TIREPLAC.RECRRPRESS1'}</t>
+          <t>{'TIREPLAC.GVWR', 'TIREPLAC.RECRRPRESS1', 'TIREPLAC.RECFRPRESS1'}</t>
         </is>
       </c>
       <c r="T285" t="inlineStr">
@@ -23395,7 +23395,7 @@
       </c>
       <c r="P287" t="inlineStr">
         <is>
-          <t>{'VPICDECODE', 'TIREPLAC'}</t>
+          <t>{'TIREPLAC', 'VPICDECODE'}</t>
         </is>
       </c>
       <c r="Q287" t="inlineStr">
@@ -23410,7 +23410,7 @@
       </c>
       <c r="S287" t="inlineStr">
         <is>
-          <t>{'TIREPLAC.VEHNO', 'VPICDECODE.Make', 'TIREPLAC.RECFRONT1', 'VPICDECODE.Model', 'VPICDECODE.CASEID', 'TIREPLAC.CASEID', 'VPICDECODE.VEHNO', 'TIREPLAC.RECREAR1'}</t>
+          <t>{'TIREPLAC.RECFRONT1', 'VPICDECODE.VEHNO', 'TIREPLAC.VEHNO', 'VPICDECODE.CASEID', 'VPICDECODE.Model', 'TIREPLAC.CASEID', 'TIREPLAC.RECREAR1', 'VPICDECODE.Make'}</t>
         </is>
       </c>
       <c r="T287" t="inlineStr">
@@ -23475,7 +23475,7 @@
       </c>
       <c r="P288" t="inlineStr">
         <is>
-          <t>{'VPICDECODE', 'TIREPLAC'}</t>
+          <t>{'TIREPLAC', 'VPICDECODE'}</t>
         </is>
       </c>
       <c r="Q288" t="inlineStr">
@@ -23490,7 +23490,7 @@
       </c>
       <c r="S288" t="inlineStr">
         <is>
-          <t>{'TIREPLAC.VEHNO', 'VPICDECODE.Make', 'TIREPLAC.RECRRPRESS1', 'TIREPLAC.RECFRONT1', 'TIREPLAC.RECFRPRESS1', 'VPICDECODE.ModelYear', 'VPICDECODE.Model', 'VPICDECODE.CASEID', 'TIREPLAC.CASEID', 'VPICDECODE.VEHNO', 'TIREPLAC.RECREAR1'}</t>
+          <t>{'TIREPLAC.RECFRONT1', 'VPICDECODE.VEHNO', 'TIREPLAC.VEHNO', 'TIREPLAC.RECRRPRESS1', 'TIREPLAC.RECFRPRESS1', 'VPICDECODE.CASEID', 'VPICDECODE.Model', 'TIREPLAC.CASEID', 'TIREPLAC.RECREAR1', 'VPICDECODE.Make', 'VPICDECODE.ModelYear'}</t>
         </is>
       </c>
       <c r="T288" t="inlineStr">
@@ -23570,7 +23570,7 @@
       </c>
       <c r="S289" t="inlineStr">
         <is>
-          <t>{'TIRE.CASEID', 'TIRE.VEHNO', 'TIRE.TIREMODEL'}</t>
+          <t>{'TIRE.TIREMODEL', 'TIRE.CASEID', 'TIRE.VEHNO'}</t>
         </is>
       </c>
       <c r="T289" t="inlineStr">
@@ -23635,7 +23635,7 @@
       </c>
       <c r="P290" t="inlineStr">
         <is>
-          <t>{'VPICDECODE', 'TIRE'}</t>
+          <t>{'TIRE', 'VPICDECODE'}</t>
         </is>
       </c>
       <c r="Q290" t="inlineStr">
@@ -23650,7 +23650,7 @@
       </c>
       <c r="S290" t="inlineStr">
         <is>
-          <t>{'VPICDECODE.Make', 'TIRE.VEHNO', 'VPICDECODE.Model', 'TIRE.TIREMODEL', 'TIRE.CASEID', 'VPICDECODE.CASEID', 'VPICDECODE.VEHNO'}</t>
+          <t>{'VPICDECODE.CASEID', 'VPICDECODE.Model', 'TIRE.CASEID', 'TIRE.VEHNO', 'VPICDECODE.VEHNO', 'TIRE.TIREMODEL', 'VPICDECODE.Make'}</t>
         </is>
       </c>
       <c r="T290" t="inlineStr">
@@ -23730,7 +23730,7 @@
       </c>
       <c r="S291" t="inlineStr">
         <is>
-          <t>{'TIRE.CASEID', 'TIRE.VEHNO', 'TIRE.TIREMODEL'}</t>
+          <t>{'TIRE.TIREMODEL', 'TIRE.CASEID', 'TIRE.VEHNO'}</t>
         </is>
       </c>
       <c r="T291" t="inlineStr">
@@ -23795,7 +23795,7 @@
       </c>
       <c r="P292" t="inlineStr">
         <is>
-          <t>{'TIRE', 'TIREDAMAGE'}</t>
+          <t>{'TIREDAMAGE', 'TIRE'}</t>
         </is>
       </c>
       <c r="Q292" t="inlineStr">
@@ -23810,7 +23810,7 @@
       </c>
       <c r="S292" t="inlineStr">
         <is>
-          <t>{'TIREDAMAGE.CASEID', 'TIRE.VEHNO', 'TIRE.TIREMODEL', 'TIRE.CASEID', 'TIREDAMAGE.VEHNO', 'TIREDAMAGE.DAMAGE'}</t>
+          <t>{'TIREDAMAGE.CASEID', 'TIRE.CASEID', 'TIREDAMAGE.VEHNO', 'TIRE.VEHNO', 'TIREDAMAGE.DAMAGE', 'TIRE.TIREMODEL'}</t>
         </is>
       </c>
       <c r="T292" t="inlineStr">
@@ -23890,7 +23890,7 @@
       </c>
       <c r="S293" t="inlineStr">
         <is>
-          <t>{'TIREPLAC.VEHNO', 'TIRE.VEHNO', 'TIREPLAC.RECFRONT1', 'TIRE.CASEID', 'TIREPLAC.CASEID', 'TIRE.TIRESIZE', 'TIRE.TIRELOC'}</t>
+          <t>{'TIREPLAC.RECFRONT1', 'TIRE.CASEID', 'TIRE.VEHNO', 'TIRE.TIRELOC', 'TIREPLAC.VEHNO', 'TIREPLAC.CASEID', 'TIRE.TIRESIZE'}</t>
         </is>
       </c>
       <c r="T293" t="inlineStr">
@@ -23955,7 +23955,7 @@
       </c>
       <c r="P294" t="inlineStr">
         <is>
-          <t>{'VPICDECODE', 'TIREPLAC', 'TIRE'}</t>
+          <t>{'TIREPLAC', 'TIRE', 'VPICDECODE'}</t>
         </is>
       </c>
       <c r="Q294" t="inlineStr">
@@ -23970,7 +23970,7 @@
       </c>
       <c r="S294" t="inlineStr">
         <is>
-          <t>{'TIREPLAC.VEHNO', 'VPICDECODE.Make', 'TIRE.VEHNO', 'TIREPLAC.RECFRONT1', 'TIRE.TIRELOC', 'VPICDECODE.Model', 'TIRE.CASEID', 'VPICDECODE.CASEID', 'TIREPLAC.CASEID', 'VPICDECODE.VEHNO', 'TIRE.TIRESIZE'}</t>
+          <t>{'TIREPLAC.RECFRONT1', 'TIRE.CASEID', 'TIRE.TIRELOC', 'TIREPLAC.VEHNO', 'VPICDECODE.VEHNO', 'TIRE.TIRESIZE', 'VPICDECODE.CASEID', 'VPICDECODE.Model', 'TIRE.VEHNO', 'TIREPLAC.CASEID', 'VPICDECODE.Make'}</t>
         </is>
       </c>
       <c r="T294" t="inlineStr">
@@ -24035,7 +24035,7 @@
       </c>
       <c r="P295" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'TIREPLAC', 'TIRE', 'VPICDECODE'}</t>
         </is>
       </c>
       <c r="Q295" t="inlineStr">
@@ -24050,7 +24050,7 @@
       </c>
       <c r="S295" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'TIREPLAC.RECFRONT1', 'TIRE.CASEID', 'TIRE.TIRELOC', 'TIREPLAC.VEHNO', 'VPICDECODE.VEHNO', 'TIRE.TIRESIZE', 'VPICDECODE.CASEID', 'TIRE.VEHNO', 'TIREPLAC.CASEID', 'VPICDECODE.Make'}</t>
         </is>
       </c>
       <c r="T295" t="inlineStr">
@@ -24210,7 +24210,7 @@
       </c>
       <c r="S297" t="inlineStr">
         <is>
-          <t>{'CHILDSEAT.OCCNO', 'CHILDSEAT.CASEID', 'DISTRACT.CASEID'}</t>
+          <t>{'DISTRACT.CASEID', 'CHILDSEAT.OCCNO', 'CHILDSEAT.CASEID'}</t>
         </is>
       </c>
       <c r="T297" t="inlineStr">
@@ -24275,7 +24275,7 @@
       </c>
       <c r="P298" t="inlineStr">
         <is>
-          <t>{'VPICDECODE', 'CHILDSEAT'}</t>
+          <t>{'CHILDSEAT', 'VPICDECODE'}</t>
         </is>
       </c>
       <c r="Q298" t="inlineStr">
@@ -24290,7 +24290,7 @@
       </c>
       <c r="S298" t="inlineStr">
         <is>
-          <t>{'VPICDECODE.Make', 'CHILDSEAT.VEHNO', 'VPICDECODE.Model', 'VPICDECODE.CASEID', 'VPICDECODE.VEHNO', 'CHILDSEAT.CASEID'}</t>
+          <t>{'VPICDECODE.CASEID', 'VPICDECODE.Model', 'CHILDSEAT.CASEID', 'CHILDSEAT.VEHNO', 'VPICDECODE.VEHNO', 'VPICDECODE.Make'}</t>
         </is>
       </c>
       <c r="T298" t="inlineStr">
@@ -24355,7 +24355,7 @@
       </c>
       <c r="P299" t="inlineStr">
         <is>
-          <t>{'CHILDSEAT', 'VPICDECODE', 'DISTRACT'}</t>
+          <t>{'DISTRACT', 'CHILDSEAT', 'VPICDECODE'}</t>
         </is>
       </c>
       <c r="Q299" t="inlineStr">
@@ -24370,7 +24370,7 @@
       </c>
       <c r="S299" t="inlineStr">
         <is>
-          <t>{'VPICDECODE.Make', 'DISTRACT.VEHNO', 'CHILDSEAT.CASEID', 'CHILDSEAT.VEHNO', 'VPICDECODE.Model', 'DISTRACT.CASEID', 'DISTRACT.DISTRACTN', 'VPICDECODE.CASEID', 'VPICDECODE.VEHNO'}</t>
+          <t>{'VPICDECODE.VEHNO', 'DISTRACT.CASEID', 'VPICDECODE.CASEID', 'VPICDECODE.Model', 'CHILDSEAT.CASEID', 'CHILDSEAT.VEHNO', 'DISTRACT.VEHNO', 'VPICDECODE.Make', 'DISTRACT.DISTRACTN'}</t>
         </is>
       </c>
       <c r="T299" t="inlineStr">
@@ -24435,7 +24435,7 @@
       </c>
       <c r="P300" t="inlineStr">
         <is>
-          <t>{'VPICDECODE', 'DISTRACT'}</t>
+          <t>{'DISTRACT', 'VPICDECODE'}</t>
         </is>
       </c>
       <c r="Q300" t="inlineStr">
@@ -24450,7 +24450,7 @@
       </c>
       <c r="S300" t="inlineStr">
         <is>
-          <t>{'VPICDECODE.Make', 'VPICDECODE.VEHNO', 'DISTRACT.CASEID', 'DISTRACT.DISTRACTN', 'VPICDECODE.CASEID', 'DISTRACT.VEHNO'}</t>
+          <t>{'VPICDECODE.CASEID', 'DISTRACT.VEHNO', 'VPICDECODE.VEHNO', 'DISTRACT.CASEID', 'VPICDECODE.Make', 'DISTRACT.DISTRACTN'}</t>
         </is>
       </c>
       <c r="T300" t="inlineStr">
@@ -24530,7 +24530,7 @@
       </c>
       <c r="S301" t="inlineStr">
         <is>
-          <t>{'FIRE.FIRE', 'VPICDECODE.Make', 'FIRE.VEHNO', 'VPICDECODE.CASEID', 'VPICDECODE.VEHNO', 'FIRE.CASEID'}</t>
+          <t>{'VPICDECODE.CASEID', 'VPICDECODE.VEHNO', 'FIRE.CASEID', 'FIRE.VEHNO', 'VPICDECODE.Make', 'FIRE.FIRE'}</t>
         </is>
       </c>
       <c r="T301" t="inlineStr">
@@ -24610,7 +24610,7 @@
       </c>
       <c r="S302" t="inlineStr">
         <is>
-          <t>{'Accountability_Levels.INSTITUTION_ID', 'Accountability_Levels.LEVEL', 'Accountability_Levels.INDICATOR', 'Accountability_Levels.SUBGROUP_NAME', 'Accountability_Levels.ENTITY_NAME'}</t>
+          <t>{'Accountability_Levels.ENTITY_NAME', 'Accountability_Levels.INDICATOR', 'Accountability_Levels.SUBGROUP_NAME', 'Accountability_Levels.LEVEL', 'Accountability_Levels.INSTITUTION_ID'}</t>
         </is>
       </c>
       <c r="T302" t="inlineStr">
@@ -24690,7 +24690,7 @@
       </c>
       <c r="S303" t="inlineStr">
         <is>
-          <t>{'Annual_EM_ELA.ENTITY_NAME', 'Annual_EM_ELA.YEAR', 'Annual_EM_ELA.PCT_NOT_TESTED', 'Annual_EM_ELA.ASSESSMENT_NAME', 'Annual_EM_ELA.SUBGROUP_NAME'}</t>
+          <t>{'Annual_EM_ELA.PCT_NOT_TESTED', 'Annual_EM_ELA.ENTITY_NAME', 'Annual_EM_ELA.ASSESSMENT_NAME', 'Annual_EM_ELA.SUBGROUP_NAME', 'Annual_EM_ELA.YEAR'}</t>
         </is>
       </c>
       <c r="T303" t="inlineStr">
@@ -24850,7 +24850,7 @@
       </c>
       <c r="S305" t="inlineStr">
         <is>
-          <t>{'Expenditures_per_Pupil.YEAR', 'Expenditures_per_Pupil.FEDERAL_EXP', 'Expenditures_per_Pupil.PUPIL_COUNT_TOT', 'Expenditures_per_Pupil.PER_FEDERAL_EXP', 'Expenditures_per_Pupil.ENTITY_NAME'}</t>
+          <t>{'Expenditures_per_Pupil.ENTITY_NAME', 'Expenditures_per_Pupil.PER_FEDERAL_EXP', 'Expenditures_per_Pupil.PUPIL_COUNT_TOT', 'Expenditures_per_Pupil.YEAR', 'Expenditures_per_Pupil.FEDERAL_EXP'}</t>
         </is>
       </c>
       <c r="T305" t="inlineStr">
@@ -24915,7 +24915,7 @@
       </c>
       <c r="P306" t="inlineStr">
         <is>
-          <t>{'Annual_EM_MATH', 'Expenditures_per_Pupil'}</t>
+          <t>{'Expenditures_per_Pupil', 'Annual_EM_MATH'}</t>
         </is>
       </c>
       <c r="Q306" t="inlineStr">
@@ -24930,7 +24930,7 @@
       </c>
       <c r="S306" t="inlineStr">
         <is>
-          <t>{'Annual_EM_MATH.YEAR', 'Expenditures_per_Pupil.YEAR', 'Annual_EM_MATH.ENTITY_NAME', 'Expenditures_per_Pupil.PUPIL_COUNT_TOT', 'Expenditures_per_Pupil.ENTITY_CD', 'Expenditures_per_Pupil.ENTITY_NAME', 'Annual_EM_MATH.SUBGROUP_NAME', 'Annual_EM_MATH.ENTITY_CD', 'Expenditures_per_Pupil.FEDERAL_EXP', 'Annual_EM_MATH.ASSESSMENT_NAME', 'Expenditures_per_Pupil.PER_FEDERAL_EXP', 'Annual_EM_MATH.MEAN_SCORE'}</t>
+          <t>{'Expenditures_per_Pupil.ENTITY_NAME', 'Expenditures_per_Pupil.PER_FEDERAL_EXP', 'Annual_EM_MATH.ENTITY_NAME', 'Annual_EM_MATH.ASSESSMENT_NAME', 'Expenditures_per_Pupil.ENTITY_CD', 'Annual_EM_MATH.YEAR', 'Annual_EM_MATH.ENTITY_CD', 'Expenditures_per_Pupil.PUPIL_COUNT_TOT', 'Expenditures_per_Pupil.YEAR', 'Expenditures_per_Pupil.FEDERAL_EXP', 'Annual_EM_MATH.MEAN_SCORE', 'Annual_EM_MATH.SUBGROUP_NAME'}</t>
         </is>
       </c>
       <c r="T306" t="inlineStr">
@@ -25010,7 +25010,7 @@
       </c>
       <c r="S307" t="inlineStr">
         <is>
-          <t>{'ACC_HS_Participation_Rate.INSTITUTION_ID', 'ACC_HS_Graduation_Rate.SUBGROUP_NAME', 'ACC_HS_Participation_Rate.ENTITY_NAME', 'ACC_HS_Graduation_Rate.ENTITY_NAME', 'ACC_HS_Participation_Rate.RATE', 'ACC_HS_Graduation_Rate.YEAR', 'ACC_HS_Participation_Rate.ENTITY_CD', 'ACC_HS_Participation_Rate.YEAR', 'ACC_HS_Participation_Rate.SUBGROUP_NAME', 'ACC_HS_Graduation_Rate.GRAD_RATE', 'ACC_HS_Graduation_Rate.ENTITY_CD', 'ACC_HS_Graduation_Rate.INSTITUTION_ID'}</t>
+          <t>{'ACC_HS_Graduation_Rate.YEAR', 'ACC_HS_Graduation_Rate.GRAD_RATE', 'ACC_HS_Participation_Rate.SUBGROUP_NAME', 'ACC_HS_Graduation_Rate.INSTITUTION_ID', 'ACC_HS_Graduation_Rate.ENTITY_CD', 'ACC_HS_Graduation_Rate.SUBGROUP_NAME', 'ACC_HS_Participation_Rate.RATE', 'ACC_HS_Participation_Rate.INSTITUTION_ID', 'ACC_HS_Graduation_Rate.ENTITY_NAME', 'ACC_HS_Participation_Rate.ENTITY_NAME', 'ACC_HS_Participation_Rate.YEAR', 'ACC_HS_Participation_Rate.ENTITY_CD'}</t>
         </is>
       </c>
       <c r="T307" t="inlineStr">
@@ -25090,7 +25090,7 @@
       </c>
       <c r="S308" t="inlineStr">
         <is>
-          <t>{'ACC_EM_Chronic_Absenteeism.ABSENT_COUNT', 'ACC_EM_Chronic_Absenteeism.ENROLLMENT', 'ACC_EM_Chronic_Absenteeism.SUBGROUP_NAME', 'ACC_EM_Chronic_Absenteeism.ENTITY_NAME', 'ACC_EM_Chronic_Absenteeism.YEAR', 'ACC_EM_Chronic_Absenteeism.ABSENT_RATE'}</t>
+          <t>{'ACC_EM_Chronic_Absenteeism.ENTITY_NAME', 'ACC_EM_Chronic_Absenteeism.ENROLLMENT', 'ACC_EM_Chronic_Absenteeism.ABSENT_COUNT', 'ACC_EM_Chronic_Absenteeism.YEAR', 'ACC_EM_Chronic_Absenteeism.SUBGROUP_NAME', 'ACC_EM_Chronic_Absenteeism.ABSENT_RATE'}</t>
         </is>
       </c>
       <c r="T308" t="inlineStr">
@@ -25170,7 +25170,7 @@
       </c>
       <c r="S309" t="inlineStr">
         <is>
-          <t>{'Annual_Regents_Exams.PER_LEVEL4', 'Annual_Regents_Exams.PER_LEVEL5', 'Annual_Regents_Exams.ENTITY_NAME', 'Annual_Regents_Exams.PER_LEVEL2', 'Annual_Regents_Exams.SUBGROUP_NAME', 'Annual_Regents_Exams.SUBJECT', 'Annual_Regents_Exams.PER_LEVEL3', 'Annual_Regents_Exams.PER_LEVEL1', 'Annual_Regents_Exams.TESTED', 'Annual_Regents_Exams.YEAR'}</t>
+          <t>{'Annual_Regents_Exams.PER_LEVEL2', 'Annual_Regents_Exams.SUBJECT', 'Annual_Regents_Exams.YEAR', 'Annual_Regents_Exams.PER_LEVEL4', 'Annual_Regents_Exams.PER_LEVEL5', 'Annual_Regents_Exams.PER_LEVEL3', 'Annual_Regents_Exams.TESTED', 'Annual_Regents_Exams.PER_LEVEL1', 'Annual_Regents_Exams.SUBGROUP_NAME', 'Annual_Regents_Exams.ENTITY_NAME'}</t>
         </is>
       </c>
       <c r="T309" t="inlineStr">
@@ -25250,7 +25250,7 @@
       </c>
       <c r="S310" t="inlineStr">
         <is>
-          <t>{'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'Accountability_Status.OVERALL_STATUS', 'Accountability_Status.ENTITY_CD', 'Accountability_Status.YEAR'}</t>
+          <t>{'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'Accountability_Status.ENTITY_CD', 'Accountability_Status.OVERALL_STATUS', 'Accountability_Status.YEAR'}</t>
         </is>
       </c>
       <c r="T310" t="inlineStr">
@@ -25330,7 +25330,7 @@
       </c>
       <c r="S311" t="inlineStr">
         <is>
-          <t>{'Accountability_Status.OVERALL_STATUS', 'Accountability_Status.MADE_PROGRESS', 'Accountability_Status.ENTITY_NAME', 'Accountability_Status.YEAR'}</t>
+          <t>{'Accountability_Status.ENTITY_NAME', 'Accountability_Status.OVERALL_STATUS', 'Accountability_Status.MADE_PROGRESS', 'Accountability_Status.YEAR'}</t>
         </is>
       </c>
       <c r="T311" t="inlineStr">
@@ -25410,7 +25410,7 @@
       </c>
       <c r="S312" t="inlineStr">
         <is>
-          <t>{'ACC_EM_Core_and_Weighted_Performance.WEIGHTED_COHORT', 'ACC_EM_Core_and_Weighted_Performance.SUBGROUP_NAME', 'ACC_EM_Core_and_Weighted_Performance.ENTITY_NAME', 'ACC_EM_Core_and_Weighted_Performance.SUBJECT', 'ACC_EM_Core_and_Weighted_Performance.CORE_COHORT'}</t>
+          <t>{'ACC_EM_Core_and_Weighted_Performance.ENTITY_NAME', 'ACC_EM_Core_and_Weighted_Performance.SUBGROUP_NAME', 'ACC_EM_Core_and_Weighted_Performance.CORE_COHORT', 'ACC_EM_Core_and_Weighted_Performance.SUBJECT', 'ACC_EM_Core_and_Weighted_Performance.WEIGHTED_COHORT'}</t>
         </is>
       </c>
       <c r="T312" t="inlineStr">
@@ -25490,7 +25490,7 @@
       </c>
       <c r="S313" t="inlineStr">
         <is>
-          <t>{'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_NAME', 'ACC_EM_Core_and_Weighted_Performance.SUBGROUP_NAME', 'ACC_EM_Core_and_Weighted_Performance.ENTITY_NAME', 'ACC_EM_Core_and_Weighted_Performance.ENTITY_CD'}</t>
+          <t>{'ACC_EM_Core_and_Weighted_Performance.ENTITY_NAME', 'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'ACC_EM_Core_and_Weighted_Performance.ENTITY_CD', 'Institution_Grouping.ENTITY_NAME', 'ACC_EM_Core_and_Weighted_Performance.SUBGROUP_NAME'}</t>
         </is>
       </c>
       <c r="T313" t="inlineStr">
@@ -25570,7 +25570,7 @@
       </c>
       <c r="S314" t="inlineStr">
         <is>
-          <t>{'Institution_Grouping.ENTITY_CD', 'ACC_EM_Core_and_Weighted_Performance.SUBGROUP_NAME', 'Institution_Grouping.GROUP_NAME', 'ACC_EM_Core_and_Weighted_Performance.ENTITY_CD'}</t>
+          <t>{'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'ACC_EM_Core_and_Weighted_Performance.ENTITY_CD', 'ACC_EM_Core_and_Weighted_Performance.SUBGROUP_NAME'}</t>
         </is>
       </c>
       <c r="T314" t="inlineStr">
@@ -25650,7 +25650,7 @@
       </c>
       <c r="S315" t="inlineStr">
         <is>
-          <t>{'ACC_EM_ELP.ENTITY_NAME', 'ACC_EM_ELP.SUBGROUP_NAME', 'ACC_EM_ELP.ELL_COUNT'}</t>
+          <t>{'ACC_EM_ELP.ELL_COUNT', 'ACC_EM_ELP.ENTITY_NAME', 'ACC_EM_ELP.SUBGROUP_NAME'}</t>
         </is>
       </c>
       <c r="T315" t="inlineStr">
@@ -25730,7 +25730,7 @@
       </c>
       <c r="S316" t="inlineStr">
         <is>
-          <t>{'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'ACC_EM_ELP.ELL_COUNT', 'ACC_EM_ELP.ENTITY_CD', 'ACC_EM_ELP.SUBGROUP_NAME'}</t>
+          <t>{'ACC_EM_ELP.SUBGROUP_NAME', 'Institution_Grouping.GROUP_NAME', 'ACC_EM_ELP.ELL_COUNT', 'Institution_Grouping.ENTITY_CD', 'ACC_EM_ELP.ENTITY_CD'}</t>
         </is>
       </c>
       <c r="T316" t="inlineStr">
@@ -25810,7 +25810,7 @@
       </c>
       <c r="S317" t="inlineStr">
         <is>
-          <t>{'ACC_EM_ELP.SUCCESS_RATIO', 'ACC_EM_ELP.ELL_COUNT', 'ACC_EM_ELP.ENTITY_NAME', 'ACC_EM_ELP.BENCHMARK', 'ACC_EM_ELP.SUBGROUP_NAME', 'ACC_EM_ELP.PROGRESS_RATE'}</t>
+          <t>{'ACC_EM_ELP.SUBGROUP_NAME', 'ACC_EM_ELP.ELL_COUNT', 'ACC_EM_ELP.BENCHMARK', 'ACC_EM_ELP.PROGRESS_RATE', 'ACC_EM_ELP.SUCCESS_RATIO', 'ACC_EM_ELP.ENTITY_NAME'}</t>
         </is>
       </c>
       <c r="T317" t="inlineStr">
@@ -25875,7 +25875,7 @@
       </c>
       <c r="P318" t="inlineStr">
         <is>
-          <t>{'ACC_EM_NYSESLAT_for_Participation', 'Institution_Grouping'}</t>
+          <t>{'Institution_Grouping', 'ACC_EM_NYSESLAT_for_Participation'}</t>
         </is>
       </c>
       <c r="Q318" t="inlineStr">
@@ -25890,7 +25890,7 @@
       </c>
       <c r="S318" t="inlineStr">
         <is>
-          <t>{'ACC_EM_NYSESLAT_for_Participation.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'ACC_EM_NYSESLAT_for_Participation.NYSESLAT_PART', 'Institution_Grouping.ENTITY_CD'}</t>
+          <t>{'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'ACC_EM_NYSESLAT_for_Participation.ENTITY_CD', 'ACC_EM_NYSESLAT_for_Participation.NYSESLAT_PART'}</t>
         </is>
       </c>
       <c r="T318" t="inlineStr">
@@ -26035,7 +26035,7 @@
       </c>
       <c r="P320" t="inlineStr">
         <is>
-          <t>{'ACC_EM_NYSESLAT_for_Participation', 'ACC_EM_ELP', 'Institution_Grouping'}</t>
+          <t>{'ACC_EM_ELP', 'Institution_Grouping', 'ACC_EM_NYSESLAT_for_Participation'}</t>
         </is>
       </c>
       <c r="Q320" t="inlineStr">
@@ -26050,7 +26050,7 @@
       </c>
       <c r="S320" t="inlineStr">
         <is>
-          <t>{'ACC_EM_NYSESLAT_for_Participation.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.ENTITY_NAME', 'ACC_EM_ELP.ENTITY_NAME', 'ACC_EM_ELP.SUBGROUP_NAME', 'ACC_EM_NYSESLAT_for_Participation.NYSESLAT_PART', 'ACC_EM_NYSESLAT_for_Participation.ENTITY_NAME', 'ACC_EM_ELP.ELL_COUNT', 'ACC_EM_ELP.ENTITY_CD', 'ACC_EM_ELP.LEVEL'}</t>
+          <t>{'ACC_EM_NYSESLAT_for_Participation.ENTITY_CD', 'ACC_EM_NYSESLAT_for_Participation.ENTITY_NAME', 'ACC_EM_ELP.SUBGROUP_NAME', 'Institution_Grouping.GROUP_NAME', 'ACC_EM_ELP.ENTITY_CD', 'Institution_Grouping.ENTITY_CD', 'ACC_EM_ELP.LEVEL', 'ACC_EM_NYSESLAT_for_Participation.NYSESLAT_PART', 'ACC_EM_ELP.ELL_COUNT', 'Institution_Grouping.ENTITY_NAME', 'ACC_EM_ELP.ENTITY_NAME'}</t>
         </is>
       </c>
       <c r="T320" t="inlineStr">
@@ -26130,7 +26130,7 @@
       </c>
       <c r="S321" t="inlineStr">
         <is>
-          <t>{'ACC_EM_Participation_Rate.SUBGROUP_NAME', 'ACC_EM_Participation_Rate.ENTITY_NAME', 'ACC_EM_Participation_Rate.SUBJECT', 'ACC_EM_Participation_Rate.YEAR', 'ACC_EM_Participation_Rate.RATE', 'ACC_EM_Participation_Rate.COHORT'}</t>
+          <t>{'ACC_EM_Participation_Rate.RATE', 'ACC_EM_Participation_Rate.COHORT', 'ACC_EM_Participation_Rate.SUBGROUP_NAME', 'ACC_EM_Participation_Rate.YEAR', 'ACC_EM_Participation_Rate.SUBJECT', 'ACC_EM_Participation_Rate.ENTITY_NAME'}</t>
         </is>
       </c>
       <c r="T321" t="inlineStr">
@@ -26210,7 +26210,7 @@
       </c>
       <c r="S322" t="inlineStr">
         <is>
-          <t>{'ACC_EM_Participation_Rate.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'ACC_EM_Participation_Rate.MET_95_PERCENT'}</t>
+          <t>{'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'ACC_EM_Participation_Rate.ENTITY_CD', 'ACC_EM_Participation_Rate.MET_95_PERCENT'}</t>
         </is>
       </c>
       <c r="T322" t="inlineStr">
@@ -26290,7 +26290,7 @@
       </c>
       <c r="S323" t="inlineStr">
         <is>
-          <t>{'ACC_EM_Participation_Rate.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'ACC_EM_Participation_Rate.RATE', 'Institution_Grouping.ENTITY_CD'}</t>
+          <t>{'Institution_Grouping.GROUP_NAME', 'ACC_EM_Participation_Rate.RATE', 'ACC_EM_Participation_Rate.ENTITY_CD', 'Institution_Grouping.ENTITY_CD'}</t>
         </is>
       </c>
       <c r="T323" t="inlineStr">
@@ -26355,7 +26355,7 @@
       </c>
       <c r="P324" t="inlineStr">
         <is>
-          <t>{'ACC_EM_Chronic_Absenteeism', 'Institution_Grouping'}</t>
+          <t>{'Institution_Grouping', 'ACC_EM_Chronic_Absenteeism'}</t>
         </is>
       </c>
       <c r="Q324" t="inlineStr">
@@ -26370,7 +26370,7 @@
       </c>
       <c r="S324" t="inlineStr">
         <is>
-          <t>{'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'ACC_EM_Chronic_Absenteeism.ENTITY_CD', 'ACC_EM_Chronic_Absenteeism.SUBJECT', 'ACC_EM_Chronic_Absenteeism.ABSENT_RATE'}</t>
+          <t>{'ACC_EM_Chronic_Absenteeism.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'ACC_EM_Chronic_Absenteeism.SUBJECT', 'ACC_EM_Chronic_Absenteeism.ABSENT_RATE'}</t>
         </is>
       </c>
       <c r="T324" t="inlineStr">
@@ -26435,7 +26435,7 @@
       </c>
       <c r="P325" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'ACC_EM_Chronic_Absenteeism'}</t>
         </is>
       </c>
       <c r="Q325" t="inlineStr">
@@ -26450,7 +26450,7 @@
       </c>
       <c r="S325" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'ACC_EM_Chronic_Absenteeism.ENTITY_NAME', 'ACC_EM_Chronic_Absenteeism.SUBGROUP_NAME', 'ACC_EM_Chronic_Absenteeism.ABSENT_RATE'}</t>
         </is>
       </c>
       <c r="T325" t="inlineStr">
@@ -26515,7 +26515,7 @@
       </c>
       <c r="P326" t="inlineStr">
         <is>
-          <t>{'ACC_EM_Chronic_Absenteeism', 'Institution_Grouping'}</t>
+          <t>{'Institution_Grouping', 'ACC_EM_Chronic_Absenteeism'}</t>
         </is>
       </c>
       <c r="Q326" t="inlineStr">
@@ -26530,7 +26530,7 @@
       </c>
       <c r="S326" t="inlineStr">
         <is>
-          <t>{'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'ACC_EM_Chronic_Absenteeism.ENTITY_CD', 'Institution_Grouping.ENTITY_NAME', 'ACC_EM_Chronic_Absenteeism.ENROLLMENT', 'ACC_EM_Chronic_Absenteeism.SUBGROUP_NAME', 'ACC_EM_Chronic_Absenteeism.ENTITY_NAME', 'ACC_EM_Chronic_Absenteeism.ABSENT_RATE', 'ACC_EM_Chronic_Absenteeism.YEAR'}</t>
+          <t>{'ACC_EM_Chronic_Absenteeism.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'ACC_EM_Chronic_Absenteeism.SUBGROUP_NAME', 'ACC_EM_Chronic_Absenteeism.YEAR', 'ACC_EM_Chronic_Absenteeism.ENROLLMENT', 'ACC_EM_Chronic_Absenteeism.ENTITY_NAME', 'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.ENTITY_NAME', 'ACC_EM_Chronic_Absenteeism.ABSENT_RATE'}</t>
         </is>
       </c>
       <c r="T326" t="inlineStr">
@@ -26610,7 +26610,7 @@
       </c>
       <c r="S327" t="inlineStr">
         <is>
-          <t>{'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'ACC_HS_Chronic_Absenteeism.ABSENT_RATE', 'ACC_HS_Chronic_Absenteeism.ENTITY_CD', 'ACC_HS_Chronic_Absenteeism.SUBGROUP_NAME'}</t>
+          <t>{'ACC_HS_Chronic_Absenteeism.ABSENT_RATE', 'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'ACC_HS_Chronic_Absenteeism.ENTITY_CD', 'ACC_HS_Chronic_Absenteeism.SUBGROUP_NAME'}</t>
         </is>
       </c>
       <c r="T327" t="inlineStr">
@@ -26675,7 +26675,7 @@
       </c>
       <c r="P328" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Institution_Grouping', 'ACC_HS_Chronic_Absenteeism'}</t>
         </is>
       </c>
       <c r="Q328" t="inlineStr">
@@ -26690,7 +26690,7 @@
       </c>
       <c r="S328" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'ACC_HS_Chronic_Absenteeism.YEAR', 'Institution_Grouping.GROUP_NAME', 'ACC_HS_Chronic_Absenteeism.ENROLLMENT', 'ACC_HS_Chronic_Absenteeism.ABSENT_COUNT', 'ACC_HS_Chronic_Absenteeism.ENTITY_NAME', 'ACC_HS_Chronic_Absenteeism.ABSENT_RATE', 'Institution_Grouping.ENTITY_CD', 'ACC_HS_Chronic_Absenteeism.ENTITY_CD', 'Institution_Grouping.ENTITY_NAME', 'ACC_HS_Chronic_Absenteeism.SUBGROUP_NAME'}</t>
         </is>
       </c>
       <c r="T328" t="inlineStr">
@@ -26770,7 +26770,7 @@
       </c>
       <c r="S329" t="inlineStr">
         <is>
-          <t>{'ACC_HS_Core_and_Weighted_Performance.SUBGROUP_NAME', 'ACC_HS_Core_and_Weighted_Performance.WEIGHTED_COHORT', 'ACC_HS_Core_and_Weighted_Performance.CORE_INDEX', 'ACC_HS_Core_and_Weighted_Performance.WEIGHTED_INDEX', 'ACC_HS_Core_and_Weighted_Performance.CORE_COHORT', 'ACC_HS_Core_and_Weighted_Performance.ENTITY_NAME', 'ACC_HS_Core_and_Weighted_Performance.YEAR', 'ACC_HS_Core_and_Weighted_Performance.SUBJECT'}</t>
+          <t>{'ACC_HS_Core_and_Weighted_Performance.WEIGHTED_COHORT', 'ACC_HS_Core_and_Weighted_Performance.YEAR', 'ACC_HS_Core_and_Weighted_Performance.CORE_COHORT', 'ACC_HS_Core_and_Weighted_Performance.CORE_INDEX', 'ACC_HS_Core_and_Weighted_Performance.ENTITY_NAME', 'ACC_HS_Core_and_Weighted_Performance.SUBGROUP_NAME', 'ACC_HS_Core_and_Weighted_Performance.WEIGHTED_INDEX', 'ACC_HS_Core_and_Weighted_Performance.SUBJECT'}</t>
         </is>
       </c>
       <c r="T329" t="inlineStr">
@@ -26835,7 +26835,7 @@
       </c>
       <c r="P330" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Institution_Grouping', 'ACC_HS_Core_and_Weighted_Performance'}</t>
         </is>
       </c>
       <c r="Q330" t="inlineStr">
@@ -26850,7 +26850,7 @@
       </c>
       <c r="S330" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'ACC_HS_Core_and_Weighted_Performance.YEAR', 'Institution_Grouping.GROUP_NAME', 'ACC_HS_Core_and_Weighted_Performance.ENTITY_NAME', 'ACC_HS_Core_and_Weighted_Performance.SUBGROUP_NAME', 'ACC_HS_Core_and_Weighted_Performance.ENTITY_CD', 'ACC_HS_Core_and_Weighted_Performance.WEIGHTED_INDEX', 'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.ENTITY_NAME', 'ACC_HS_Core_and_Weighted_Performance.SUBJECT'}</t>
         </is>
       </c>
       <c r="T330" t="inlineStr">
@@ -26915,7 +26915,7 @@
       </c>
       <c r="P331" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Institution_Grouping', 'ACC_HS_Core_and_Weighted_Performance'}</t>
         </is>
       </c>
       <c r="Q331" t="inlineStr">
@@ -26930,7 +26930,7 @@
       </c>
       <c r="S331" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'ACC_HS_Core_and_Weighted_Performance.ENTITY_CD', 'ACC_HS_Core_and_Weighted_Performance.WEIGHTED_INDEX', 'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'ACC_HS_Core_and_Weighted_Performance.ENTITY_NAME', 'Institution_Grouping.ENTITY_NAME', 'ACC_HS_Core_and_Weighted_Performance.SUBJECT'}</t>
         </is>
       </c>
       <c r="T331" t="inlineStr">
@@ -27010,7 +27010,7 @@
       </c>
       <c r="S332" t="inlineStr">
         <is>
-          <t>{'ACC_HS_ELP.LEVEL', 'ACC_HS_ELP.PROGRESS_RATE', 'ACC_HS_ELP.SUCCESS_RATIO', 'ACC_HS_ELP.SUBGROUP_NAME', 'ACC_HS_ELP.ENTITY_NAME', 'ACC_HS_ELP.BENCHMARK', 'ACC_HS_ELP.ELL_COUNT', 'ACC_HS_ELP.YEAR'}</t>
+          <t>{'ACC_HS_ELP.BENCHMARK', 'ACC_HS_ELP.SUCCESS_RATIO', 'ACC_HS_ELP.SUBGROUP_NAME', 'ACC_HS_ELP.ENTITY_NAME', 'ACC_HS_ELP.LEVEL', 'ACC_HS_ELP.ELL_COUNT', 'ACC_HS_ELP.PROGRESS_RATE', 'ACC_HS_ELP.YEAR'}</t>
         </is>
       </c>
       <c r="T332" t="inlineStr">
@@ -27090,7 +27090,7 @@
       </c>
       <c r="S333" t="inlineStr">
         <is>
-          <t>{'ACC_HS_ELP.SUBGROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'ACC_HS_ELP.ELL_COUNT', 'ACC_HS_ELP.ENTITY_CD'}</t>
+          <t>{'ACC_HS_ELP.ENTITY_CD', 'ACC_HS_ELP.SUBGROUP_NAME', 'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'ACC_HS_ELP.ELL_COUNT'}</t>
         </is>
       </c>
       <c r="T333" t="inlineStr">
@@ -27155,7 +27155,7 @@
       </c>
       <c r="P334" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'ACC_HS_ELP', 'Institution_Grouping', 'Expenditures_per_Pupil'}</t>
         </is>
       </c>
       <c r="Q334" t="inlineStr">
@@ -27170,7 +27170,7 @@
       </c>
       <c r="S334" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Expenditures_per_Pupil.ENTITY_NAME', 'Expenditures_per_Pupil.PER_FED_STATE_LOCAL_EXP', 'Institution_Grouping.GROUP_NAME', 'Expenditures_per_Pupil.ENTITY_CD', 'ACC_HS_ELP.ENTITY_CD', 'ACC_HS_ELP.SUBGROUP_NAME', 'Expenditures_per_Pupil.YEAR', 'ACC_HS_ELP.ENTITY_NAME', 'Institution_Grouping.ENTITY_CD', 'ACC_HS_ELP.ELL_COUNT', 'Institution_Grouping.ENTITY_NAME', 'ACC_HS_ELP.YEAR'}</t>
         </is>
       </c>
       <c r="T334" t="inlineStr">
@@ -27250,7 +27250,7 @@
       </c>
       <c r="S335" t="inlineStr">
         <is>
-          <t>{'Accountability_Status_by_Subgroup.OVERALL_STATUS', 'Accountability_Status_by_Subgroup.YEAR', 'Accountability_Status_by_Subgroup.SUBGROUP_NAME'}</t>
+          <t>{'Accountability_Status_by_Subgroup.OVERALL_STATUS', 'Accountability_Status_by_Subgroup.SUBGROUP_NAME', 'Accountability_Status_by_Subgroup.YEAR'}</t>
         </is>
       </c>
       <c r="T335" t="inlineStr">
@@ -27330,7 +27330,7 @@
       </c>
       <c r="S336" t="inlineStr">
         <is>
-          <t>{'Accountability_Status_by_Subgroup.YEAR', 'Accountability_Status_by_Subgroup.SCHOOL_TYPE', 'Accountability_Status_by_Subgroup.SUBGROUP_NAME'}</t>
+          <t>{'Accountability_Status_by_Subgroup.SCHOOL_TYPE', 'Accountability_Status_by_Subgroup.SUBGROUP_NAME', 'Accountability_Status_by_Subgroup.YEAR'}</t>
         </is>
       </c>
       <c r="T336" t="inlineStr">
@@ -27410,7 +27410,7 @@
       </c>
       <c r="S337" t="inlineStr">
         <is>
-          <t>{'Accountability_Status_by_Subgroup.YEAR', 'Accountability_Status_by_Subgroup.SCHOOL_TYPE', 'Accountability_Status_by_Subgroup.ENTITY_NAME', 'Accountability_Status_by_Subgroup.OVERALL_STATUS', 'Accountability_Status_by_Subgroup.SUBGROUP_NAME'}</t>
+          <t>{'Accountability_Status_by_Subgroup.OVERALL_STATUS', 'Accountability_Status_by_Subgroup.SCHOOL_TYPE', 'Accountability_Status_by_Subgroup.SUBGROUP_NAME', 'Accountability_Status_by_Subgroup.ENTITY_NAME', 'Accountability_Status_by_Subgroup.YEAR'}</t>
         </is>
       </c>
       <c r="T337" t="inlineStr">
@@ -27475,7 +27475,7 @@
       </c>
       <c r="P338" t="inlineStr">
         <is>
-          <t>{'Annual_EM_SCIENCE', 'Institution_Grouping'}</t>
+          <t>{'Institution_Grouping', 'Annual_EM_SCIENCE'}</t>
         </is>
       </c>
       <c r="Q338" t="inlineStr">
@@ -27490,7 +27490,7 @@
       </c>
       <c r="S338" t="inlineStr">
         <is>
-          <t>{'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'Annual_EM_SCIENCE.LEVEL1_%TESTED', 'Annual_EM_SCIENCE.ENTITY_CD', 'Annual_EM_SCIENCE.LEVEL2_%TESTED', 'Annual_EM_SCIENCE.LEVEL4_%TESTED', 'Annual_EM_SCIENCE.ASSESSMENT_NAME', 'Annual_EM_SCIENCE.LEVEL3_%TESTED'}</t>
+          <t>{'Annual_EM_SCIENCE.LEVEL2_%TESTED', 'Annual_EM_SCIENCE.ASSESSMENT_NAME', 'Annual_EM_SCIENCE.LEVEL4_%TESTED', 'Institution_Grouping.GROUP_NAME', 'Annual_EM_SCIENCE.LEVEL1_%TESTED', 'Institution_Grouping.ENTITY_CD', 'Annual_EM_SCIENCE.LEVEL3_%TESTED', 'Annual_EM_SCIENCE.ENTITY_CD'}</t>
         </is>
       </c>
       <c r="T338" t="inlineStr">
@@ -27555,7 +27555,7 @@
       </c>
       <c r="P339" t="inlineStr">
         <is>
-          <t>{'Annual_EM_SCIENCE', 'Institution_Grouping'}</t>
+          <t>{'Institution_Grouping', 'Annual_EM_SCIENCE'}</t>
         </is>
       </c>
       <c r="Q339" t="inlineStr">
@@ -27570,7 +27570,7 @@
       </c>
       <c r="S339" t="inlineStr">
         <is>
-          <t>{'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'Annual_EM_SCIENCE.LEVEL1_%TESTED', 'Annual_EM_SCIENCE.ENTITY_CD', 'Annual_EM_SCIENCE.LEVEL2_%TESTED', 'Annual_EM_SCIENCE.LEVEL4_%TESTED', 'Annual_EM_SCIENCE.ASSESSMENT_NAME', 'Annual_EM_SCIENCE.LEVEL3_%TESTED', 'Annual_EM_SCIENCE.SUBGROUP_NAME'}</t>
+          <t>{'Annual_EM_SCIENCE.LEVEL2_%TESTED', 'Annual_EM_SCIENCE.ASSESSMENT_NAME', 'Annual_EM_SCIENCE.LEVEL4_%TESTED', 'Institution_Grouping.GROUP_NAME', 'Annual_EM_SCIENCE.LEVEL1_%TESTED', 'Institution_Grouping.ENTITY_CD', 'Annual_EM_SCIENCE.LEVEL3_%TESTED', 'Annual_EM_SCIENCE.ENTITY_CD', 'Annual_EM_SCIENCE.SUBGROUP_NAME'}</t>
         </is>
       </c>
       <c r="T339" t="inlineStr">
@@ -27730,7 +27730,7 @@
       </c>
       <c r="S341" t="inlineStr">
         <is>
-          <t>{'Annual_NYSESLAT.SUBGROUP_NAME', 'Annual_NYSESLAT.ENTITY_NAME', 'Annual_NYSESLAT.PER_EXP', 'Annual_NYSESLAT.SUBJECT', 'Annual_NYSESLAT.YEAR'}</t>
+          <t>{'Annual_NYSESLAT.SUBJECT', 'Annual_NYSESLAT.ENTITY_NAME', 'Annual_NYSESLAT.SUBGROUP_NAME', 'Annual_NYSESLAT.YEAR', 'Annual_NYSESLAT.PER_EXP'}</t>
         </is>
       </c>
       <c r="T341" t="inlineStr">
@@ -27810,7 +27810,7 @@
       </c>
       <c r="S342" t="inlineStr">
         <is>
-          <t>{'Annual_NYSESLAT.YEAR', 'Annual_NYSESLAT.SUBGROUP_NAME', 'Annual_NYSESLAT.PER_EMER', 'Annual_NYSESLAT.ENTITY_NAME', 'Annual_NYSESLAT.PER_EXP', 'Annual_NYSESLAT.PER_ENT', 'Annual_NYSESLAT.SUBJECT', 'Annual_NYSESLAT.PER_TRAN'}</t>
+          <t>{'Annual_NYSESLAT.ENTITY_NAME', 'Annual_NYSESLAT.PER_EMER', 'Annual_NYSESLAT.PER_ENT', 'Annual_NYSESLAT.SUBJECT', 'Annual_NYSESLAT.PER_TRAN', 'Annual_NYSESLAT.SUBGROUP_NAME', 'Annual_NYSESLAT.YEAR', 'Annual_NYSESLAT.PER_EXP'}</t>
         </is>
       </c>
       <c r="T342" t="inlineStr">
@@ -27875,7 +27875,7 @@
       </c>
       <c r="P343" t="inlineStr">
         <is>
-          <t>{'Annual_NYSESLAT', 'Institution_Grouping'}</t>
+          <t>{'Institution_Grouping', 'Annual_NYSESLAT'}</t>
         </is>
       </c>
       <c r="Q343" t="inlineStr">
@@ -27890,7 +27890,7 @@
       </c>
       <c r="S343" t="inlineStr">
         <is>
-          <t>{'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'Annual_NYSESLAT.ENTITY_CD', 'Annual_NYSESLAT.PER_ENT', 'Annual_NYSESLAT.SUBJECT', 'Annual_NYSESLAT.YEAR'}</t>
+          <t>{'Annual_NYSESLAT.SUBJECT', 'Annual_NYSESLAT.YEAR', 'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'Annual_NYSESLAT.ENTITY_CD', 'Annual_NYSESLAT.PER_ENT'}</t>
         </is>
       </c>
       <c r="T343" t="inlineStr">
@@ -27955,7 +27955,7 @@
       </c>
       <c r="P344" t="inlineStr">
         <is>
-          <t>{'Annual_NYSESLAT', 'Institution_Grouping'}</t>
+          <t>{'Institution_Grouping', 'Annual_NYSESLAT'}</t>
         </is>
       </c>
       <c r="Q344" t="inlineStr">
@@ -27970,7 +27970,7 @@
       </c>
       <c r="S344" t="inlineStr">
         <is>
-          <t>{'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'Annual_NYSESLAT.ENTITY_CD', 'Annual_NYSESLAT.YEAR', 'Annual_NYSESLAT.PER_EMER', 'Annual_NYSESLAT.PER_COM', 'Annual_NYSESLAT.PER_EXP', 'Annual_NYSESLAT.PER_ENT', 'Annual_NYSESLAT.SUBJECT', 'Annual_NYSESLAT.PER_TRAN'}</t>
+          <t>{'Annual_NYSESLAT.PER_EMER', 'Institution_Grouping.GROUP_NAME', 'Annual_NYSESLAT.ENTITY_CD', 'Annual_NYSESLAT.PER_ENT', 'Annual_NYSESLAT.SUBJECT', 'Annual_NYSESLAT.PER_TRAN', 'Annual_NYSESLAT.PER_COM', 'Annual_NYSESLAT.YEAR', 'Institution_Grouping.ENTITY_CD', 'Annual_NYSESLAT.PER_EXP'}</t>
         </is>
       </c>
       <c r="T344" t="inlineStr">
@@ -28050,7 +28050,7 @@
       </c>
       <c r="S345" t="inlineStr">
         <is>
-          <t>{'Annual_NYSESLAT.NUM_EXP', 'Annual_NYSESLAT.YEAR', 'Annual_NYSESLAT.NUM_ENT', 'Annual_NYSESLAT.SUBGROUP_NAME', 'Annual_NYSESLAT.ENTITY_NAME', 'Annual_NYSESLAT.SUBJECT', 'Annual_NYSESLAT.NUM_TRAN', 'Annual_NYSESLAT.NUM_EMER'}</t>
+          <t>{'Annual_NYSESLAT.ENTITY_NAME', 'Annual_NYSESLAT.NUM_EMER', 'Annual_NYSESLAT.SUBJECT', 'Annual_NYSESLAT.NUM_ENT', 'Annual_NYSESLAT.SUBGROUP_NAME', 'Annual_NYSESLAT.YEAR', 'Annual_NYSESLAT.NUM_EXP', 'Annual_NYSESLAT.NUM_TRAN'}</t>
         </is>
       </c>
       <c r="T345" t="inlineStr">
@@ -28130,7 +28130,7 @@
       </c>
       <c r="S346" t="inlineStr">
         <is>
-          <t>{'BOCES_and_N/RC.SCHOOL_NAME', 'BOCES_and_N/RC.YEAR', 'BOCES_and_N/RC.BOCES_NAME'}</t>
+          <t>{'BOCES_and_N/RC.BOCES_NAME', 'BOCES_and_N/RC.SCHOOL_NAME', 'BOCES_and_N/RC.YEAR'}</t>
         </is>
       </c>
       <c r="T346" t="inlineStr">
@@ -28290,7 +28290,7 @@
       </c>
       <c r="S348" t="inlineStr">
         <is>
-          <t>{'BOCES_and_N/RC.BOCES_NAME', 'Expenditures_per_Pupil.YEAR', 'BOCES_and_N/RC.YEAR', 'BOCES_and_N/RC.ENTITY_CD', 'Expenditures_per_Pupil.PER_FEDERAL_EXP', 'Expenditures_per_Pupil.ENTITY_CD', 'Expenditures_per_Pupil.PER_STATE_LOCAL_EXP'}</t>
+          <t>{'BOCES_and_N/RC.BOCES_NAME', 'Expenditures_per_Pupil.PER_FEDERAL_EXP', 'Expenditures_per_Pupil.YEAR', 'BOCES_and_N/RC.YEAR', 'BOCES_and_N/RC.ENTITY_CD', 'Expenditures_per_Pupil.PER_STATE_LOCAL_EXP', 'Expenditures_per_Pupil.ENTITY_CD'}</t>
         </is>
       </c>
       <c r="T348" t="inlineStr">
@@ -28530,7 +28530,7 @@
       </c>
       <c r="S351" t="inlineStr">
         <is>
-          <t>{'Inexperienced_Teachers_and_Principals.PER_TEACH_INEXP', 'Inexperienced_Teachers_and_Principals.YEAR', 'Inexperienced_Teachers_and_Principals.ENTITY_NAME', 'Inexperienced_Teachers_and_Principals.NUM_TEACH_INEXP', 'Inexperienced_Teachers_and_Principals.NUM_TEACH'}</t>
+          <t>{'Inexperienced_Teachers_and_Principals.YEAR', 'Inexperienced_Teachers_and_Principals.NUM_TEACH', 'Inexperienced_Teachers_and_Principals.ENTITY_NAME', 'Inexperienced_Teachers_and_Principals.NUM_TEACH_INEXP', 'Inexperienced_Teachers_and_Principals.PER_TEACH_INEXP'}</t>
         </is>
       </c>
       <c r="T351" t="inlineStr">
@@ -28595,7 +28595,7 @@
       </c>
       <c r="P352" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Institution_Grouping', 'Inexperienced_Teachers_and_Principals'}</t>
         </is>
       </c>
       <c r="Q352" t="inlineStr">
@@ -28610,7 +28610,7 @@
       </c>
       <c r="S352" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Inexperienced_Teachers_and_Principals.ENTITY_CD', 'Inexperienced_Teachers_and_Principals.YEAR', 'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.ENTITY_NAME', 'Inexperienced_Teachers_and_Principals.ENTITY_NAME', 'Inexperienced_Teachers_and_Principals.PER_TEACH_INEXP'}</t>
         </is>
       </c>
       <c r="T352" t="inlineStr">
@@ -28675,7 +28675,7 @@
       </c>
       <c r="P353" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'BOCES_and_N/RC', 'Inexperienced_Teachers_and_Principals'}</t>
         </is>
       </c>
       <c r="Q353" t="inlineStr">
@@ -28690,7 +28690,7 @@
       </c>
       <c r="S353" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Inexperienced_Teachers_and_Principals.ENTITY_CD', 'BOCES_and_N/RC.DISTRICT_NAME', 'BOCES_and_N/RC.ENTITY_CD', 'Inexperienced_Teachers_and_Principals.PER_TEACH_INEXP'}</t>
         </is>
       </c>
       <c r="T353" t="inlineStr">
@@ -28850,7 +28850,7 @@
       </c>
       <c r="S355" t="inlineStr">
         <is>
-          <t>{'Postsecondary_Enrollment.ENTITY_NAME', 'Postsecondary_Enrollment.OUT_4_YR_CNT', 'Postsecondary_Enrollment.SUBGROUP_NAME'}</t>
+          <t>{'Postsecondary_Enrollment.ENTITY_NAME', 'Postsecondary_Enrollment.SUBGROUP_NAME', 'Postsecondary_Enrollment.OUT_4_YR_CNT'}</t>
         </is>
       </c>
       <c r="T355" t="inlineStr">
@@ -28930,7 +28930,7 @@
       </c>
       <c r="S356" t="inlineStr">
         <is>
-          <t>{'Postsecondary_Enrollment.PER_NYS_PUB_2_YR', 'Postsecondary_Enrollment.ENTITY_NAME', 'Postsecondary_Enrollment.PER_NYS_PUB_4_YR', 'Postsecondary_Enrollment.SUBGROUP_NAME', 'Postsecondary_Enrollment.YEAR'}</t>
+          <t>{'Postsecondary_Enrollment.SUBGROUP_NAME', 'Postsecondary_Enrollment.YEAR', 'Postsecondary_Enrollment.PER_NYS_PUB_4_YR', 'Postsecondary_Enrollment.PER_NYS_PUB_2_YR', 'Postsecondary_Enrollment.ENTITY_NAME'}</t>
         </is>
       </c>
       <c r="T356" t="inlineStr">
@@ -28995,7 +28995,7 @@
       </c>
       <c r="P357" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Teachers_Teaching_Out_of_Certification', 'Institution_Grouping'}</t>
         </is>
       </c>
       <c r="Q357" t="inlineStr">
@@ -29010,7 +29010,7 @@
       </c>
       <c r="S357" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Teachers_Teaching_Out_of_Certification.ENTITY_NAME', 'Teachers_Teaching_Out_of_Certification.NUM_OUT_CERT', 'Teachers_Teaching_Out_of_Certification.YEAR', 'Institution_Grouping.GROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.ENTITY_NAME', 'Teachers_Teaching_Out_of_Certification.ENTITY_CD'}</t>
         </is>
       </c>
       <c r="T357" t="inlineStr">
@@ -29090,7 +29090,7 @@
       </c>
       <c r="S358" t="inlineStr">
         <is>
-          <t>{'Teachers_Teaching_Out_of_Certification.PER_OUT_CERT', 'Teachers_Teaching_Out_of_Certification.ENTITY_NAME', 'Teachers_Teaching_Out_of_Certification.NUM_OUT_CERT', 'Teachers_Teaching_Out_of_Certification.YEAR'}</t>
+          <t>{'Teachers_Teaching_Out_of_Certification.ENTITY_NAME', 'Teachers_Teaching_Out_of_Certification.NUM_OUT_CERT', 'Teachers_Teaching_Out_of_Certification.YEAR', 'Teachers_Teaching_Out_of_Certification.PER_OUT_CERT'}</t>
         </is>
       </c>
       <c r="T358" t="inlineStr">
@@ -29155,7 +29155,7 @@
       </c>
       <c r="P359" t="inlineStr">
         <is>
-          <t>{'Teachers_Teaching_Out_of_Certification', 'BOCES_and_N/RC'}</t>
+          <t>{'BOCES_and_N/RC', 'Teachers_Teaching_Out_of_Certification'}</t>
         </is>
       </c>
       <c r="Q359" t="inlineStr">
@@ -29170,7 +29170,7 @@
       </c>
       <c r="S359" t="inlineStr">
         <is>
-          <t>{'BOCES_and_N/RC.COUNTY_NAME', 'Teachers_Teaching_Out_of_Certification.ENTITY_CD', 'Teachers_Teaching_Out_of_Certification.NUM_OUT_CERT', 'BOCES_and_N/RC.ENTITY_CD'}</t>
+          <t>{'Teachers_Teaching_Out_of_Certification.NUM_OUT_CERT', 'BOCES_and_N/RC.ENTITY_CD', 'BOCES_and_N/RC.COUNTY_NAME', 'Teachers_Teaching_Out_of_Certification.ENTITY_CD'}</t>
         </is>
       </c>
       <c r="T359" t="inlineStr">
@@ -29250,7 +29250,7 @@
       </c>
       <c r="S360" t="inlineStr">
         <is>
-          <t>{'Total_Cohort_Regents_Exams.SUBJECT', 'Total_Cohort_Regents_Exams.LEVEL3_COUNT', 'Total_Cohort_Regents_Exams.TEST_COUNT', 'Total_Cohort_Regents_Exams.LEVEL4_COUNT', 'Total_Cohort_Regents_Exams.SUBGROUP_NAME', 'Total_Cohort_Regents_Exams.COHORT', 'Total_Cohort_Regents_Exams.LEVEL2_COUNT', 'Total_Cohort_Regents_Exams.COHORT_COUNT', 'Total_Cohort_Regents_Exams.LEVEL1_COUNT', 'Total_Cohort_Regents_Exams.ENTITY_NAME'}</t>
+          <t>{'Total_Cohort_Regents_Exams.LEVEL1_COUNT', 'Total_Cohort_Regents_Exams.LEVEL4_COUNT', 'Total_Cohort_Regents_Exams.LEVEL2_COUNT', 'Total_Cohort_Regents_Exams.COHORT_COUNT', 'Total_Cohort_Regents_Exams.TEST_COUNT', 'Total_Cohort_Regents_Exams.COHORT', 'Total_Cohort_Regents_Exams.ENTITY_NAME', 'Total_Cohort_Regents_Exams.LEVEL3_COUNT', 'Total_Cohort_Regents_Exams.SUBJECT', 'Total_Cohort_Regents_Exams.SUBGROUP_NAME'}</t>
         </is>
       </c>
       <c r="T360" t="inlineStr">
@@ -29315,7 +29315,7 @@
       </c>
       <c r="P361" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Institution_Grouping', 'Total_Cohort_Regents_Exams'}</t>
         </is>
       </c>
       <c r="Q361" t="inlineStr">
@@ -29330,7 +29330,7 @@
       </c>
       <c r="S361" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Total_Cohort_Regents_Exams.ENTITY_CD', 'Institution_Grouping.GROUP_NAME', 'Total_Cohort_Regents_Exams.ENTITY_NAME', 'Total_Cohort_Regents_Exams.COHORT', 'Total_Cohort_Regents_Exams.LEVEL4_%COHORT', 'Total_Cohort_Regents_Exams.SUBJECT', 'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.ENTITY_NAME', 'Total_Cohort_Regents_Exams.SUBGROUP_NAME'}</t>
         </is>
       </c>
       <c r="T361" t="inlineStr">
@@ -29490,7 +29490,7 @@
       </c>
       <c r="S363" t="inlineStr">
         <is>
-          <t>{'Annual_EM_SCIENCE.SUBGROUP_NAME', 'Annual_EM_SCIENCE.ASSESSMENT_NAME', 'Annual_EM_SCIENCE.TOTAL_COUNT', 'Annual_EM_SCIENCE.YEAR', 'Annual_EM_SCIENCE.ENTITY_NAME'}</t>
+          <t>{'Annual_EM_SCIENCE.ASSESSMENT_NAME', 'Annual_EM_SCIENCE.TOTAL_COUNT', 'Annual_EM_SCIENCE.ENTITY_NAME', 'Annual_EM_SCIENCE.YEAR', 'Annual_EM_SCIENCE.SUBGROUP_NAME'}</t>
         </is>
       </c>
       <c r="T363" t="inlineStr">
@@ -29555,7 +29555,7 @@
       </c>
       <c r="P364" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Postsecondary_Enrollment', 'Institution_Grouping'}</t>
         </is>
       </c>
       <c r="Q364" t="inlineStr">
@@ -29570,7 +29570,7 @@
       </c>
       <c r="S364" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'Postsecondary_Enrollment.ENTITY_CD', 'Postsecondary_Enrollment.YEAR', 'Institution_Grouping.GROUP_NAME', 'Postsecondary_Enrollment.PER_OUT_4_YR', 'Postsecondary_Enrollment.SUBGROUP_NAME', 'Institution_Grouping.ENTITY_CD', 'Institution_Grouping.ENTITY_NAME', 'Postsecondary_Enrollment.ENTITY_NAME'}</t>
         </is>
       </c>
       <c r="T364" t="inlineStr">
@@ -30130,7 +30130,7 @@
       </c>
       <c r="S371" t="inlineStr">
         <is>
-          <t>{'tlu_Contacts.City', 'tlu_Contacts.Zip_Code'}</t>
+          <t>{'tlu_Contacts.Zip_Code', 'tlu_Contacts.City'}</t>
         </is>
       </c>
       <c r="T371" t="inlineStr">
@@ -30210,7 +30210,7 @@
       </c>
       <c r="S372" t="inlineStr">
         <is>
-          <t>{'tbl_Events.Start_Date', 'tbl_Events.Verified_by', 'tbl_Events.Repeat_Sample', 'tbl_Events.Station_ID', 'tbl_Events.Event_ID'}</t>
+          <t>{'tbl_Events.Station_ID', 'tbl_Events.Repeat_Sample', 'tbl_Events.Event_ID', 'tbl_Events.Start_Date', 'tbl_Events.Verified_by'}</t>
         </is>
       </c>
       <c r="T372" t="inlineStr">
@@ -30290,7 +30290,7 @@
       </c>
       <c r="S373" t="inlineStr">
         <is>
-          <t>{'tlu_Species.Species_ID', 'tlu_Species.Habitat', 'tbl_Observations.Species_ID'}</t>
+          <t>{'tlu_Species.Species_ID', 'tbl_Observations.Species_ID', 'tlu_Species.Habitat'}</t>
         </is>
       </c>
       <c r="T373" t="inlineStr">
@@ -30370,7 +30370,7 @@
       </c>
       <c r="S374" t="inlineStr">
         <is>
-          <t>{'tlu_Species.Species_ID', 'tlu_Species.Habitat', 'tbl_Observations.Species_ID'}</t>
+          <t>{'tlu_Species.Species_ID', 'tbl_Observations.Species_ID', 'tlu_Species.Habitat'}</t>
         </is>
       </c>
       <c r="T374" t="inlineStr">
@@ -30450,7 +30450,7 @@
       </c>
       <c r="S375" t="inlineStr">
         <is>
-          <t>{'tbl_Observations.Event_ID', 'tbl_Events.Event_ID'}</t>
+          <t>{'tbl_Events.Event_ID', 'tbl_Observations.Event_ID'}</t>
         </is>
       </c>
       <c r="T375" t="inlineStr">
@@ -30515,7 +30515,7 @@
       </c>
       <c r="P376" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Observations', 'tlu_Species'}</t>
         </is>
       </c>
       <c r="Q376" t="inlineStr">
@@ -30530,7 +30530,7 @@
       </c>
       <c r="S376" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tlu_Species.Common_Name', 'tlu_Species.Scientific_Name', 'tlu_Species.Species_ID', 'tbl_Observations.Species_ID'}</t>
         </is>
       </c>
       <c r="T376" t="inlineStr">
@@ -30595,7 +30595,7 @@
       </c>
       <c r="P377" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Events', 'tbl_Habitat'}</t>
         </is>
       </c>
       <c r="Q377" t="inlineStr">
@@ -30610,7 +30610,7 @@
       </c>
       <c r="S377" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Habitat.Understory_Comp', 'tbl_Events.Event_ID', 'tbl_Habitat.Event_ID', 'tbl_Events.Entered_by', 'tbl_Habitat.Canopy_Comp'}</t>
         </is>
       </c>
       <c r="T377" t="inlineStr">
@@ -30690,7 +30690,7 @@
       </c>
       <c r="S378" t="inlineStr">
         <is>
-          <t>{'tbl_Event_Details.Rain', 'tbl_Events.Event_ID', 'tbl_Event_Details.Wind', 'tbl_Events.Entered_by', 'tbl_Event_Details.Cloud', 'tbl_Event_Details.Gust', 'tbl_Event_Details.Event_ID', 'tbl_Events.Updated_by'}</t>
+          <t>{'tbl_Event_Details.Cloud', 'tbl_Events.Event_ID', 'tbl_Event_Details.Wind', 'tbl_Events.Entered_by', 'tbl_Events.Updated_by', 'tbl_Event_Details.Rain', 'tbl_Event_Details.Event_ID', 'tbl_Event_Details.Gust'}</t>
         </is>
       </c>
       <c r="T378" t="inlineStr">
@@ -30915,7 +30915,7 @@
       </c>
       <c r="P381" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Detections', 'tbl_Observations', 'tlu_Species'}</t>
         </is>
       </c>
       <c r="Q381" t="inlineStr">
@@ -30930,7 +30930,7 @@
       </c>
       <c r="S381" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Observations.Observation_ID', 'tbl_Observations.Species_ID', 'tbl_Detections.Distance', 'tlu_Species.Common_Name', 'tbl_Detections.Observation_ID', 'tlu_Species.Species_ID'}</t>
         </is>
       </c>
       <c r="T381" t="inlineStr">
@@ -31010,7 +31010,7 @@
       </c>
       <c r="S382" t="inlineStr">
         <is>
-          <t>{'tlu_Species.Common_Name', 'xref_Species_Alternate_Names.Alternate_Name', 'tlu_Species.Species_ID', 'tlu_Species.Family', 'xref_Species_Alternate_Names.Species_ID'}</t>
+          <t>{'tlu_Species.Common_Name', 'tlu_Species.Species_ID', 'tlu_Species.Family', 'xref_Species_Alternate_Names.Alternate_Name', 'xref_Species_Alternate_Names.Species_ID'}</t>
         </is>
       </c>
       <c r="T382" t="inlineStr">
@@ -31155,7 +31155,7 @@
       </c>
       <c r="P384" t="inlineStr">
         <is>
-          <t>{'tbl_Stations_UTMs', 'tbl_Stations'}</t>
+          <t>{'tbl_Stations', 'tbl_Stations_UTMs'}</t>
         </is>
       </c>
       <c r="Q384" t="inlineStr">
@@ -31170,7 +31170,7 @@
       </c>
       <c r="S384" t="inlineStr">
         <is>
-          <t>{'tbl_Stations_UTMs.Y_final', 'tbl_Stations_UTMs.Station_ID', 'tbl_Stations.Station', 'tbl_Stations.Station_ID', 'tbl_Stations_UTMs.X_final'}</t>
+          <t>{'tbl_Stations.Station_ID', 'tbl_Stations_UTMs.X_final', 'tbl_Stations.Station', 'tbl_Stations_UTMs.Station_ID', 'tbl_Stations_UTMs.Y_final'}</t>
         </is>
       </c>
       <c r="T384" t="inlineStr">
@@ -31250,7 +31250,7 @@
       </c>
       <c r="S385" t="inlineStr">
         <is>
-          <t>{'tlu_Contacts.Last_Name', 'tlu_Contacts.First_Name', 'tlu_Contacts.Position_Title', 'tlu_Contacts.Organization'}</t>
+          <t>{'tlu_Contacts.Last_Name', 'tlu_Contacts.Organization', 'tlu_Contacts.First_Name', 'tlu_Contacts.Position_Title'}</t>
         </is>
       </c>
       <c r="T385" t="inlineStr">
@@ -31315,7 +31315,7 @@
       </c>
       <c r="P386" t="inlineStr">
         <is>
-          <t>{'tbl_Locations', 'tbl_Sites'}</t>
+          <t>{'tbl_Sites', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q386" t="inlineStr">
@@ -31330,7 +31330,7 @@
       </c>
       <c r="S386" t="inlineStr">
         <is>
-          <t>{'tbl_Locations.Site_ID', 'tbl_Locations.Island', 'tbl_Sites.Site_Name', 'tbl_Sites.Site_ID'}</t>
+          <t>{'tbl_Locations.Island', 'tbl_Sites.Site_Name', 'tbl_Sites.Site_ID', 'tbl_Locations.Site_ID'}</t>
         </is>
       </c>
       <c r="T386" t="inlineStr">
@@ -31490,7 +31490,7 @@
       </c>
       <c r="S388" t="inlineStr">
         <is>
-          <t>{'tlu_Species.Scientific_Name', 'tlu_Species.Family', 'tlu_Species.Common_Name', 'tlu_Species.Habitat'}</t>
+          <t>{'tlu_Species.Common_Name', 'tlu_Species.Scientific_Name', 'tlu_Species.Family', 'tlu_Species.Habitat'}</t>
         </is>
       </c>
       <c r="T388" t="inlineStr">
@@ -31635,7 +31635,7 @@
       </c>
       <c r="P390" t="inlineStr">
         <is>
-          <t>{'tbl_Observations', 'tbl_Event_Details'}</t>
+          <t>{'tbl_Event_Details', 'tbl_Observations'}</t>
         </is>
       </c>
       <c r="Q390" t="inlineStr">
@@ -31650,7 +31650,7 @@
       </c>
       <c r="S390" t="inlineStr">
         <is>
-          <t>{'tbl_Event_Details.Cloud', 'tbl_Event_Details.Event_ID', 'tbl_Observations.Event_ID'}</t>
+          <t>{'tbl_Event_Details.Event_ID', 'tbl_Event_Details.Cloud', 'tbl_Observations.Event_ID'}</t>
         </is>
       </c>
       <c r="T390" t="inlineStr">
@@ -31795,7 +31795,7 @@
       </c>
       <c r="P392" t="inlineStr">
         <is>
-          <t>{'tbl_Transect', 'tbl_Locations', 'tbl_Stations'}</t>
+          <t>{'tbl_Stations', 'tbl_Transect', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q392" t="inlineStr">
@@ -31810,7 +31810,7 @@
       </c>
       <c r="S392" t="inlineStr">
         <is>
-          <t>{'tbl_Transect.Transect_ID', 'tbl_Stations.Transect_ID', 'tbl_Locations.Location_ID', 'tbl_Locations.Island', 'tbl_Transect.Location_ID'}</t>
+          <t>{'tbl_Transect.Transect_ID', 'tbl_Transect.Location_ID', 'tbl_Locations.Location_ID', 'tbl_Locations.Island', 'tbl_Stations.Transect_ID'}</t>
         </is>
       </c>
       <c r="T392" t="inlineStr">
@@ -31875,7 +31875,7 @@
       </c>
       <c r="P393" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Stations', 'tbl_Transect', 'tbl_Locations'}</t>
         </is>
       </c>
       <c r="Q393" t="inlineStr">
@@ -31890,7 +31890,7 @@
       </c>
       <c r="S393" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Transect.Transect_ID', 'tbl_Transect.Location_ID', 'tbl_Locations.Location_ID', 'tbl_Locations.Island', 'tbl_Stations.Transect_ID'}</t>
         </is>
       </c>
       <c r="T393" t="inlineStr">
@@ -31955,7 +31955,7 @@
       </c>
       <c r="P394" t="inlineStr">
         <is>
-          <t>{'tbl_Events', 'tlu_Species', 'tbl_Observations', 'tbl_Event_Details'}</t>
+          <t>{'tbl_Events', 'tbl_Event_Details', 'tbl_Observations', 'tlu_Species'}</t>
         </is>
       </c>
       <c r="Q394" t="inlineStr">
@@ -31970,7 +31970,7 @@
       </c>
       <c r="S394" t="inlineStr">
         <is>
-          <t>{'tlu_Species.Species_ID', 'tlu_Species.Species_Code', 'tlu_Species.Family', 'tbl_Event_Details.Rain', 'tbl_Events.Event_ID', 'tbl_Event_Details.Event_ID', 'tbl_Observations.Event_ID', 'tbl_Observations.Species_ID'}</t>
+          <t>{'tbl_Events.Event_ID', 'tlu_Species.Species_ID', 'tlu_Species.Family', 'tlu_Species.Species_Code', 'tbl_Event_Details.Rain', 'tbl_Observations.Species_ID', 'tbl_Observations.Event_ID', 'tbl_Event_Details.Event_ID'}</t>
         </is>
       </c>
       <c r="T394" t="inlineStr">
@@ -32035,7 +32035,7 @@
       </c>
       <c r="P395" t="inlineStr">
         <is>
-          <t>{'tlu_Contacts', 'tbl_Observations', 'tlu_Species', 'xref_Event_Contacts'}</t>
+          <t>{'tlu_Contacts', 'tbl_Observations', 'xref_Event_Contacts', 'tlu_Species'}</t>
         </is>
       </c>
       <c r="Q395" t="inlineStr">
@@ -32050,7 +32050,7 @@
       </c>
       <c r="S395" t="inlineStr">
         <is>
-          <t>{'tlu_Species.Scientific_Name', 'tlu_Contacts.First_Name', 'xref_Event_Contacts.Event_ID', 'tlu_Species.Species_ID', 'tlu_Species.Common_Name', 'tbl_Observations.Event_ID', 'xref_Event_Contacts.Contact_ID', 'tlu_Contacts.Last_Name', 'tbl_Observations.Species_ID', 'tlu_Contacts.Contact_ID'}</t>
+          <t>{'tlu_Species.Scientific_Name', 'tlu_Contacts.Contact_ID', 'tlu_Contacts.Last_Name', 'tlu_Species.Common_Name', 'tlu_Species.Species_ID', 'xref_Event_Contacts.Event_ID', 'tbl_Observations.Species_ID', 'tbl_Observations.Event_ID', 'xref_Event_Contacts.Contact_ID', 'tlu_Contacts.First_Name'}</t>
         </is>
       </c>
       <c r="T395" t="inlineStr">
@@ -32115,7 +32115,7 @@
       </c>
       <c r="P396" t="inlineStr">
         <is>
-          <t>{'tbl_Events', 'tlu_Species', 'tbl_Observations', 'tbl_Stations'}</t>
+          <t>{'tbl_Events', 'tbl_Stations', 'tbl_Observations', 'tlu_Species'}</t>
         </is>
       </c>
       <c r="Q396" t="inlineStr">
@@ -32130,7 +32130,7 @@
       </c>
       <c r="S396" t="inlineStr">
         <is>
-          <t>{'tlu_Species.Species_ID', 'tbl_Stations.Station', 'tbl_Events.Event_ID', 'tlu_Species.Common_Name', 'tbl_Observations.Event_ID', 'tbl_Stations.Station_ID', 'tbl_Observations.Species_ID', 'tbl_Events.Station_ID'}</t>
+          <t>{'tbl_Events.Station_ID', 'tbl_Events.Event_ID', 'tlu_Species.Common_Name', 'tlu_Species.Species_ID', 'tbl_Stations.Station_ID', 'tbl_Observations.Species_ID', 'tbl_Observations.Event_ID', 'tbl_Stations.Station'}</t>
         </is>
       </c>
       <c r="T396" t="inlineStr">
@@ -32210,7 +32210,7 @@
       </c>
       <c r="S397" t="inlineStr">
         <is>
-          <t>{'tbl_Stations.Station', 'tbl_Stations.Station_ID', 'tbl_Events.Station_ID'}</t>
+          <t>{'tbl_Stations.Station_ID', 'tbl_Events.Station_ID', 'tbl_Stations.Station'}</t>
         </is>
       </c>
       <c r="T397" t="inlineStr">
@@ -32275,7 +32275,7 @@
       </c>
       <c r="P398" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Stations'}</t>
         </is>
       </c>
       <c r="Q398" t="inlineStr">
@@ -32290,7 +32290,7 @@
       </c>
       <c r="S398" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Stations.Lat_final', 'tbl_Stations.Long_final', 'tbl_Stations.Station'}</t>
         </is>
       </c>
       <c r="T398" t="inlineStr">
@@ -32355,7 +32355,7 @@
       </c>
       <c r="P399" t="inlineStr">
         <is>
-          <t>{'tbl_Events', 'tlu_Species', 'tbl_Observations', 'tbl_Stations'}</t>
+          <t>{'tbl_Events', 'tbl_Stations', 'tbl_Observations', 'tlu_Species'}</t>
         </is>
       </c>
       <c r="Q399" t="inlineStr">
@@ -32370,7 +32370,7 @@
       </c>
       <c r="S399" t="inlineStr">
         <is>
-          <t>{'tlu_Species.Common_Name', 'tbl_Observations.Event_ID', 'tlu_Species.Species_ID', 'tbl_Stations.Station_ID', 'tbl_Observations.Species_ID', 'tbl_Events.Station_ID', 'tbl_Events.Event_ID'}</t>
+          <t>{'tbl_Stations.Station_ID', 'tbl_Events.Station_ID', 'tbl_Events.Event_ID', 'tbl_Observations.Species_ID', 'tbl_Observations.Event_ID', 'tlu_Species.Common_Name', 'tlu_Species.Species_ID'}</t>
         </is>
       </c>
       <c r="T399" t="inlineStr">
@@ -32435,7 +32435,7 @@
       </c>
       <c r="P400" t="inlineStr">
         <is>
-          <t>{'tbl_Events', 'tlu_Species', 'tbl_Observations', 'tbl_Stations'}</t>
+          <t>{'tbl_Events', 'tbl_Stations', 'tbl_Observations', 'tlu_Species'}</t>
         </is>
       </c>
       <c r="Q400" t="inlineStr">
@@ -32450,7 +32450,7 @@
       </c>
       <c r="S400" t="inlineStr">
         <is>
-          <t>{'tlu_Species.Common_Name', 'tbl_Observations.Event_ID', 'tlu_Species.Species_ID', 'tbl_Stations.Station_ID', 'tbl_Observations.Species_ID', 'tbl_Events.Station_ID', 'tbl_Events.Event_ID'}</t>
+          <t>{'tbl_Stations.Station_ID', 'tbl_Events.Station_ID', 'tbl_Events.Event_ID', 'tbl_Observations.Species_ID', 'tbl_Observations.Event_ID', 'tlu_Species.Common_Name', 'tlu_Species.Species_ID'}</t>
         </is>
       </c>
       <c r="T400" t="inlineStr">
@@ -32530,7 +32530,7 @@
       </c>
       <c r="S401" t="inlineStr">
         <is>
-          <t>{'tlu_Contacts.First_Name', 'xref_Event_Contacts.Contact_ID', 'tlu_Contacts.Organization', 'tlu_Contacts.Last_Name', 'tlu_Contacts.Contact_ID'}</t>
+          <t>{'tlu_Contacts.Organization', 'tlu_Contacts.Contact_ID', 'xref_Event_Contacts.Contact_ID', 'tlu_Contacts.Last_Name', 'tlu_Contacts.First_Name'}</t>
         </is>
       </c>
       <c r="T401" t="inlineStr">
@@ -32595,7 +32595,7 @@
       </c>
       <c r="P402" t="inlineStr">
         <is>
-          <t>{'tbl_Events', 'tbl_Habitat', 'tlu_Species', 'tbl_Observations'}</t>
+          <t>{'tbl_Events', 'tbl_Habitat', 'tbl_Observations', 'tlu_Species'}</t>
         </is>
       </c>
       <c r="Q402" t="inlineStr">
@@ -32610,7 +32610,7 @@
       </c>
       <c r="S402" t="inlineStr">
         <is>
-          <t>{'tlu_Species.Scientific_Name', 'tbl_Habitat.Event_ID', 'tlu_Species.Species_ID', 'tbl_Events.Event_ID', 'tbl_Habitat.Canopy_Height', 'tlu_Species.Common_Name', 'tbl_Observations.Event_ID', 'tbl_Observations.Species_ID'}</t>
+          <t>{'tlu_Species.Scientific_Name', 'tbl_Events.Event_ID', 'tlu_Species.Common_Name', 'tlu_Species.Species_ID', 'tbl_Habitat.Event_ID', 'tbl_Habitat.Canopy_Height', 'tbl_Observations.Species_ID', 'tbl_Observations.Event_ID'}</t>
         </is>
       </c>
       <c r="T402" t="inlineStr">
@@ -32675,7 +32675,7 @@
       </c>
       <c r="P403" t="inlineStr">
         <is>
-          <t>{'tlu_Contacts', 'xref_Species_Alternate_Names', 'tbl_Stations', 'xref_Event_Contacts', 'tbl_Transect', 'tbl_Observations', 'tbl_Locations', 'tlu_Species', 'tbl_Sites', 'tbl_Events'}</t>
+          <t>{'tbl_Events', 'xref_Species_Alternate_Names', 'tlu_Species', 'tbl_Locations', 'tbl_Transect', 'tbl_Stations', 'tlu_Contacts', 'tbl_Observations', 'xref_Event_Contacts', 'tbl_Sites'}</t>
         </is>
       </c>
       <c r="Q403" t="inlineStr">
@@ -32690,7 +32690,7 @@
       </c>
       <c r="S403" t="inlineStr">
         <is>
-          <t>{'tbl_Stations.Transect_ID', 'tbl_Locations.Location_ID', 'xref_Event_Contacts.Event_ID', 'xref_Species_Alternate_Names.Alternate_Name', 'xref_Species_Alternate_Names.Species_ID', 'tlu_Species.Family', 'tbl_Transect.Location_ID', 'tbl_Events.Event_ID', 'tbl_Sites.Site_ID', 'tbl_Events.Event_Notes', 'tlu_Species.Common_Name', 'tbl_Observations.Event_ID', 'tbl_Locations.Site_ID', 'tlu_Contacts.Last_Name', 'tbl_Transect.Transect', 'tbl_Stations.Station_ID', 'tbl_Locations.Island', 'tbl_Events.Station_ID', 'tbl_Transect.Transect_Type', 'tlu_Contacts.Contact_ID', 'tlu_Species.Scientific_Name', 'tbl_Transect.Transect_ID', 'tbl_Sites.Site_Name', 'tbl_Stations.Station', 'tlu_Species.Species_ID', 'tbl_Stations.Lat_final', 'tbl_Observations.Species_ID', 'xref_Event_Contacts.Contact_ID', 'tbl_Locations.Loc_Name'}</t>
+          <t>{'tlu_Contacts.Contact_ID', 'tbl_Transect.Transect', 'tbl_Events.Event_Notes', 'tlu_Species.Common_Name', 'tbl_Locations.Island', 'tlu_Species.Species_ID', 'tlu_Species.Family', 'tlu_Contacts.Last_Name', 'xref_Species_Alternate_Names.Alternate_Name', 'tbl_Stations.Station_ID', 'tbl_Observations.Species_ID', 'xref_Event_Contacts.Contact_ID', 'tbl_Stations.Station', 'tbl_Sites.Site_Name', 'tbl_Sites.Site_ID', 'xref_Species_Alternate_Names.Species_ID', 'tlu_Species.Scientific_Name', 'tbl_Events.Station_ID', 'tbl_Events.Event_ID', 'tbl_Transect.Transect_Type', 'tbl_Locations.Location_ID', 'xref_Event_Contacts.Event_ID', 'tbl_Stations.Lat_final', 'tbl_Transect.Transect_ID', 'tbl_Transect.Location_ID', 'tbl_Locations.Loc_Name', 'tbl_Observations.Event_ID', 'tbl_Stations.Transect_ID', 'tbl_Locations.Site_ID'}</t>
         </is>
       </c>
       <c r="T403" t="inlineStr">
@@ -32755,7 +32755,7 @@
       </c>
       <c r="P404" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Events', 'tlu_Species', 'tbl_Locations', 'tbl_Transect', 'tbl_Stations', 'tbl_Observations', 'tlu_Contacts', 'xref_Event_Contacts'}</t>
         </is>
       </c>
       <c r="Q404" t="inlineStr">
@@ -32770,7 +32770,7 @@
       </c>
       <c r="S404" t="inlineStr">
         <is>
-          <t>set()</t>
+          <t>{'tbl_Events.Station_ID', 'tbl_Events.Event_ID', 'tlu_Contacts.Contact_ID', 'tbl_Locations.Location_ID', 'tlu_Species.Common_Name', 'tbl_Locations.Island', 'tlu_Species.Species_ID', 'xref_Event_Contacts.Event_ID', 'tbl_Stations.Station_ID', 'tbl_Transect.Transect_ID', 'tbl_Transect.Location_ID', 'tbl_Observations.Species_ID', 'tbl_Observations.Event_ID', 'xref_Event_Contacts.Contact_ID', 'tbl_Stations.Transect_ID'}</t>
         </is>
       </c>
       <c r="T404" t="inlineStr">
@@ -32915,7 +32915,7 @@
       </c>
       <c r="P406" t="inlineStr">
         <is>
-          <t>{'OPEX', 'OUDP'}</t>
+          <t>{'OUDP', 'OPEX'}</t>
         </is>
       </c>
       <c r="Q406" t="inlineStr">
@@ -32930,7 +32930,7 @@
       </c>
       <c r="S406" t="inlineStr">
         <is>
-          <t>{'OPEX.PayeeCity', 'OPEX.PayeeZip', 'OUDP.Name', 'OPEX.PayCountry', 'OPEX.PayeeState', 'OPEX.PayeeName', 'OPEX.PayeeStree', 'OPEX.Department', 'OUDP.Code'}</t>
+          <t>{'OPEX.Department', 'OPEX.PayeeName', 'OPEX.PayeeStree', 'OPEX.PayeeZip', 'OPEX.PayeeCity', 'OPEX.PayCountry', 'OUDP.Code', 'OPEX.PayeeState', 'OUDP.Name'}</t>
         </is>
       </c>
       <c r="T406" t="inlineStr">
@@ -32995,7 +32995,7 @@
       </c>
       <c r="P407" t="inlineStr">
         <is>
-          <t>{'CHO1', 'OCHO'}</t>
+          <t>{'OCHO', 'CHO1'}</t>
         </is>
       </c>
       <c r="Q407" t="inlineStr">
@@ -33010,7 +33010,7 @@
       </c>
       <c r="S407" t="inlineStr">
         <is>
-          <t>{'OCHO.AcctNum', 'CHO1.CheckKey', 'OCHO.CheckKey'}</t>
+          <t>{'CHO1.CheckKey', 'OCHO.AcctNum', 'OCHO.CheckKey'}</t>
         </is>
       </c>
       <c r="T407" t="inlineStr">
@@ -33090,7 +33090,7 @@
       </c>
       <c r="S408" t="inlineStr">
         <is>
-          <t>{'OCHO.AcctNum', 'OCHO.Deduction', 'OCHO.DdctPrcnt'}</t>
+          <t>{'OCHO.DdctPrcnt', 'OCHO.AcctNum', 'OCHO.Deduction'}</t>
         </is>
       </c>
       <c r="T408" t="inlineStr">
@@ -33170,7 +33170,7 @@
       </c>
       <c r="S409" t="inlineStr">
         <is>
-          <t>{'ORCT.CreateDate', 'ORCT.TrsfrSumFC', 'ORCT.Address', 'ORCT.CardName', 'ORCT.CardCode', 'ORCT.DocCurr'}</t>
+          <t>{'ORCT.DocCurr', 'ORCT.Address', 'ORCT.CardCode', 'ORCT.TrsfrSumFC', 'ORCT.CardName', 'ORCT.CreateDate'}</t>
         </is>
       </c>
       <c r="T409" t="inlineStr">
@@ -33235,7 +33235,7 @@
       </c>
       <c r="P410" t="inlineStr">
         <is>
-          <t>{'ORCT', 'RCT1'}</t>
+          <t>{'RCT1', 'ORCT'}</t>
         </is>
       </c>
       <c r="Q410" t="inlineStr">
@@ -33250,7 +33250,7 @@
       </c>
       <c r="S410" t="inlineStr">
         <is>
-          <t>{'RCT1.DocNum', 'RCT1.AcctNum', 'ORCT.WTOnhldPst', 'ORCT.CheckSumFC', 'ORCT.DocNum', 'RCT1.CountryCod'}</t>
+          <t>{'ORCT.CheckSumFC', 'ORCT.WTOnhldPst', 'RCT1.AcctNum', 'ORCT.DocNum', 'RCT1.CountryCod', 'RCT1.DocNum'}</t>
         </is>
       </c>
       <c r="T410" t="inlineStr">
@@ -33410,7 +33410,7 @@
       </c>
       <c r="S412" t="inlineStr">
         <is>
-          <t>{'ORCT.DocNum', 'RCT3.FirstSum', 'RCT3.DocNum'}</t>
+          <t>{'RCT3.DocNum', 'ORCT.DocNum', 'RCT3.FirstSum'}</t>
         </is>
       </c>
       <c r="T412" t="inlineStr">
@@ -33490,7 +33490,7 @@
       </c>
       <c r="S413" t="inlineStr">
         <is>
-          <t>{'OCRH.DeposDate', 'OCRH.RctAbs', 'OCRH.DepNum', 'OCRH.CardCode'}</t>
+          <t>{'OCRH.RctAbs', 'OCRH.DepNum', 'OCRH.CardCode', 'OCRH.DeposDate'}</t>
         </is>
       </c>
       <c r="T413" t="inlineStr">
@@ -33570,7 +33570,7 @@
       </c>
       <c r="S414" t="inlineStr">
         <is>
-          <t>{'OCTG.VATFirst', 'OCTG.ExtraDays', 'OCTG.PymntGroup', 'OCTG.InstNum'}</t>
+          <t>{'OCTG.InstNum', 'OCTG.ExtraDays', 'OCTG.VATFirst', 'OCTG.PymntGroup'}</t>
         </is>
       </c>
       <c r="T414" t="inlineStr">
@@ -33635,7 +33635,7 @@
       </c>
       <c r="P415" t="inlineStr">
         <is>
-          <t>{'OCRD', 'OCRG'}</t>
+          <t>{'OCRG', 'OCRD'}</t>
         </is>
       </c>
       <c r="Q415" t="inlineStr">
@@ -33650,7 +33650,7 @@
       </c>
       <c r="S415" t="inlineStr">
         <is>
-          <t>{'OCRG.GroupCode', 'OCRG.GroupName', 'OCRD.GroupCode'}</t>
+          <t>{'OCRG.GroupCode', 'OCRD.GroupCode', 'OCRG.GroupName'}</t>
         </is>
       </c>
       <c r="T415" t="inlineStr">
@@ -33730,7 +33730,7 @@
       </c>
       <c r="S416" t="inlineStr">
         <is>
-          <t>{'OCPR.Position', 'OCPR.E_MailL', 'OCPR.Cellolar', 'OCPR.Address', 'OCPR.Name'}</t>
+          <t>{'OCPR.Position', 'OCPR.Cellolar', 'OCPR.Address', 'OCPR.E_MailL', 'OCPR.Name'}</t>
         </is>
       </c>
       <c r="T416" t="inlineStr">
@@ -33890,7 +33890,7 @@
       </c>
       <c r="S418" t="inlineStr">
         <is>
-          <t>{'OSLP.GroupCode', 'OCOG.GroupCode', 'OCOG.GroupName', 'OSLP.SlpName'}</t>
+          <t>{'OSLP.GroupCode', 'OSLP.SlpName', 'OCOG.GroupName', 'OCOG.GroupCode'}</t>
         </is>
       </c>
       <c r="T418" t="inlineStr">
@@ -33970,7 +33970,7 @@
       </c>
       <c r="S419" t="inlineStr">
         <is>
-          <t>{'OSLP.Mobil', 'OSLP.SlpName', 'OSLP.Email', 'OSLP.GroupCode', 'OCOG.GroupName', 'OCOG.GroupCode'}</t>
+          <t>{'OSLP.GroupCode', 'OSLP.Mobil', 'OCOG.GroupCode', 'OCOG.GroupName', 'OSLP.Email', 'OSLP.SlpName'}</t>
         </is>
       </c>
       <c r="T419" t="inlineStr">
@@ -34050,7 +34050,7 @@
       </c>
       <c r="S420" t="inlineStr">
         <is>
-          <t>{'OCRD.PymCode', 'OCRD.CardCode', 'CRD1.CardCode', 'CRD1.TaxCode', 'OCRD.CDPNum'}</t>
+          <t>{'OCRD.PymCode', 'CRD1.CardCode', 'OCRD.CardCode', 'OCRD.CDPNum', 'CRD1.TaxCode'}</t>
         </is>
       </c>
       <c r="T420" t="inlineStr">
@@ -34130,7 +34130,7 @@
       </c>
       <c r="S421" t="inlineStr">
         <is>
-          <t>{'OCLG.CntctTime', 'OCLG.CreateDate', 'OCLG.CntctDate', 'OCLG.ClgCode', 'OCLG.Details'}</t>
+          <t>{'OCLG.CntctDate', 'OCLG.CreateDate', 'OCLG.Details', 'OCLG.ClgCode', 'OCLG.CntctTime'}</t>
         </is>
       </c>
       <c r="T421" t="inlineStr">
@@ -34195,7 +34195,7 @@
       </c>
       <c r="P422" t="inlineStr">
         <is>
-          <t>{'OCRD', 'OCRB'}</t>
+          <t>{'OCRB', 'OCRD'}</t>
         </is>
       </c>
       <c r="Q422" t="inlineStr">
@@ -34210,7 +34210,7 @@
       </c>
       <c r="S422" t="inlineStr">
         <is>
-          <t>{'OCRB.City', 'OCRD.Country', 'OCRD.CardCode', 'OCRB.BankCode', 'OCRD.City', 'OCRB.CardCode', 'OCRB.Country', 'OCRB.Account', 'OCRB.Branch', 'OCRD.CardName', 'OCRD.BankCode'}</t>
+          <t>{'OCRB.BankCode', 'OCRB.CardCode', 'OCRB.Country', 'OCRD.CardCode', 'OCRD.BankCode', 'OCRB.Branch', 'OCRD.City', 'OCRB.City', 'OCRD.Country', 'OCRD.CardName', 'OCRB.Account'}</t>
         </is>
       </c>
       <c r="T422" t="inlineStr">
@@ -34290,7 +34290,7 @@
       </c>
       <c r="S423" t="inlineStr">
         <is>
-          <t>{'OCRD.Balance', 'OCRD.PymCode', 'OCRD.Currency'}</t>
+          <t>{'OCRD.PymCode', 'OCRD.Balance', 'OCRD.Currency'}</t>
         </is>
       </c>
       <c r="T423" t="inlineStr">
@@ -34355,7 +34355,7 @@
       </c>
       <c r="P424" t="inlineStr">
         <is>
-          <t>{'TGG1', 'OTGG'}</t>
+          <t>{'OTGG', 'TGG1'}</t>
         </is>
       </c>
       <c r="Q424" t="inlineStr">
@@ -34370,7 +34370,7 @@
       </c>
       <c r="S424" t="inlineStr">
         <is>
-          <t>{'OTGG.TargetCode', 'TGG1.TargetCode', 'TGG1.Position', 'TGG1.LicTradNum', 'OTGG.TargetType', 'TGG1.E_Mail'}</t>
+          <t>{'TGG1.Position', 'TGG1.E_Mail', 'TGG1.TargetCode', 'OTGG.TargetType', 'TGG1.LicTradNum', 'OTGG.TargetCode'}</t>
         </is>
       </c>
       <c r="T424" t="inlineStr">
@@ -34435,7 +34435,7 @@
       </c>
       <c r="P425" t="inlineStr">
         <is>
-          <t>{'OACT', 'JDT1'}</t>
+          <t>{'JDT1', 'OACT'}</t>
         </is>
       </c>
       <c r="Q425" t="inlineStr">
@@ -34450,7 +34450,7 @@
       </c>
       <c r="S425" t="inlineStr">
         <is>
-          <t>{'OACT.AcctName', 'OACT.AcctCode', 'JDT1.Account'}</t>
+          <t>{'JDT1.Account', 'OACT.AcctName', 'OACT.AcctCode'}</t>
         </is>
       </c>
       <c r="T425" t="inlineStr">
@@ -34530,7 +34530,7 @@
       </c>
       <c r="S426" t="inlineStr">
         <is>
-          <t>{'JDT1.Credit', 'JDT1.Debit', 'JDT1.DueDate'}</t>
+          <t>{'JDT1.Debit', 'JDT1.Credit', 'JDT1.DueDate'}</t>
         </is>
       </c>
       <c r="T426" t="inlineStr">
@@ -34610,7 +34610,7 @@
       </c>
       <c r="S427" t="inlineStr">
         <is>
-          <t>{'BGT1.AcctCode', 'BGT1.CredLTotal', 'OACT.AcctName', 'BGT1.DebLTotal', 'OACT.AcctCode'}</t>
+          <t>{'BGT1.CredLTotal', 'OACT.AcctCode', 'BGT1.DebLTotal', 'BGT1.AcctCode', 'OACT.AcctName'}</t>
         </is>
       </c>
       <c r="T427" t="inlineStr">
@@ -34690,7 +34690,7 @@
       </c>
       <c r="S428" t="inlineStr">
         <is>
-          <t>{'OACG.Name', 'OACT.CurrTotal', 'OACT.AcctName', 'OACG.AbsId', 'OACT.Category'}</t>
+          <t>{'OACT.Category', 'OACT.CurrTotal', 'OACG.Name', 'OACG.AbsId', 'OACT.AcctName'}</t>
         </is>
       </c>
       <c r="T428" t="inlineStr">
@@ -34755,7 +34755,7 @@
       </c>
       <c r="P429" t="inlineStr">
         <is>
-          <t>{'OTAX', 'TAX1'}</t>
+          <t>{'TAX1', 'OTAX'}</t>
         </is>
       </c>
       <c r="Q429" t="inlineStr">
@@ -34770,7 +34770,7 @@
       </c>
       <c r="S429" t="inlineStr">
         <is>
-          <t>{'TAX1.AbsEntry', 'OTAX.SrcObjAbs', 'TAX1.TaxCode', 'OTAX.AbsEntry', 'TAX1.VatPercent', 'TAX1.VatSum'}</t>
+          <t>{'TAX1.VatPercent', 'OTAX.AbsEntry', 'TAX1.VatSum', 'TAX1.TaxCode', 'TAX1.AbsEntry', 'OTAX.SrcObjAbs'}</t>
         </is>
       </c>
       <c r="T429" t="inlineStr">
@@ -35010,7 +35010,7 @@
       </c>
       <c r="S432" t="inlineStr">
         <is>
-          <t>{'OFRC.FatherNum', 'OFRC.Name'}</t>
+          <t>{'OFRC.Name', 'OFRC.FatherNum'}</t>
         </is>
       </c>
       <c r="T432" t="inlineStr">
@@ -35090,7 +35090,7 @@
       </c>
       <c r="S433" t="inlineStr">
         <is>
-          <t>{'FRC1.CalcMethod', 'FRC1.CFWId', 'FRC1.CalMethod2', 'OFRC.CatId', 'OFRC.Name', 'FRC1.CalMethod3', 'FRC1.CatId'}</t>
+          <t>{'FRC1.CFWId', 'FRC1.CatId', 'OFRC.Name', 'FRC1.CalMethod2', 'OFRC.CatId', 'FRC1.CalcMethod', 'FRC1.CalMethod3'}</t>
         </is>
       </c>
       <c r="T433" t="inlineStr">
@@ -35170,7 +35170,7 @@
       </c>
       <c r="S434" t="inlineStr">
         <is>
-          <t>{'OPRJ.PrjName', 'OPRJ.ValidFrom', 'OPRJ.PrjCode'}</t>
+          <t>{'OPRJ.PrjCode', 'OPRJ.PrjName', 'OPRJ.ValidFrom'}</t>
         </is>
       </c>
       <c r="T434" t="inlineStr">
@@ -35250,7 +35250,7 @@
       </c>
       <c r="S435" t="inlineStr">
         <is>
-          <t>{'PMG1.EXPCOSTS', 'PMG1.START', 'PMG1.DSCRIPTION'}</t>
+          <t>{'PMG1.START', 'PMG1.EXPCOSTS', 'PMG1.DSCRIPTION'}</t>
         </is>
       </c>
       <c r="T435" t="inlineStr">
@@ -35395,7 +35395,7 @@
       </c>
       <c r="P437" t="inlineStr">
         <is>
-          <t>{'ODAB', 'DAB1'}</t>
+          <t>{'DAB1', 'ODAB'}</t>
         </is>
       </c>
       <c r="Q437" t="inlineStr">
@@ -35410,7 +35410,7 @@
       </c>
       <c r="S437" t="inlineStr">
         <is>
-          <t>{'ODAB.AbsEntry', 'DAB1.DsbEntry', 'ODAB.DashbdCode'}</t>
+          <t>{'DAB1.DsbEntry', 'ODAB.DashbdCode', 'ODAB.AbsEntry'}</t>
         </is>
       </c>
       <c r="T437" t="inlineStr">
@@ -35475,7 +35475,7 @@
       </c>
       <c r="P438" t="inlineStr">
         <is>
-          <t>{'ODAB', 'DAB1'}</t>
+          <t>{'DAB1', 'ODAB'}</t>
         </is>
       </c>
       <c r="Q438" t="inlineStr">
@@ -35490,7 +35490,7 @@
       </c>
       <c r="S438" t="inlineStr">
         <is>
-          <t>{'ODAB.Status', 'ODAB.DashbdName', 'DAB1.DsbEntry', 'DAB1.QryCtgry', 'DAB1.QryName', 'ODAB.AbsEntry', 'ODAB.DashbdPath'}</t>
+          <t>{'ODAB.Status', 'ODAB.DashbdName', 'DAB1.QryCtgry', 'DAB1.QryName', 'ODAB.DashbdPath', 'DAB1.DsbEntry', 'ODAB.AbsEntry'}</t>
         </is>
       </c>
       <c r="T438" t="inlineStr">
@@ -35570,7 +35570,7 @@
       </c>
       <c r="S439" t="inlineStr">
         <is>
-          <t>{'OKPS.KpsType', 'OKPS.KpsCode', 'OKPS.FieldsNum', 'OKPS.KpsName'}</t>
+          <t>{'OKPS.KpsName', 'OKPS.FieldsNum', 'OKPS.KpsCode', 'OKPS.KpsType'}</t>
         </is>
       </c>
       <c r="T439" t="inlineStr">
@@ -35650,7 +35650,7 @@
       </c>
       <c r="S440" t="inlineStr">
         <is>
-          <t>{'ORSC.ResCode', 'RSC4.ResCode', 'ORSC.ResGrpCod', 'RSC4.EmpID', 'ORSC.ResName', 'ORSC.StdCost1', 'ORSC.ResType'}</t>
+          <t>{'RSC4.EmpID', 'ORSC.ResType', 'ORSC.StdCost1', 'RSC4.ResCode', 'ORSC.ResName', 'ORSC.ResGrpCod', 'ORSC.ResCode'}</t>
         </is>
       </c>
       <c r="T440" t="inlineStr">
@@ -35715,7 +35715,7 @@
       </c>
       <c r="P441" t="inlineStr">
         <is>
-          <t>{'ORSC', 'RSC6'}</t>
+          <t>{'RSC6', 'ORSC'}</t>
         </is>
       </c>
       <c r="Q441" t="inlineStr">
@@ -35730,7 +35730,7 @@
       </c>
       <c r="S441" t="inlineStr">
         <is>
-          <t>{'ORSC.ResCode', 'RSC6.WeekDay', 'RSC6.ResCode', 'RSC6.CapFactor1', 'ORSC.ResName'}</t>
+          <t>{'RSC6.ResCode', 'RSC6.WeekDay', 'RSC6.CapFactor1', 'ORSC.ResName', 'ORSC.ResCode'}</t>
         </is>
       </c>
       <c r="T441" t="inlineStr">
@@ -35795,7 +35795,7 @@
       </c>
       <c r="P442" t="inlineStr">
         <is>
-          <t>{'PMG2', 'OPMG'}</t>
+          <t>{'OPMG', 'PMG2'}</t>
         </is>
       </c>
       <c r="Q442" t="inlineStr">
@@ -35810,7 +35810,7 @@
       </c>
       <c r="S442" t="inlineStr">
         <is>
-          <t>{'OPMG.AbsEntry', 'PMG2.SOLUTION', 'PMG2.REMARKS', 'OPMG.NAME', 'PMG2.AbsEntry'}</t>
+          <t>{'OPMG.AbsEntry', 'OPMG.NAME', 'PMG2.SOLUTION', 'PMG2.REMARKS', 'PMG2.AbsEntry'}</t>
         </is>
       </c>
       <c r="T442" t="inlineStr">
@@ -35890,7 +35890,7 @@
       </c>
       <c r="S443" t="inlineStr">
         <is>
-          <t>{'OCPT._Top', 'CPT1.AbsEntry', 'CPT1._Right', 'CPT1._Bottom', 'OCPT.Name', 'OCPT.AbsEntry', 'CPT1._Top', 'OCPT._Left', 'CPT1._Left'}</t>
+          <t>{'CPT1._Left', 'CPT1._Bottom', 'CPT1.AbsEntry', 'OCPT.AbsEntry', 'CPT1._Right', 'OCPT.Name', 'OCPT._Left', 'CPT1._Top', 'OCPT._Top'}</t>
         </is>
       </c>
       <c r="T443" t="inlineStr">
@@ -35970,7 +35970,7 @@
       </c>
       <c r="S444" t="inlineStr">
         <is>
-          <t>{'OBOB.DescField', 'OBOB.TableName'}</t>
+          <t>{'OBOB.TableName', 'OBOB.DescField'}</t>
         </is>
       </c>
       <c r="T444" t="inlineStr">
@@ -36035,7 +36035,7 @@
       </c>
       <c r="P445" t="inlineStr">
         <is>
-          <t>{'OHEM', 'OHTM', 'HTM1'}</t>
+          <t>{'HTM1', 'OHTM', 'OHEM'}</t>
         </is>
       </c>
       <c r="Q445" t="inlineStr">
@@ -36050,7 +36050,7 @@
       </c>
       <c r="S445" t="inlineStr">
         <is>
-          <t>{'HTM1.teamID', 'OHTM.name', 'OHTM.teamID', 'OHEM.firstName', 'OHEM.lastName', 'HTM1.empID', 'OHEM.empID'}</t>
+          <t>{'OHTM.teamID', 'OHTM.name', 'HTM1.teamID', 'HTM1.empID', 'OHEM.lastName', 'OHEM.empID', 'OHEM.firstName'}</t>
         </is>
       </c>
       <c r="T445" t="inlineStr">
@@ -36195,7 +36195,7 @@
       </c>
       <c r="P447" t="inlineStr">
         <is>
-          <t>{'OHEM', 'OHTM', 'HTM1'}</t>
+          <t>{'HTM1', 'OHTM', 'OHEM'}</t>
         </is>
       </c>
       <c r="Q447" t="inlineStr">
@@ -36210,7 +36210,7 @@
       </c>
       <c r="S447" t="inlineStr">
         <is>
-          <t>{'HTM1.teamID', 'OHTM.name', 'OHTM.teamID', 'HTM1.empID', 'OHEM.empID', 'OHEM.salary'}</t>
+          <t>{'OHTM.teamID', 'OHTM.name', 'HTM1.teamID', 'HTM1.empID', 'OHEM.salary', 'OHEM.empID'}</t>
         </is>
       </c>
       <c r="T447" t="inlineStr">
@@ -36290,7 +36290,7 @@
       </c>
       <c r="S448" t="inlineStr">
         <is>
-          <t>{'OHEM.homeTel', 'OHEM.mobile', 'OHEM.pager', 'OHEM.lastName', 'OHEM.firstName', 'OHEM.officeTel'}</t>
+          <t>{'OHEM.mobile', 'OHEM.officeTel', 'OHEM.pager', 'OHEM.lastName', 'OHEM.firstName', 'OHEM.homeTel'}</t>
         </is>
       </c>
       <c r="T448" t="inlineStr">
@@ -36370,7 +36370,7 @@
       </c>
       <c r="S449" t="inlineStr">
         <is>
-          <t>{'OHEM.firstName', 'OHEM.SurnameSP', 'OHEM.FNameSP', 'OHEM.lastName'}</t>
+          <t>{'OHEM.lastName', 'OHEM.firstName', 'OHEM.SurnameSP', 'OHEM.FNameSP'}</t>
         </is>
       </c>
       <c r="T449" t="inlineStr">
@@ -36435,7 +36435,7 @@
       </c>
       <c r="P450" t="inlineStr">
         <is>
-          <t>{'OHEM', 'OHTY'}</t>
+          <t>{'OHTY', 'OHEM'}</t>
         </is>
       </c>
       <c r="Q450" t="inlineStr">
@@ -36450,7 +36450,7 @@
       </c>
       <c r="S450" t="inlineStr">
         <is>
-          <t>{'OHEM.nChildren', 'OHEM.type', 'OHTY.typeID', 'OHEM.StatusOfE', 'OHEM.lastName', 'OHTY.name'}</t>
+          <t>{'OHEM.nChildren', 'OHTY.typeID', 'OHEM.lastName', 'OHEM.StatusOfE', 'OHEM.type', 'OHTY.name'}</t>
         </is>
       </c>
       <c r="T450" t="inlineStr">
@@ -36610,7 +36610,7 @@
       </c>
       <c r="S452" t="inlineStr">
         <is>
-          <t>{'OHEM.HeaInsType', 'OHEM.HeaInsName', 'OHEM.lastName', 'OHEM.HeaInsCode', 'OHEM.empID'}</t>
+          <t>{'OHEM.HeaInsCode', 'OHEM.HeaInsName', 'OHEM.lastName', 'OHEM.HeaInsType', 'OHEM.empID'}</t>
         </is>
       </c>
       <c r="T452" t="inlineStr">
@@ -36690,7 +36690,7 @@
       </c>
       <c r="S453" t="inlineStr">
         <is>
-          <t>{'OHEM.JTCode', 'OHEM.lastName'}</t>
+          <t>{'OHEM.lastName', 'OHEM.JTCode'}</t>
         </is>
       </c>
       <c r="T453" t="inlineStr">
@@ -36755,7 +36755,7 @@
       </c>
       <c r="P454" t="inlineStr">
         <is>
-          <t>{'OHEM', 'OHTM', 'HTM1'}</t>
+          <t>{'HTM1', 'OHTM', 'OHEM'}</t>
         </is>
       </c>
       <c r="Q454" t="inlineStr">
@@ -36770,7 +36770,7 @@
       </c>
       <c r="S454" t="inlineStr">
         <is>
-          <t>{'HTM1.teamID', 'OHTM.name', 'OHTM.teamID', 'OHEM.VacCurYear', 'HTM1.empID', 'OHEM.empID'}</t>
+          <t>{'OHTM.teamID', 'OHTM.name', 'HTM1.teamID', 'HTM1.empID', 'OHEM.VacCurYear', 'OHEM.empID'}</t>
         </is>
       </c>
       <c r="T454" t="inlineStr">
@@ -36835,7 +36835,7 @@
       </c>
       <c r="P455" t="inlineStr">
         <is>
-          <t>{'OHEM', 'HTM1'}</t>
+          <t>{'HTM1', 'OHEM'}</t>
         </is>
       </c>
       <c r="Q455" t="inlineStr">
@@ -36850,7 +36850,7 @@
       </c>
       <c r="S455" t="inlineStr">
         <is>
-          <t>{'HTM1.empID', 'HTM1.teamID', 'OHEM.empID', 'OHEM.CPF'}</t>
+          <t>{'OHEM.CPF', 'OHEM.empID', 'HTM1.teamID', 'HTM1.empID'}</t>
         </is>
       </c>
       <c r="T455" t="inlineStr">
@@ -36915,7 +36915,7 @@
       </c>
       <c r="P456" t="inlineStr">
         <is>
-          <t>{'OHEM', 'OHTY'}</t>
+          <t>{'OHTY', 'OHEM'}</t>
         </is>
       </c>
       <c r="Q456" t="inlineStr">
@@ -36930,7 +36930,7 @@
       </c>
       <c r="S456" t="inlineStr">
         <is>
-          <t>{'OHTY.name', 'OHEM.type', 'OHTY.typeID', 'OHEM.TaxClass', 'OHEM.MunKey', 'OHEM.InTaxLiabi'}</t>
+          <t>{'OHTY.typeID', 'OHEM.MunKey', 'OHEM.InTaxLiabi', 'OHEM.type', 'OHEM.TaxClass', 'OHTY.name'}</t>
         </is>
       </c>
       <c r="T456" t="inlineStr">
@@ -36995,7 +36995,7 @@
       </c>
       <c r="P457" t="inlineStr">
         <is>
-          <t>{'OHEM', 'HEM6'}</t>
+          <t>{'HEM6', 'OHEM'}</t>
         </is>
       </c>
       <c r="Q457" t="inlineStr">
@@ -37010,7 +37010,7 @@
       </c>
       <c r="S457" t="inlineStr">
         <is>
-          <t>{'HEM6.empID', 'OHEM.empID', 'HEM6.roleID', 'OHEM.salary'}</t>
+          <t>{'HEM6.empID', 'OHEM.salary', 'OHEM.empID', 'HEM6.roleID'}</t>
         </is>
       </c>
       <c r="T457" t="inlineStr">
@@ -37090,7 +37090,7 @@
       </c>
       <c r="S458" t="inlineStr">
         <is>
-          <t>{'OHEM.birthDate', 'OHEM.homeCity', 'OHEM.brthCountr', 'OHEM.homeCountr', 'OHEM.homeCounty', 'OHEM.jobTitle'}</t>
+          <t>{'OHEM.homeCountr', 'OHEM.jobTitle', 'OHEM.brthCountr', 'OHEM.birthDate', 'OHEM.homeCounty', 'OHEM.homeCity'}</t>
         </is>
       </c>
       <c r="T458" t="inlineStr">
@@ -37170,7 +37170,7 @@
       </c>
       <c r="S459" t="inlineStr">
         <is>
-          <t>{'OHEM.citizenshp', 'OHEM.passportNo', 'OHEM.lastName', 'OHEM.StatusOfP'}</t>
+          <t>{'OHEM.lastName', 'OHEM.passportNo', 'OHEM.StatusOfP', 'OHEM.citizenshp'}</t>
         </is>
       </c>
       <c r="T459" t="inlineStr">
@@ -37250,7 +37250,7 @@
       </c>
       <c r="S460" t="inlineStr">
         <is>
-          <t>{'OHEM.workCity', 'OHEM.emplCost', 'OHEM.homeCity', 'OHEM.lastName', 'OHEM.firstName'}</t>
+          <t>{'OHEM.emplCost', 'OHEM.workCity', 'OHEM.lastName', 'OHEM.firstName', 'OHEM.homeCity'}</t>
         </is>
       </c>
       <c r="T460" t="inlineStr">
@@ -37315,7 +37315,7 @@
       </c>
       <c r="P461" t="inlineStr">
         <is>
-          <t>{'OHEM', 'OHTM', 'HTM1'}</t>
+          <t>{'HTM1', 'OHTM', 'OHEM'}</t>
         </is>
       </c>
       <c r="Q461" t="inlineStr">
@@ -37330,7 +37330,7 @@
       </c>
       <c r="S461" t="inlineStr">
         <is>
-          <t>{'OHEM.workCity', 'OHEM.homeTel', 'OHTM.name', 'OHTM.teamID', 'OHEM.officeTel', 'HTM1.empID', 'HTM1.teamID', 'OHEM.MunKey', 'OHEM.homeCity', 'OHEM.empID'}</t>
+          <t>{'OHTM.name', 'HTM1.empID', 'OHEM.empID', 'OHEM.MunKey', 'OHEM.homeCity', 'OHTM.teamID', 'OHEM.officeTel', 'HTM1.teamID', 'OHEM.workCity', 'OHEM.homeTel'}</t>
         </is>
       </c>
       <c r="T461" t="inlineStr">
@@ -37395,7 +37395,7 @@
       </c>
       <c r="P462" t="inlineStr">
         <is>
-          <t>{'OHEM', 'OHTM', 'HTM1'}</t>
+          <t>{'HTM1', 'OHTM', 'OHEM'}</t>
         </is>
       </c>
       <c r="Q462" t="inlineStr">
@@ -37410,7 +37410,7 @@
       </c>
       <c r="S462" t="inlineStr">
         <is>
-          <t>{'OHEM.StreetNoW', 'OHTM.name', 'OHTM.teamID', 'OHEM.StatusOfP', 'OHEM.StatusOfE', 'HTM1.empID', 'HTM1.teamID', 'OHEM.empID', 'OHEM.StreetNoH'}</t>
+          <t>{'OHTM.name', 'OHEM.StatusOfP', 'HTM1.empID', 'OHEM.StatusOfE', 'OHEM.empID', 'OHTM.teamID', 'OHEM.StreetNoH', 'HTM1.teamID', 'OHEM.StreetNoW'}</t>
         </is>
       </c>
       <c r="T462" t="inlineStr">
@@ -37490,7 +37490,7 @@
       </c>
       <c r="S463" t="inlineStr">
         <is>
-          <t>{'OHEM.TaxOName', 'OHEM.PymMeth', 'OHEM.AddiCurr', 'OHEM.ExemptCurr'}</t>
+          <t>{'OHEM.ExemptCurr', 'OHEM.PymMeth', 'OHEM.TaxOName', 'OHEM.AddiCurr'}</t>
         </is>
       </c>
       <c r="T463" t="inlineStr">
@@ -37570,7 +37570,7 @@
       </c>
       <c r="S464" t="inlineStr">
         <is>
-          <t>{'OHEM.homeStreet', 'OHEM.homeZip', 'OHEM.lastName', 'OHEM.martStatus', 'OHEM.homeBlock', 'OHEM.homeState'}</t>
+          <t>{'OHEM.homeZip', 'OHEM.lastName', 'OHEM.homeStreet', 'OHEM.homeBlock', 'OHEM.homeState', 'OHEM.martStatus'}</t>
         </is>
       </c>
       <c r="T464" t="inlineStr">
@@ -37650,7 +37650,7 @@
       </c>
       <c r="S465" t="inlineStr">
         <is>
-          <t>{'OITM.IsCommited', 'OITM.OnHand', 'OITM.ItemName', 'OITM.OnOrder'}</t>
+          <t>{'OITM.OnOrder', 'OITM.OnHand', 'OITM.IsCommited', 'OITM.ItemName'}</t>
         </is>
       </c>
       <c r="T465" t="inlineStr">
@@ -37730,7 +37730,7 @@
       </c>
       <c r="S466" t="inlineStr">
         <is>
-          <t>{'ITM1.Price', 'OITM.ItemCode', 'OITM.IsCommited', 'OITM.ItemName', 'ITM1.ItemCode'}</t>
+          <t>{'OITM.ItemCode', 'ITM1.ItemCode', 'ITM1.Price', 'OITM.IsCommited', 'OITM.ItemName'}</t>
         </is>
       </c>
       <c r="T466" t="inlineStr">
@@ -37810,7 +37810,7 @@
       </c>
       <c r="S467" t="inlineStr">
         <is>
-          <t>{'ITM2.ItemCode', 'OITM.LastPurPrc', 'ITM2.VendorCode', 'OITM.ItemCode', 'OITM.ItemName', 'OITM.Consig'}</t>
+          <t>{'OITM.LastPurPrc', 'OITM.ItemCode', 'OITM.ItemName', 'ITM2.VendorCode', 'ITM2.ItemCode', 'OITM.Consig'}</t>
         </is>
       </c>
       <c r="T467" t="inlineStr">
@@ -37890,7 +37890,7 @@
       </c>
       <c r="S468" t="inlineStr">
         <is>
-          <t>{'ITM4.Length1', 'ITM4.ItemCode', 'ITM4.Width1', 'ITM4.QtyPerPack', 'ITM4.Volume', 'OITM.ItemCode', 'ITM4.Height1', 'OITM.ItemName'}</t>
+          <t>{'ITM4.Volume', 'ITM4.Length1', 'ITM4.Width1', 'ITM4.Height1', 'ITM4.QtyPerPack', 'OITM.ItemName', 'OITM.ItemCode', 'ITM4.ItemCode'}</t>
         </is>
       </c>
       <c r="T468" t="inlineStr">
@@ -37970,7 +37970,7 @@
       </c>
       <c r="S469" t="inlineStr">
         <is>
-          <t>{'ITM7.UsefulLife', 'ITM7.DprArea', 'ITM7.RemainLife', 'ITM7.RemainDays'}</t>
+          <t>{'ITM7.DprArea', 'ITM7.UsefulLife', 'ITM7.RemainLife', 'ITM7.RemainDays'}</t>
         </is>
       </c>
       <c r="T469" t="inlineStr">
@@ -38050,7 +38050,7 @@
       </c>
       <c r="S470" t="inlineStr">
         <is>
-          <t>{'OPKG.PkgType', 'OPKG.Volume'}</t>
+          <t>{'OPKG.Volume', 'OPKG.PkgType'}</t>
         </is>
       </c>
       <c r="T470" t="inlineStr">
@@ -38130,7 +38130,7 @@
       </c>
       <c r="S471" t="inlineStr">
         <is>
-          <t>{'OITM.ItemCode', 'OBCD.BcdCode', 'OBCD.UomEntry', 'OITM.ItemName', 'OBCD.ItemCode'}</t>
+          <t>{'OBCD.UomEntry', 'OITM.ItemCode', 'OBCD.ItemCode', 'OBCD.BcdCode', 'OITM.ItemName'}</t>
         </is>
       </c>
       <c r="T471" t="inlineStr">
@@ -38210,7 +38210,7 @@
       </c>
       <c r="S472" t="inlineStr">
         <is>
-          <t>{'OBFC.DispName', 'OBFC.UpdateDate', 'OBFC.Activated', 'OBFC.DataSource'}</t>
+          <t>{'OBFC.Activated', 'OBFC.DispName', 'OBFC.DataSource', 'OBFC.UpdateDate'}</t>
         </is>
       </c>
       <c r="T472" t="inlineStr">
@@ -38290,7 +38290,7 @@
       </c>
       <c r="S473" t="inlineStr">
         <is>
-          <t>{'OITB.ItmsGrpCod', 'OITM.ItmsGrpCod', 'OITB.ItmsGrpNam'}</t>
+          <t>{'OITB.ItmsGrpCod', 'OITB.ItmsGrpNam', 'OITM.ItmsGrpCod'}</t>
         </is>
       </c>
       <c r="T473" t="inlineStr">
@@ -38355,7 +38355,7 @@
       </c>
       <c r="P474" t="inlineStr">
         <is>
-          <t>{'OITM', 'ITM4', 'OITB'}</t>
+          <t>{'OITM', 'OITB', 'ITM4'}</t>
         </is>
       </c>
       <c r="Q474" t="inlineStr">
@@ -38370,7 +38370,7 @@
       </c>
       <c r="S474" t="inlineStr">
         <is>
-          <t>{'OITM.ItemCode', 'ITM4.ItemCode', 'OITM.ItmsGrpCod', 'OITB.ItmsGrpCod', 'ITM4.Volume', 'OITB.ItmsGrpNam'}</t>
+          <t>{'OITB.ItmsGrpCod', 'ITM4.Volume', 'OITM.ItemCode', 'ITM4.ItemCode', 'OITM.ItmsGrpCod', 'OITB.ItmsGrpNam'}</t>
         </is>
       </c>
       <c r="T474" t="inlineStr">
@@ -38435,7 +38435,7 @@
       </c>
       <c r="P475" t="inlineStr">
         <is>
-          <t>{'OECM', 'ECM1'}</t>
+          <t>{'ECM1', 'OECM'}</t>
         </is>
       </c>
       <c r="Q475" t="inlineStr">
@@ -38450,7 +38450,7 @@
       </c>
       <c r="S475" t="inlineStr">
         <is>
-          <t>{'ECM1.Code', 'ECM1.ParamName', 'OECM.Descr', 'ECM1.ParamPrms', 'OECM.Code'}</t>
+          <t>{'ECM1.ParamPrms', 'OECM.Descr', 'ECM1.Code', 'OECM.Code', 'ECM1.ParamName'}</t>
         </is>
       </c>
       <c r="T475" t="inlineStr">
@@ -38530,7 +38530,7 @@
       </c>
       <c r="S476" t="inlineStr">
         <is>
-          <t>{'ECM4.ObjXPath', 'OECM.Descr', 'OECM.Code', 'ECM4.FieldXPath', 'ECM4.Code'}</t>
+          <t>{'ECM4.FieldXPath', 'OECM.Descr', 'OECM.Code', 'ECM4.ObjXPath', 'ECM4.Code'}</t>
         </is>
       </c>
       <c r="T476" t="inlineStr">
@@ -38690,7 +38690,7 @@
       </c>
       <c r="S478" t="inlineStr">
         <is>
-          <t>{'OQAG.AUTHGRPCD', 'OQAG.CreateDate', 'OQAG.LogInstanc', 'OQAG.UpdateDate', 'OQAG.AUTHGRPN'}</t>
+          <t>{'OQAG.CreateDate', 'OQAG.UpdateDate', 'OQAG.LogInstanc', 'OQAG.AUTHGRPCD', 'OQAG.AUTHGRPN'}</t>
         </is>
       </c>
       <c r="T478" t="inlineStr">
@@ -38850,7 +38850,7 @@
       </c>
       <c r="S480" t="inlineStr">
         <is>
-          <t>{'RDOC.TypeCode', 'RDOC.ScreenFont', 'RDOC.EmailFont'}</t>
+          <t>{'RDOC.ScreenFont', 'RDOC.TypeCode', 'RDOC.EmailFont'}</t>
         </is>
       </c>
       <c r="T480" t="inlineStr">
@@ -38930,7 +38930,7 @@
       </c>
       <c r="S481" t="inlineStr">
         <is>
-          <t>{'RTYP.CODE', 'RTYP.DEFLT_REP', 'RDOC.DocCode', 'RTYP.NAME'}</t>
+          <t>{'RTYP.DEFLT_REP', 'RDOC.DocCode', 'RTYP.NAME', 'RTYP.CODE'}</t>
         </is>
       </c>
       <c r="T481" t="inlineStr">
@@ -39010,7 +39010,7 @@
       </c>
       <c r="S482" t="inlineStr">
         <is>
-          <t>{'RDOC.TypeCode', 'RITM.DocCode', 'RDOC.DocCode', 'RDOC.DocName'}</t>
+          <t>{'RDOC.DocCode', 'RITM.DocCode', 'RDOC.DocName', 'RDOC.TypeCode'}</t>
         </is>
       </c>
       <c r="T482" t="inlineStr">
@@ -39090,7 +39090,7 @@
       </c>
       <c r="S483" t="inlineStr">
         <is>
-          <t>{'RDOC.SwpInEmail', 'RDOC.ExtOnErr', 'RDOC.NumRepArs'}</t>
+          <t>{'RDOC.ExtOnErr', 'RDOC.NumRepArs', 'RDOC.SwpInEmail'}</t>
         </is>
       </c>
       <c r="T483" t="inlineStr">
@@ -39170,7 +39170,7 @@
       </c>
       <c r="S484" t="inlineStr">
         <is>
-          <t>{'RITM.BGGreen', 'RITM.BGRed', 'RITM.BrdrRed', 'RITM.FGGreen', 'RITM.BrdrGreen', 'RITM.Height', 'RITM.FGRed', 'RITM.FGBlue', 'RITM.MrkrGreen', 'RITM.MrkrBlue', 'RITM.MrkrRed', 'RITM.BGBlue', 'RITM.BrdrBlue'}</t>
+          <t>{'RITM.FGGreen', 'RITM.BGRed', 'RITM.MrkrBlue', 'RITM.BGGreen', 'RITM.FGBlue', 'RITM.Height', 'RITM.BGBlue', 'RITM.FGRed', 'RITM.MrkrGreen', 'RITM.BrdrRed', 'RITM.MrkrRed', 'RITM.BrdrGreen', 'RITM.BrdrBlue'}</t>
         </is>
       </c>
       <c r="T484" t="inlineStr">
@@ -39395,7 +39395,7 @@
       </c>
       <c r="P487" t="inlineStr">
         <is>
-          <t>{'OPR1', 'OOPR'}</t>
+          <t>{'OOPR', 'OPR1'}</t>
         </is>
       </c>
       <c r="Q487" t="inlineStr">
@@ -39410,7 +39410,7 @@
       </c>
       <c r="S487" t="inlineStr">
         <is>
-          <t>{'OPR1.OpprId', 'OPR1.ClosePrcnt', 'OOPR.CardCode', 'OOPR.OpprId'}</t>
+          <t>{'OPR1.ClosePrcnt', 'OPR1.OpprId', 'OOPR.CardCode', 'OOPR.OpprId'}</t>
         </is>
       </c>
       <c r="T487" t="inlineStr">
@@ -39490,7 +39490,7 @@
       </c>
       <c r="S488" t="inlineStr">
         <is>
-          <t>{'OPR1.CloseDate', 'OPR1.WtSumLoc', 'OPR1.WtSumSys'}</t>
+          <t>{'OPR1.WtSumLoc', 'OPR1.CloseDate', 'OPR1.WtSumSys'}</t>
         </is>
       </c>
       <c r="T488" t="inlineStr">
@@ -39570,7 +39570,7 @@
       </c>
       <c r="S489" t="inlineStr">
         <is>
-          <t>{'OPRC.PrcCode', 'OPRC.Active', 'OPRC.DataSource', 'OPRC.PrcName', 'OPRC.Balance', 'OPRC.ValidFrom'}</t>
+          <t>{'OPRC.PrcCode', 'OPRC.PrcName', 'OPRC.Balance', 'OPRC.Active', 'OPRC.ValidFrom', 'OPRC.DataSource'}</t>
         </is>
       </c>
       <c r="T489" t="inlineStr">
@@ -39650,7 +39650,7 @@
       </c>
       <c r="S490" t="inlineStr">
         <is>
-          <t>{'OOPR.CardName', 'OOPR.RealProfS', 'OOPR.CloPrcnt', 'OOPR.RealSumSys', 'OOPR.RealProfL', 'OOPR.RealSumLoc'}</t>
+          <t>{'OOPR.RealProfL', 'OOPR.RealSumLoc', 'OOPR.CardName', 'OOPR.RealSumSys', 'OOPR.RealProfS', 'OOPR.CloPrcnt'}</t>
         </is>
       </c>
       <c r="T490" t="inlineStr">
@@ -39730,7 +39730,7 @@
       </c>
       <c r="S491" t="inlineStr">
         <is>
-          <t>{'OPR1.CloseDate', 'OPR1.ClosePrcnt', 'OPR1.OpenDate'}</t>
+          <t>{'OPR1.ClosePrcnt', 'OPR1.OpenDate', 'OPR1.CloseDate'}</t>
         </is>
       </c>
       <c r="T491" t="inlineStr">
@@ -39810,7 +39810,7 @@
       </c>
       <c r="S492" t="inlineStr">
         <is>
-          <t>{'OOPR.Status', 'OOPR.OpenDate'}</t>
+          <t>{'OOPR.OpenDate', 'OOPR.Status'}</t>
         </is>
       </c>
       <c r="T492" t="inlineStr">
@@ -40035,7 +40035,7 @@
       </c>
       <c r="P495" t="inlineStr">
         <is>
-          <t>{'OCTR', 'CTR1'}</t>
+          <t>{'CTR1', 'OCTR'}</t>
         </is>
       </c>
       <c r="Q495" t="inlineStr">
@@ -40370,7 +40370,7 @@
       </c>
       <c r="S499" t="inlineStr">
         <is>
-          <t>{'OQUE.email', 'OQUE.descript', 'OQUE.manager'}</t>
+          <t>{'OQUE.descript', 'OQUE.email', 'OQUE.manager'}</t>
         </is>
       </c>
       <c r="T499" t="inlineStr">
@@ -40450,7 +40450,7 @@
       </c>
       <c r="S500" t="inlineStr">
         <is>
-          <t>{'OSCL.customer', 'OSCL.priority', 'OSCL.custmrName'}</t>
+          <t>{'OSCL.priority', 'OSCL.custmrName', 'OSCL.customer'}</t>
         </is>
       </c>
       <c r="T500" t="inlineStr">
@@ -40515,7 +40515,7 @@
       </c>
       <c r="P501" t="inlineStr">
         <is>
-          <t>{'OSCO', 'OSCL'}</t>
+          <t>{'OSCL', 'OSCO'}</t>
         </is>
       </c>
       <c r="Q501" t="inlineStr">
@@ -40530,7 +40530,7 @@
       </c>
       <c r="S501" t="inlineStr">
         <is>
-          <t>{'OSCO.Name', 'OSCO.originID', 'OSCL.AssignDate', 'OSCL.origin', 'OSCL.respOnDate', 'OSCL.resolOnDat'}</t>
+          <t>{'OSCL.resolOnDat', 'OSCO.Name', 'OSCL.origin', 'OSCO.originID', 'OSCL.respOnDate', 'OSCL.AssignDate'}</t>
         </is>
       </c>
       <c r="T501" t="inlineStr">
@@ -40610,7 +40610,7 @@
       </c>
       <c r="S502" t="inlineStr">
         <is>
-          <t>{'OSCL.BPShipAddr', 'OSCL.BPE_Mail', 'OSCL.BPBillAddr', 'OSCL.custmrName'}</t>
+          <t>{'OSCL.BPBillAddr', 'OSCL.BPShipAddr', 'OSCL.custmrName', 'OSCL.BPE_Mail'}</t>
         </is>
       </c>
       <c r="T502" t="inlineStr">
@@ -40690,7 +40690,7 @@
       </c>
       <c r="S503" t="inlineStr">
         <is>
-          <t>{'OCTR.CstmrCode', 'OCTR.CstmrName', 'OSCL.customer'}</t>
+          <t>{'OCTR.CstmrName', 'OSCL.customer', 'OCTR.CstmrCode'}</t>
         </is>
       </c>
       <c r="T503" t="inlineStr">
@@ -40770,7 +40770,7 @@
       </c>
       <c r="S504" t="inlineStr">
         <is>
-          <t>{'OINS.custmrName', 'OINS.internalSN', 'OINS.itemCode'}</t>
+          <t>{'OINS.internalSN', 'OINS.custmrName', 'OINS.itemCode'}</t>
         </is>
       </c>
       <c r="T504" t="inlineStr">

</xml_diff>